<commit_message>
Adding a identified missing list to the checkvars.py script #83
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="269">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -812,6 +812,21 @@
   </si>
   <si>
     <t xml:space="preserve">Total reactive nitrogen volume mixing ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrfso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can not be produced by LPJ-GUESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Warlind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shrubFrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agesno</t>
   </si>
 </sst>
 </file>
@@ -895,7 +910,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -906,6 +921,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -925,10 +944,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F128" activeCellId="0" sqref="F128:F138"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C116" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F143" activeCellId="0" sqref="F143:F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3561,6 +3580,39 @@
         <v>11</v>
       </c>
     </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C143" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E143" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F143" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C144" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E144" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F144" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C145" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E145" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F145" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update ignore comment for n2o
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="73">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -97,22 +97,25 @@
     <t xml:space="preserve">Mole Fraction of N2O</t>
   </si>
   <si>
+    <t xml:space="preserve">Component not available in TM5. It is one of the prescribed greenhouse gases in IFS. WMO grib code: 210063, but not available in IFS output.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommi Bergman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6hrLev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude alevel time1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bs550aer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerosol backscatter coefficient</t>
+  </si>
+  <si>
     <t xml:space="preserve">Component not available in TM5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tommi Bergman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6hrLev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude alevel time1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bs550aer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aerosol backscatter coefficient</t>
   </si>
   <si>
     <t xml:space="preserve">AERmon</t>
@@ -356,7 +359,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -490,7 +493,7 @@
         <v>30</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>26</v>
@@ -499,19 +502,19 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>26</v>
@@ -519,19 +522,19 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>26</v>
@@ -539,19 +542,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>26</v>
@@ -559,19 +562,19 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>26</v>
@@ -579,19 +582,19 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>26</v>
@@ -599,19 +602,19 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>26</v>
@@ -619,19 +622,19 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>26</v>
@@ -639,19 +642,19 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>26</v>
@@ -659,19 +662,19 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>26</v>
@@ -679,19 +682,19 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>26</v>
@@ -699,19 +702,19 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>26</v>
@@ -719,19 +722,19 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>26</v>
@@ -739,19 +742,19 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>26</v>
@@ -759,19 +762,19 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>26</v>
@@ -779,19 +782,19 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>26</v>
@@ -799,19 +802,19 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>26</v>
@@ -819,19 +822,19 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>26</v>
@@ -839,19 +842,19 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>26</v>
@@ -859,35 +862,35 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add the cmor variables ccb and mc to the basic ignored file
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="121">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -46,6 +46,39 @@
     <t xml:space="preserve">extensive variable description</t>
   </si>
   <si>
+    <t xml:space="preserve">Amon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ccb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Pressure at Convective Cloud Base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too much effort?: convective cloud cover ccc[185] &gt; 0.5 or &gt; 0.0, this mask combine with cloud base height cbh[228023], therafter with surface pressure sp[134] and lapse rate the cct can be calculated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where convective cloud is present in the grid cell, the instantaneous cloud base altitude should be that of the bottom of the lowest level containing convective cloud. Missing data should be reported in the absence of convective cloud. The time mean should be calculated from these quantities averaging over occasions when convective cloud is present only, and should contain missing data for occasions when no convective cloud is present during the meaning period.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude alevhalf time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convective Mass Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too much effort?: IFS var in PEXTRA, the CUFLXN routine produces PFMU (MASSFLUX IN UPDRAFTS) and PFMD (MASSFLUX DOWNDRAFTS) KG/(M2*S) which can be combined. Which gib code?, via?: sources/ifs-36r4/src/ifs/phys_ec/callpar.F90 in variables PGFL(JL,JK,YERA40(5)%MP) and PGFL(JL,JK,YERA40(6)%MP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The net mass flux should represent the difference between the updraft and downdraft components.  The flux is computed as the mass divided by the area of the grid cell.</t>
+  </si>
+  <si>
     <t xml:space="preserve">CF3hr</t>
   </si>
   <si>
@@ -65,12 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fraction of time that shallow convection occurs in the grid cell.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longitude latitude time</t>
   </si>
   <si>
     <t xml:space="preserve">ci</t>
@@ -439,13 +466,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -469,10 +500,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -514,7 +545,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
@@ -527,209 +568,204 @@
       <c r="D3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8de0f30b91b15720398fc10fd712a182.html","web")</f>
-        <v>0</v>
+      <c r="E3" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/13484743dd3369c69df93379e6dafbb5.html","web")</f>
+        <v>web</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6d790fe4caa7feff46a41ae7b3811e52.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="H4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="str">
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8de0f30b91b15720398fc10fd712a182.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/29fae9ea0f236a3eb144026e1bafde28.html","web")</f>
         <v>web</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="0" t="s">
+      <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f27656eeae247192e82aa1032c911399.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0062272a6a4176b8c32af87642b062c5.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="G7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="0" t="s">
+      <c r="H7" s="3" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E9" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8de0f30b91b15720398fc10fd712a182.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f27656eeae247192e82aa1032c911399.html","web")</f>
         <v>0</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/942125e5a461fef57b1477b9a2bd5fa0.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="0" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0062272a6a4176b8c32af87642b062c5.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E12" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a77f2a-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8de0f30b91b15720398fc10fd712a182.html","web")</f>
         <v>0</v>
       </c>
       <c r="F12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="E13" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/942125e5a461fef57b1477b9a2bd5fa0.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/98114e26-b896-11e6-a189-5404a60d96b5.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>45</v>
+      <c r="G13" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>46</v>
@@ -738,103 +774,76 @@
         <v>47</v>
       </c>
       <c r="E15" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e8d5bdfd24b275f0530646361967483d.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a77f2a-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cfe4bddb7dbbfc57c19837e7f99d2dda.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E17" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4ffc1f50b844980dbbae006dbcfca869.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/98114e26-b896-11e6-a189-5404a60d96b5.html","web")</f>
         <v>0</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E18" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ea546e38aa8fc0e021f03e746e1adb10.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e8d5bdfd24b275f0530646361967483d.html","web")</f>
         <v>0</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>57</v>
@@ -843,14 +852,14 @@
         <v>58</v>
       </c>
       <c r="E19" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/691673a210102ac652eed2b784dd2ab4.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cfe4bddb7dbbfc57c19837e7f99d2dda.html","web")</f>
         <v>0</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>59</v>
@@ -858,10 +867,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>60</v>
@@ -870,14 +879,14 @@
         <v>61</v>
       </c>
       <c r="E20" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a4e52f0f3833b395c09c73f1b6f3f748.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4ffc1f50b844980dbbae006dbcfca869.html","web")</f>
         <v>0</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>62</v>
@@ -885,10 +894,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>63</v>
@@ -897,533 +906,614 @@
         <v>64</v>
       </c>
       <c r="E21" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe6bdb96-a41f-11e5-9025-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ea546e38aa8fc0e021f03e746e1adb10.html","web")</f>
         <v>0</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc8f92a2635774d636748ec8007c4bab.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/691673a210102ac652eed2b784dd2ab4.html","web")</f>
         <v>0</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E23" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2b133ea2-1b42-11e6-a696-35cd2d8034df.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a4e52f0f3833b395c09c73f1b6f3f748.html","web")</f>
         <v>0</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E24" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/942125e5a461fef57b1477b9a2bd5fa0.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fe6bdb96-a41f-11e5-9025-ac72891c3257.html","web")</f>
         <v>0</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E25" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/218a6b28-8995-11e6-b63d-5404a60d96b5.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc8f92a2635774d636748ec8007c4bab.html","web")</f>
         <v>0</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E26" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a0c10a4b65d3b79db581a649058a08b1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2b133ea2-1b42-11e6-a696-35cd2d8034df.html","web")</f>
         <v>0</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>79</v>
       </c>
       <c r="E27" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a2609abee6ecd5d535a48e29ae70e852.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/942125e5a461fef57b1477b9a2bd5fa0.html","web")</f>
         <v>0</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>80</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/218a6b28-8995-11e6-b63d-5404a60d96b5.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="E29" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a0c10a4b65d3b79db581a649058a08b1.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a2609abee6ecd5d535a48e29ae70e852.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f27656eeae247192e82aa1032c911399.html","web")</f>
         <v>0</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F32" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0062272a6a4176b8c32af87642b062c5.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0062272a6a4176b8c32af87642b062c5.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="0" t="n">
+      <c r="H34" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bdb1045bec7f58e9e6221cd39bb34c2f.html","web")</f>
         <v>0</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/942125e5a461fef57b1477b9a2bd5fa0.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154d00de9ab9aff72373a673df10946a.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>94</v>
+      <c r="F36" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E38" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bdb1045bec7f58e9e6221cd39bb34c2f.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/942125e5a461fef57b1477b9a2bd5fa0.html","web")</f>
         <v>0</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154d00de9ab9aff72373a673df10946a.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B40" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="0" t="s">
+      <c r="E41" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bdb1045bec7f58e9e6221cd39bb34c2f.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="G41" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="E40" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51e0588121783d77407236e0d2eb5d14.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="0" t="s">
+      <c r="H41" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0062272a6a4176b8c32af87642b062c5.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>102</v>
+        <v>9</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="E43" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8de0f30b91b15720398fc10fd712a182.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51e0588121783d77407236e0d2eb5d14.html","web")</f>
         <v>0</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="C45" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0062272a6a4176b8c32af87642b062c5.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="E46" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8de0f30b91b15720398fc10fd712a182.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f27656eeae247192e82aa1032c911399.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F45" s="0" t="s">
+      <c r="G46" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="0" t="s">
+      <c r="H46" s="0" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E47" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/96a44ea6-b096-11e6-aab6-ac72891c3257.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="E48" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/afef6490-b096-11e6-aab6-ac72891c3257.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f27656eeae247192e82aa1032c911399.html","web")</f>
         <v>0</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G48" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="H48" s="0" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E49" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc8f92a2635774d636748ec8007c4bab.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="E50" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/96a44ea6-b096-11e6-aab6-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/afef6490-b096-11e6-aab6-ac72891c3257.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc8f92a2635774d636748ec8007c4bab.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E53" s="0" t="n">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/942125e5a461fef57b1477b9a2bd5fa0.html","web")</f>
         <v>0</v>
       </c>
-      <c r="F50" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>34</v>
+      <c r="F53" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the basic ignored file for the H-TESSEL comment adjustments for the 9 involved variables.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="473">
   <si>
     <t>Table</t>
   </si>
@@ -1039,7 +1039,10 @@
     <t>near-surface air temperature (2m above displacement height, i.e. t_ref) on land use tile</t>
   </si>
   <si>
-    <t>Can not be produced by LPJ-GUESS: H-TESSEL?</t>
+    <t>Can not be produced by either LPJ-GUESS or H-TESSEL.</t>
+  </si>
+  <si>
+    <t>David Warlind &amp; Andrea Alessandri</t>
   </si>
   <si>
     <t>tslsiLut</t>
@@ -5827,7 +5830,7 @@
         <v>341</v>
       </c>
       <c r="H150" t="s">
-        <v>15</v>
+        <v>342</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -5835,16 +5838,16 @@
         <v>194</v>
       </c>
       <c r="B151" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C151" t="s">
         <v>18</v>
       </c>
       <c r="D151" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E151" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F151">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e417e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -5854,10 +5857,10 @@
         <v>341</v>
       </c>
       <c r="H151" t="s">
-        <v>15</v>
+        <v>342</v>
       </c>
       <c r="I151" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -5865,7 +5868,7 @@
         <v>194</v>
       </c>
       <c r="B152" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C152" t="s">
         <v>18</v>
@@ -5874,7 +5877,7 @@
         <v>339</v>
       </c>
       <c r="E152" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F152">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59178a72-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -5884,10 +5887,10 @@
         <v>341</v>
       </c>
       <c r="H152" t="s">
-        <v>15</v>
+        <v>342</v>
       </c>
       <c r="I152" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -5895,16 +5898,16 @@
         <v>194</v>
       </c>
       <c r="B153" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C153" t="s">
         <v>18</v>
       </c>
       <c r="D153" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E153" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F153">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590ee804-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -5914,7 +5917,7 @@
         <v>341</v>
       </c>
       <c r="H153" t="s">
-        <v>15</v>
+        <v>342</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -5922,16 +5925,16 @@
         <v>194</v>
       </c>
       <c r="B154" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C154" t="s">
         <v>18</v>
       </c>
       <c r="D154" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E154" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F154">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e590c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -5941,7 +5944,7 @@
         <v>341</v>
       </c>
       <c r="H154" t="s">
-        <v>15</v>
+        <v>342</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -5949,16 +5952,16 @@
         <v>194</v>
       </c>
       <c r="B155" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C155" t="s">
         <v>18</v>
       </c>
       <c r="D155" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E155" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F155">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912e6d4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -5968,7 +5971,7 @@
         <v>341</v>
       </c>
       <c r="H155" t="s">
-        <v>15</v>
+        <v>342</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -5976,16 +5979,16 @@
         <v>194</v>
       </c>
       <c r="B156" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C156" t="s">
         <v>18</v>
       </c>
       <c r="D156" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E156" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F156">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912c3de-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -5995,7 +5998,7 @@
         <v>341</v>
       </c>
       <c r="H156" t="s">
-        <v>15</v>
+        <v>342</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -6003,16 +6006,16 @@
         <v>194</v>
       </c>
       <c r="B157" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C157" t="s">
         <v>18</v>
       </c>
       <c r="D157" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E157" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="F157">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e379c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6022,7 +6025,7 @@
         <v>341</v>
       </c>
       <c r="H157" t="s">
-        <v>15</v>
+        <v>342</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -6030,16 +6033,16 @@
         <v>194</v>
       </c>
       <c r="B158" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C158" t="s">
         <v>18</v>
       </c>
       <c r="D158" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E158" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F158">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3f30557c-b89b-11e6-be04-ac72891c3257.html","web")</f>
@@ -6049,7 +6052,7 @@
         <v>341</v>
       </c>
       <c r="H158" t="s">
-        <v>15</v>
+        <v>342</v>
       </c>
     </row>
     <row r="159" spans="1:9">
@@ -6057,7 +6060,7 @@
         <v>194</v>
       </c>
       <c r="B159" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C159" t="s">
         <v>18</v>
@@ -6066,20 +6069,20 @@
         <v>230</v>
       </c>
       <c r="E159" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F159">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914640a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="G159" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H159" t="s">
         <v>15</v>
       </c>
       <c r="I159" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -6114,16 +6117,16 @@
         <v>194</v>
       </c>
       <c r="B161" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C161" t="s">
         <v>11</v>
       </c>
       <c r="D161" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E161" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F161">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59147ddc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6136,7 +6139,7 @@
         <v>15</v>
       </c>
       <c r="I161" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -6144,7 +6147,7 @@
         <v>194</v>
       </c>
       <c r="B162" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C162" t="s">
         <v>11</v>
@@ -6153,7 +6156,7 @@
         <v>30</v>
       </c>
       <c r="E162" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="F162">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f885e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6171,7 +6174,7 @@
         <v>194</v>
       </c>
       <c r="B163" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C163" t="s">
         <v>11</v>
@@ -6180,7 +6183,7 @@
         <v>30</v>
       </c>
       <c r="E163" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F163">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a070-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6198,7 +6201,7 @@
         <v>194</v>
       </c>
       <c r="B164" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C164" t="s">
         <v>11</v>
@@ -6207,7 +6210,7 @@
         <v>30</v>
       </c>
       <c r="E164" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F164">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f95c4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6225,7 +6228,7 @@
         <v>194</v>
       </c>
       <c r="B165" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C165" t="s">
         <v>11</v>
@@ -6234,7 +6237,7 @@
         <v>30</v>
       </c>
       <c r="E165" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F165">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f2436-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6252,7 +6255,7 @@
         <v>194</v>
       </c>
       <c r="B166" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C166" t="s">
         <v>11</v>
@@ -6261,7 +6264,7 @@
         <v>30</v>
       </c>
       <c r="E166" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F166">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59132b58-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6279,7 +6282,7 @@
         <v>194</v>
       </c>
       <c r="B167" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C167" t="s">
         <v>11</v>
@@ -6288,7 +6291,7 @@
         <v>30</v>
       </c>
       <c r="E167" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F167">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f9ace-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6306,7 +6309,7 @@
         <v>194</v>
       </c>
       <c r="B168" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C168" t="s">
         <v>11</v>
@@ -6315,7 +6318,7 @@
         <v>30</v>
       </c>
       <c r="E168" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F168">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590dd13a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6333,7 +6336,7 @@
         <v>194</v>
       </c>
       <c r="B169" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C169" t="s">
         <v>11</v>
@@ -6342,7 +6345,7 @@
         <v>30</v>
       </c>
       <c r="E169" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="F169">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59176d94-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6360,7 +6363,7 @@
         <v>194</v>
       </c>
       <c r="B170" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C170" t="s">
         <v>11</v>
@@ -6369,7 +6372,7 @@
         <v>30</v>
       </c>
       <c r="E170" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F170">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917788e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
@@ -6384,7 +6387,7 @@
     </row>
     <row r="172" spans="1:9">
       <c r="A172" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B172" t="s">
         <v>35</v>
@@ -6411,7 +6414,7 @@
     </row>
     <row r="173" spans="1:9">
       <c r="A173" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B173" t="s">
         <v>39</v>
@@ -6441,7 +6444,7 @@
     </row>
     <row r="174" spans="1:9">
       <c r="A174" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B174" t="s">
         <v>43</v>
@@ -6468,7 +6471,7 @@
     </row>
     <row r="176" spans="1:9">
       <c r="A176" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B176" t="s">
         <v>48</v>
@@ -6495,7 +6498,7 @@
     </row>
     <row r="178" spans="1:9">
       <c r="A178" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B178" t="s">
         <v>43</v>
@@ -6522,10 +6525,10 @@
     </row>
     <row r="180" spans="1:9">
       <c r="A180" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B180" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C180" t="s">
         <v>18</v>
@@ -6534,7 +6537,7 @@
         <v>30</v>
       </c>
       <c r="E180" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F180">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154d00de9ab9aff72373a673df10946a.html","web")</f>
@@ -6547,42 +6550,42 @@
         <v>15</v>
       </c>
       <c r="I180" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="181" spans="1:9">
       <c r="A181" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B181" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C181" t="s">
         <v>18</v>
       </c>
       <c r="D181" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E181" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F181">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59136b72-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="G181" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="H181" t="s">
         <v>15</v>
       </c>
       <c r="I181" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B182" t="s">
         <v>112</v>
@@ -6609,7 +6612,7 @@
     </row>
     <row r="183" spans="1:9">
       <c r="A183" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B183" t="s">
         <v>115</v>
@@ -6639,7 +6642,7 @@
     </row>
     <row r="184" spans="1:9">
       <c r="A184" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B184" t="s">
         <v>119</v>
@@ -6669,10 +6672,10 @@
     </row>
     <row r="185" spans="1:9">
       <c r="A185" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B185" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C185" t="s">
         <v>18</v>
@@ -6681,28 +6684,28 @@
         <v>30</v>
       </c>
       <c r="E185" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F185">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/be3bec2766baa15a7d57b8c2689fdf3d.html","web")</f>
         <v>0</v>
       </c>
       <c r="G185" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="H185" t="s">
         <v>15</v>
       </c>
       <c r="I185" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="186" spans="1:9">
       <c r="A186" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B186" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C186" t="s">
         <v>18</v>
@@ -6711,28 +6714,28 @@
         <v>30</v>
       </c>
       <c r="E186" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F186">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f126552ec807a8280d6d43ed084f2fc9.html","web")</f>
         <v>0</v>
       </c>
       <c r="G186" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H186" t="s">
         <v>15</v>
       </c>
       <c r="I186" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="187" spans="1:9">
       <c r="A187" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B187" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C187" t="s">
         <v>18</v>
@@ -6741,28 +6744,28 @@
         <v>30</v>
       </c>
       <c r="E187" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F187">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/15fea217c64dbec48b115765548b89ae.html","web")</f>
         <v>0</v>
       </c>
       <c r="G187" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="H187" t="s">
         <v>15</v>
       </c>
       <c r="I187" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="188" spans="1:9">
       <c r="A188" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B188" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C188" t="s">
         <v>11</v>
@@ -6771,37 +6774,37 @@
         <v>30</v>
       </c>
       <c r="E188" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F188">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d6623215ad4c16c43b649e0c17ebad7e.html","web")</f>
         <v>0</v>
       </c>
       <c r="G188" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H188" t="s">
         <v>15</v>
       </c>
       <c r="I188" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="189" spans="1:9">
       <c r="A189" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B189" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C189" t="s">
         <v>11</v>
       </c>
       <c r="D189" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E189" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F189">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/374e24b1cf7c24eb75126ea6e39ac478.html","web")</f>
@@ -6814,24 +6817,24 @@
         <v>15</v>
       </c>
       <c r="I189" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="190" spans="1:9">
       <c r="A190" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B190" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C190" t="s">
         <v>11</v>
       </c>
       <c r="D190" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E190" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F190">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1e93ae651487e683206b923c11fd6db1.html","web")</f>
@@ -6844,24 +6847,24 @@
         <v>15</v>
       </c>
       <c r="I190" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="191" spans="1:9">
       <c r="A191" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B191" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C191" t="s">
         <v>11</v>
       </c>
       <c r="D191" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E191" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F191">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9289080901a39eba6ade178d596795a.html","web")</f>
@@ -6874,24 +6877,24 @@
         <v>15</v>
       </c>
       <c r="I191" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="192" spans="1:9">
       <c r="A192" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B192" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C192" t="s">
         <v>11</v>
       </c>
       <c r="D192" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E192" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="F192">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b28e47214f0b71847c966828df0837ff.html","web")</f>
@@ -6904,24 +6907,24 @@
         <v>15</v>
       </c>
       <c r="I192" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="193" spans="1:9">
       <c r="A193" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B193" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C193" t="s">
         <v>11</v>
       </c>
       <c r="D193" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E193" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="F193">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2ca96cd5a4e83feb0d493bf9aa1a5b59.html","web")</f>
@@ -6934,24 +6937,24 @@
         <v>15</v>
       </c>
       <c r="I193" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="194" spans="1:9">
       <c r="A194" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B194" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C194" t="s">
         <v>11</v>
       </c>
       <c r="D194" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E194" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="F194">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/351c26a0f5a0cefa8f1183f2f12e1aa3.html","web")</f>
@@ -6964,15 +6967,15 @@
         <v>15</v>
       </c>
       <c r="I194" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="195" spans="1:9">
       <c r="A195" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B195" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C195" t="s">
         <v>11</v>
@@ -6981,14 +6984,14 @@
         <v>30</v>
       </c>
       <c r="E195" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F195">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/f7237f04672f809d49922d1b995f281f.html","web")</f>
         <v>0</v>
       </c>
       <c r="G195" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="H195" t="s">
         <v>15</v>
@@ -6996,10 +6999,10 @@
     </row>
     <row r="196" spans="1:9">
       <c r="A196" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B196" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C196" t="s">
         <v>11</v>
@@ -7008,14 +7011,14 @@
         <v>30</v>
       </c>
       <c r="E196" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F196">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/640213ff812312e3ac8bf134f483ed0d.html","web")</f>
         <v>0</v>
       </c>
       <c r="G196" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H196" t="s">
         <v>15</v>
@@ -7023,10 +7026,10 @@
     </row>
     <row r="197" spans="1:9">
       <c r="A197" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B197" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C197" t="s">
         <v>11</v>
@@ -7035,7 +7038,7 @@
         <v>30</v>
       </c>
       <c r="E197" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F197">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/df06d844bd95ddd2f0f62f54941c4b88.html","web")</f>
@@ -7048,15 +7051,15 @@
         <v>15</v>
       </c>
       <c r="I197" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="198" spans="1:9">
       <c r="A198" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B198" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C198" t="s">
         <v>11</v>
@@ -7065,7 +7068,7 @@
         <v>30</v>
       </c>
       <c r="E198" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F198">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fb5bd0286cdca991d0f67c498513f602.html","web")</f>
@@ -7078,15 +7081,15 @@
         <v>15</v>
       </c>
       <c r="I198" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="199" spans="1:9">
       <c r="A199" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B199" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C199" t="s">
         <v>11</v>
@@ -7095,7 +7098,7 @@
         <v>30</v>
       </c>
       <c r="E199" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F199">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/091b217c2450d012fb2e192dee04053f.html","web")</f>
@@ -7108,15 +7111,15 @@
         <v>15</v>
       </c>
       <c r="I199" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="201" spans="1:9">
       <c r="A201" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B201" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C201" t="s">
         <v>18</v>
@@ -7125,25 +7128,25 @@
         <v>30</v>
       </c>
       <c r="E201" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F201">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51e0588121783d77407236e0d2eb5d14.html","web")</f>
         <v>0</v>
       </c>
       <c r="G201" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="H201" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="I201" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="203" spans="1:9">
       <c r="A203" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B203" t="s">
         <v>43</v>
@@ -7152,7 +7155,7 @@
         <v>18</v>
       </c>
       <c r="D203" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E203" t="s">
         <v>45</v>
@@ -7170,7 +7173,7 @@
     </row>
     <row r="204" spans="1:9">
       <c r="A204" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B204" t="s">
         <v>35</v>
@@ -7179,7 +7182,7 @@
         <v>18</v>
       </c>
       <c r="D204" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E204" t="s">
         <v>36</v>
@@ -7197,7 +7200,7 @@
     </row>
     <row r="205" spans="1:9">
       <c r="A205" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B205" t="s">
         <v>39</v>
@@ -7206,7 +7209,7 @@
         <v>18</v>
       </c>
       <c r="D205" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E205" t="s">
         <v>40</v>
@@ -7227,7 +7230,7 @@
     </row>
     <row r="206" spans="1:9">
       <c r="A206" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B206" t="s">
         <v>17</v>
@@ -7236,7 +7239,7 @@
         <v>18</v>
       </c>
       <c r="D206" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E206" t="s">
         <v>20</v>
@@ -7257,7 +7260,7 @@
     </row>
     <row r="207" spans="1:9">
       <c r="A207" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B207" t="s">
         <v>24</v>
@@ -7266,7 +7269,7 @@
         <v>18</v>
       </c>
       <c r="D207" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E207" t="s">
         <v>25</v>
@@ -7287,10 +7290,10 @@
     </row>
     <row r="209" spans="1:9">
       <c r="A209" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B209" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C209" t="s">
         <v>18</v>
@@ -7299,25 +7302,25 @@
         <v>230</v>
       </c>
       <c r="E209" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F209">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5914640a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="G209" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H209" t="s">
         <v>15</v>
       </c>
       <c r="I209" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="210" spans="1:9">
       <c r="A210" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B210" t="s">
         <v>229</v>
@@ -7347,7 +7350,7 @@
     </row>
     <row r="211" spans="1:9">
       <c r="A211" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B211" t="s">
         <v>29</v>
@@ -7374,19 +7377,19 @@
     </row>
     <row r="213" spans="1:9">
       <c r="A213" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B213" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C213" t="s">
         <v>18</v>
       </c>
       <c r="D213" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E213" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F213">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/96a44ea6-b096-11e6-aab6-ac72891c3257.html","web")</f>
@@ -7399,24 +7402,24 @@
         <v>52</v>
       </c>
       <c r="I213" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="214" spans="1:9">
       <c r="A214" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B214" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C214" t="s">
         <v>18</v>
       </c>
       <c r="D214" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E214" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="F214">
         <f>HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/afef6490-b096-11e6-aab6-ac72891c3257.html","web")</f>
@@ -7429,12 +7432,12 @@
         <v>52</v>
       </c>
       <c r="I214" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="215" spans="1:9">
       <c r="A215" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B215" t="s">
         <v>178</v>
@@ -7443,7 +7446,7 @@
         <v>18</v>
       </c>
       <c r="D215" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E215" t="s">
         <v>179</v>
@@ -7461,7 +7464,7 @@
     </row>
     <row r="216" spans="1:9">
       <c r="A216" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B216" t="s">
         <v>48</v>
@@ -7470,7 +7473,7 @@
         <v>18</v>
       </c>
       <c r="D216" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E216" t="s">
         <v>183</v>

</xml_diff>

<commit_message>
Update basic ignored file for ISMIP6 and RFMIP (step 3) due to drq version 01.00.27.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4159" uniqueCount="1206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4229" uniqueCount="1220">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3638,6 +3638,48 @@
   </si>
   <si>
     <t xml:space="preserve">This is what the atmosphere sees (on its own grid).  This field should be equivalent to the combined natural fluxes of carbon  that account for natural exchanges between the atmosphere and land (nep) or ocean (fgco2) reservoirs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IyrAnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modelCellAreai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cell area of the ice sheet model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal area of ice-sheet grid cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sftgif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xant yant time typeli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of Grid Cell Covered with Glacier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of grid cell covered by land ice (ice sheet, ice shelf, ice cap, glacier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sftgrf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xant yant time typegis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grounded Ice Sheet  Area Fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of grid cell covered by grounded ice sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alevhalf spectband</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in IFS: All Up and downwelling radiation is only at the TOA and the surface available in IFS standard output. In IFS it is not possible to distinguish output in spectral intervals. Note here also global area and time averages are asked. Or maybe output at a certain diagnostic time step is meant? (No grib code available on table 128 -  Grib 1 for different spectral bands). Would it be possible to output 2 spectral bands: UV and NIR both of them diffuse and parallel. We need to ask expert of the radiation code.</t>
   </si>
 </sst>
 </file>
@@ -3757,10 +3799,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K452"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A432" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A437" activeCellId="0" sqref="437:452"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A453" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A458" activeCellId="0" sqref="A458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3774,7 +3816,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -18759,6 +18801,263 @@
         <v>240</v>
       </c>
     </row>
+    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A454" s="0" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B454" s="0" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C454" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D454" s="0" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E454" s="0" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F454" s="0" t="s">
+        <v>1167</v>
+      </c>
+      <c r="G454" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H454" s="2" t="s">
+        <v>1168</v>
+      </c>
+      <c r="I454" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="J454" s="0" t="s">
+        <v>1209</v>
+      </c>
+      <c r="K454" s="0" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A455" s="0" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B455" s="0" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C455" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D455" s="0" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E455" s="0" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F455" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G455" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H455" s="2" t="s">
+        <v>1168</v>
+      </c>
+      <c r="I455" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="J455" s="0" t="s">
+        <v>1213</v>
+      </c>
+      <c r="K455" s="0" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A456" s="0" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B456" s="0" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C456" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D456" s="0" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E456" s="0" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F456" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G456" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H456" s="2" t="s">
+        <v>1168</v>
+      </c>
+      <c r="I456" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="J456" s="0" t="s">
+        <v>1217</v>
+      </c>
+      <c r="K456" s="0" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A458" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B458" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="C458" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D458" s="0" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E458" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="F458" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G458" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bcfeacf77d49ef51a6ee66a1ab0ebcb4.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H458" s="0" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I458" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J458" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="K458" s="0" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A459" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B459" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C459" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D459" s="0" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E459" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="F459" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G459" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c323f38340e4846931ad4891232d839d.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H459" s="0" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I459" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J459" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="K459" s="0" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A460" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B460" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="C460" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D460" s="0" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E460" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="F460" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G460" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c432bfbfc0e7f4403f91af39736ff61c.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H460" s="0" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I460" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J460" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="K460" s="0" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A461" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B461" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C461" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D461" s="0" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E461" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="F461" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G461" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/eb9ac643cd9c73cae960d6d2db7b901d.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H461" s="0" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I461" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J461" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="K461" s="0" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Adding the ignored endoresed LS3MIP variables to the basic  ignored file.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4229" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4389" uniqueCount="1274">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3680,6 +3680,168 @@
   </si>
   <si>
     <t xml:space="preserve">Not available in IFS: All Up and downwelling radiation is only at the TOA and the surface available in IFS standard output. In IFS it is not possible to distinguish output in spectral intervals. Note here also global area and time averages are asked. Or maybe output at a certain diagnostic time step is meant? (No grib code available on table 128 -  Grib 1 for different spectral bands). Would it be possible to output 2 spectral bands: UV and NIR both of them diffuse and parallel. We need to ask expert of the radiation code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfdsnb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downward heat flux at snow base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in IFS output, however it is computed in H-TESSEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gijs, Andrea, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat flux from snow into the ice or land under the snow.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LS3MIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat transferred to snowpack by rainfall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emanuel Dutra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat transferred to a snow cover by rain..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Water Evaporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The surface called 'surface' means the lower boundary of the atmosphere. 'Water' means water in all phases, including frozen i.e. ice and snow. Evaporation is the conversion of liquid or solid into vapor. (The conversion of solid alone into vapor is called 'sublimation'). The quantity with standard name surface_water_evaporation_flux does not include transpiration from vegetation. In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics. Unless indicated in the cell_methods attribute, a quantity is assumed to apply to the whole area of each horizontal grid box. Previously, the qualifier where_type was used to specify that the quantity applies only to the part of the grid box of the named type. Names containing the where_type qualifier are deprecated and newly created data should use the cell_methods attribute to indicate the horizontal area to which the quantity applies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sblnosn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sublimation of the snow free area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The phrase 'tendency_of_X' means derivative of X with respect to time. 'Content' indicates a quantity per unit area. The 'atmosphere content' of a quantity refers to the vertical integral from the surface to the top of the atmosphere. For the content between specified levels in the atmosphere, standard names including content_of_atmosphere_layer are used. Atmosphere water vapor content is sometimes referred to as 'precipitable water', although this term does not imply the water could all be precipitated. The specification of a physical process by the phrase due_to_process means that the quantity named is a single term in a sum of terms which together compose the general quantity named by omitting the phrase. Sublimation is the conversion of solid into vapor. Unless indicated in the cell_methods attribute, a quantity is assumed to apply to the whole area of each horizontal grid box.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snrefr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-freezing of water in the snow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics. The surface called 'surface' means the lower boundary of the atmosphere. 'Surface snow and ice refreezing flux' means the mass flux of surface  meltwater which refreezes within the snow or firn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qgwr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groundwater recharge from soil layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not represented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics. Groundwater is subsurface water below the depth of the water table. The quantity with standard name liquid_water_mass_flux_from_soil_to_groundwater is the downward flux of liquid water within soil at the depth of the water table, or downward flux from the base of the soil model if the water table depth is greater.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">River Discharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m3 s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outflow of River Water from Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rivi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">River Inflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inflow of River Water into Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dgw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change in Groundwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The phrase 'change_over_time_in_X' means change in a quantity X over a time-interval, which should be defined by the bounds of the time coordinate. 'Water' means water in all phases. Groundwater is subsurface water below the depth of the water table. 'Amount' means mass per unit area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drivw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change in River Storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The phrase 'change_over_time_in_X' means change in a quantity X over a time-interval, which should be defined by the bounds of the time coordinate. 'Water' means water in all phases. 'River' refers to the water in the fluvial system (stream and floodplain). 'Amount' means mass per unit area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snwc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWE intercepted by the vegetation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no represented: equal to zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total water mass of the snowpack (liquid or frozen), averaged over a grid cell and interecepted by the canopy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Water Storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not represented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total liquid water storage, other than soil, snow or interception storage (i.e. lakes, river channel or depression storage).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water table depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prrsn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of rainfall on snow.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not available </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The fraction of the grid averaged rainfall which falls on the snow pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prsnsn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of snowfall (including hail and graupel) on snow.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The fraction of the snowfall which falls on the snow pack</t>
   </si>
 </sst>
 </file>
@@ -3801,8 +3963,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A453" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A458" activeCellId="0" sqref="A458"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A458" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A463" activeCellId="0" sqref="A463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19053,6 +19215,599 @@
         <v>703</v>
       </c>
     </row>
+    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A463" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B463" s="0" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C463" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D463" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E463" s="0" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F463" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G463" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/712494ba-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H463" s="0" t="s">
+        <v>1222</v>
+      </c>
+      <c r="I463" s="0" t="s">
+        <v>1223</v>
+      </c>
+      <c r="J463" s="0" t="s">
+        <v>1224</v>
+      </c>
+      <c r="K463" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A464" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B464" s="0" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C464" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D464" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E464" s="0" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F464" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G464" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913462e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H464" s="0" t="s">
+        <v>1228</v>
+      </c>
+      <c r="I464" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J464" s="0" t="s">
+        <v>1230</v>
+      </c>
+      <c r="K464" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A465" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B465" s="0" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C465" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D465" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E465" s="0" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F465" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G465" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917ca14-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H465" s="0" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I465" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J465" s="0" t="s">
+        <v>1234</v>
+      </c>
+      <c r="K465" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A466" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B466" s="0" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C466" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D466" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E466" s="0" t="s">
+        <v>1236</v>
+      </c>
+      <c r="F466" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G466" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f541a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H466" s="0" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I466" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J466" s="0" t="s">
+        <v>1237</v>
+      </c>
+      <c r="K466" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A467" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B467" s="0" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C467" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D467" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E467" s="0" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F467" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G467" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59171af6-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H467" s="0" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I467" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J467" s="0" t="s">
+        <v>1240</v>
+      </c>
+      <c r="K467" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A468" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B468" s="0" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C468" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D468" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E468" s="0" t="s">
+        <v>1242</v>
+      </c>
+      <c r="F468" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G468" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591768a8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H468" s="0" t="s">
+        <v>1243</v>
+      </c>
+      <c r="I468" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J468" s="0" t="s">
+        <v>1244</v>
+      </c>
+      <c r="K468" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A469" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B469" s="0" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C469" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D469" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E469" s="0" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F469" s="0" t="s">
+        <v>1247</v>
+      </c>
+      <c r="G469" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e05c4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H469" s="0" t="s">
+        <v>1243</v>
+      </c>
+      <c r="I469" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J469" s="0" t="s">
+        <v>1248</v>
+      </c>
+      <c r="K469" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B470" s="0" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C470" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D470" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E470" s="0" t="s">
+        <v>1250</v>
+      </c>
+      <c r="F470" s="0" t="s">
+        <v>1247</v>
+      </c>
+      <c r="G470" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e034e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H470" s="0" t="s">
+        <v>1243</v>
+      </c>
+      <c r="I470" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J470" s="0" t="s">
+        <v>1251</v>
+      </c>
+      <c r="K470" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B471" s="0" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C471" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D471" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E471" s="0" t="s">
+        <v>1253</v>
+      </c>
+      <c r="F471" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="G471" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59148822-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H471" s="0" t="s">
+        <v>1243</v>
+      </c>
+      <c r="I471" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J471" s="0" t="s">
+        <v>1254</v>
+      </c>
+      <c r="K471" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B472" s="0" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C472" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D472" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E472" s="0" t="s">
+        <v>1256</v>
+      </c>
+      <c r="F472" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="G472" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591313de-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H472" s="0" t="s">
+        <v>1243</v>
+      </c>
+      <c r="I472" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J472" s="0" t="s">
+        <v>1257</v>
+      </c>
+      <c r="K472" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B473" s="0" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C473" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D473" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E473" s="0" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F473" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="G473" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e536c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H473" s="0" t="s">
+        <v>1260</v>
+      </c>
+      <c r="I473" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J473" s="0" t="s">
+        <v>1261</v>
+      </c>
+      <c r="K473" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B474" s="0" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C474" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D474" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E474" s="0" t="s">
+        <v>1263</v>
+      </c>
+      <c r="F474" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="G474" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590eaf60-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H474" s="0" t="s">
+        <v>1264</v>
+      </c>
+      <c r="I474" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J474" s="0" t="s">
+        <v>1265</v>
+      </c>
+      <c r="K474" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A475" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B475" s="0" t="s">
+        <v>904</v>
+      </c>
+      <c r="C475" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D475" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E475" s="0" t="s">
+        <v>1266</v>
+      </c>
+      <c r="F475" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G475" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913c4dc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H475" s="0" t="s">
+        <v>1243</v>
+      </c>
+      <c r="I475" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J475" s="0" t="s">
+        <v>907</v>
+      </c>
+      <c r="K475" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B476" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C476" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D476" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E476" s="0" t="s">
+        <v>1268</v>
+      </c>
+      <c r="F476" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G476" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e3260-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H476" s="0" t="s">
+        <v>1269</v>
+      </c>
+      <c r="I476" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J476" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="K476" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B477" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C477" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D477" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E477" s="0" t="s">
+        <v>1272</v>
+      </c>
+      <c r="F477" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G477" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917ed1e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H477" s="0" t="s">
+        <v>1269</v>
+      </c>
+      <c r="I477" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J477" s="0" t="s">
+        <v>1273</v>
+      </c>
+      <c r="K477" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B478" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C478" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D478" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E478" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="F478" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="G478" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51e0588121783d77407236e0d2eb5d14.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H478" s="0" t="s">
+        <v>1269</v>
+      </c>
+      <c r="I478" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J478" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="K478" s="0" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add a block of missing Emon variables to the ignored list. Adjust in pre-list file the column format to default format.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4389" uniqueCount="1274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4509" uniqueCount="1312">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -3356,6 +3356,120 @@
   </si>
   <si>
     <t xml:space="preserve">All-sky Surface Longwave radiative flux due to Dust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsdscsdiff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Diffuse Downwelling Clear Sky Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in IFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gijs, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downwelling radiation is radiation from above. It does not mean 'net downward'. When thought of as being incident on a surface, a radiative flux is sometimes called 'irradiance'.  In addition, it is identical with the quantity measured by a cosine-collector light-meter and sometimes called 'vector irradiance'. 'Diffuse' radiation is radiation that has been scattered by particles in the atmosphere such as cloud droplets and aerosols. In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called  'flux density' in physics. The surface called 'surface' means the lower boundary of the atmosphere. A phrase 'assuming_condition' indicates that the named quantity is the value which would obtain if all aspects of the system were unaltered except for the assumption of the circumstances specified by the condition. 'shortwave' means shortwave radiation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pr18O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation Flux of Water containing Oxygen-18 (H2 18O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation mass flux of water molecules that contain the oxygen-18 isotope (H2 18O), including solid and liquid phases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prsn18O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation Flux of Snow and Ice containing Oxygen-18 (H2 18O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation mass flux of water molecules that contain the oxygen-18 isotope (H2 18O), including solid phase only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pr2h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation Flux of Water containing Deuterium (1H 2H O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation mass flux of water molecules that contain one atom of the hydrogen-2 isotope (1H 2H O), including solid and liquid phases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prsn2h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation Flux of Snow and Ice containing Deuterium (1H 2H O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation mass flux of water molecules that contain one atom of the hydrogen-2 isotope (1H 2H O), including solid phase only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pr17O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation Flux of Water containing Oxygen-17 (H2 17O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation mass flux of water molecules that contain the oxygen-17 isotope (H2 17O), including solid and liquid phases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prsn17O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation Flux of Snow and Ice containing Oxygen-17 (H2 17O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation mass flux of water molecules that contain the oxygen-17 isotope (H2 17O), including solid phase only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prw17O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass of Water containing Oxygen-17 (H2 17O) in Layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water vapor path for water molecules that contain oxygen-17 (H2 17O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prw2H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass of Water containing Deuterium (1H 2H O) in Layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water vapor path for water molecules that contain one atom of the hydrogen-2 isotope (1H 2H O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw18O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isotopic Ratio of Oxygen-17 in Sea Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio of abundance of oxygen-17 (17O) atoms to oxgen-16 (16O) atoms in sea water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sw2H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isotopic Ratio of Deuterium in Sea Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio of abundance of hydrogen-2 (2H) atoms to hydrogen-1 (1H) atoms in sea water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prw18O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isotopic Ratio of Oxygen-18 in Sea Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio of abundance of oxygen-18 (18O) atoms to oxgen-16 (16O) atoms in sea water</t>
   </si>
   <si>
     <t xml:space="preserve">Lmon</t>
@@ -3963,11 +4077,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A458" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A463" activeCellId="0" sqref="A463"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A404" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A421" activeCellId="0" sqref="A421"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
@@ -4018,6 +4132,7 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>11</v>
@@ -4054,6 +4169,7 @@
         <v>20</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>21</v>
@@ -4090,6 +4206,7 @@
         <v>30</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>31</v>
@@ -5278,6 +5395,7 @@
         <v>39</v>
       </c>
     </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>151</v>
@@ -5452,6 +5570,7 @@
         <v>157</v>
       </c>
     </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>179</v>
@@ -5485,6 +5604,7 @@
         <v>183</v>
       </c>
     </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>184</v>
@@ -5845,6 +5965,7 @@
         <v>191</v>
       </c>
     </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>224</v>
@@ -5917,6 +6038,7 @@
         <v>237</v>
       </c>
     </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>238</v>
@@ -6667,6 +6789,7 @@
         <v>240</v>
       </c>
     </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>309</v>
@@ -6703,6 +6826,7 @@
         <v>315</v>
       </c>
     </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>316</v>
@@ -6919,6 +7043,7 @@
         <v>339</v>
       </c>
     </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>343</v>
@@ -8107,6 +8232,7 @@
         <v>404</v>
       </c>
     </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>405</v>
@@ -10333,6 +10459,7 @@
         <v>552</v>
       </c>
     </row>
+    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
         <v>553</v>
@@ -10981,6 +11108,7 @@
         <v>593</v>
       </c>
     </row>
+    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
         <v>594</v>
@@ -11299,6 +11427,7 @@
         <v>605</v>
       </c>
     </row>
+    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
         <v>617</v>
@@ -11335,6 +11464,7 @@
         <v>621</v>
       </c>
     </row>
+    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
         <v>622</v>
@@ -11983,6 +12113,7 @@
         <v>638</v>
       </c>
     </row>
+    <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
         <v>689</v>
@@ -12847,6 +12978,7 @@
         <v>703</v>
       </c>
     </row>
+    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
         <v>751</v>
@@ -13060,6 +13192,7 @@
         <v>593</v>
       </c>
     </row>
+    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
         <v>752</v>
@@ -13204,6 +13337,7 @@
         <v>30</v>
       </c>
     </row>
+    <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
         <v>767</v>
@@ -13417,6 +13551,7 @@
         <v>772</v>
       </c>
     </row>
+    <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
         <v>784</v>
@@ -13453,6 +13588,7 @@
         <v>786</v>
       </c>
     </row>
+    <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
         <v>787</v>
@@ -13489,6 +13625,7 @@
         <v>593</v>
       </c>
     </row>
+    <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
         <v>793</v>
@@ -13777,6 +13914,7 @@
         <v>812</v>
       </c>
     </row>
+    <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
         <v>819</v>
@@ -13993,6 +14131,7 @@
         <v>30</v>
       </c>
     </row>
+    <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
         <v>835</v>
@@ -14137,6 +14276,7 @@
         <v>691</v>
       </c>
     </row>
+    <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
         <v>837</v>
@@ -14281,6 +14421,7 @@
         <v>593</v>
       </c>
     </row>
+    <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
         <v>854</v>
@@ -18094,12 +18235,47 @@
         <v>812</v>
       </c>
     </row>
-    <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A421" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="B421" s="0" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C421" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D421" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E421" s="0" t="s">
+        <v>1113</v>
+      </c>
+      <c r="F421" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="G421" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H421" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="I421" s="0" t="s">
+        <v>1115</v>
+      </c>
+      <c r="J421" s="0" t="s">
+        <v>1116</v>
+      </c>
+      <c r="K421" s="0" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="0" t="s">
-        <v>1112</v>
+        <v>854</v>
       </c>
       <c r="B422" s="0" t="s">
-        <v>1113</v>
+        <v>1117</v>
       </c>
       <c r="C422" s="0" t="s">
         <v>23</v>
@@ -18108,70 +18284,68 @@
         <v>137</v>
       </c>
       <c r="E422" s="0" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F422" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G422" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H422" s="0" t="s">
         <v>1114</v>
       </c>
-      <c r="F422" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="G422" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154d00de9ab9aff72373a673df10946a.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H422" s="0" t="s">
-        <v>797</v>
-      </c>
       <c r="I422" s="0" t="s">
-        <v>18</v>
+        <v>1115</v>
       </c>
       <c r="J422" s="0" t="s">
+        <v>1119</v>
+      </c>
+      <c r="K422" s="0" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A423" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="B423" s="0" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C423" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D423" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E423" s="0" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F423" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H423" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="I423" s="0" t="s">
         <v>1115</v>
       </c>
-      <c r="K422" s="0" t="s">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="0" t="s">
-        <v>1112</v>
-      </c>
-      <c r="B423" s="0" t="s">
-        <v>1117</v>
-      </c>
-      <c r="C423" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D423" s="0" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E423" s="0" t="s">
-        <v>1119</v>
-      </c>
-      <c r="F423" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="G423" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59136b72-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H423" s="0" t="s">
-        <v>1120</v>
-      </c>
-      <c r="I423" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="J423" s="0" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="K423" s="0" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="s">
-        <v>1112</v>
+        <v>854</v>
       </c>
       <c r="B424" s="0" t="s">
-        <v>838</v>
+        <v>1123</v>
       </c>
       <c r="C424" s="0" t="s">
         <v>23</v>
@@ -18180,34 +18354,33 @@
         <v>137</v>
       </c>
       <c r="E424" s="0" t="s">
-        <v>839</v>
+        <v>1124</v>
       </c>
       <c r="F424" s="0" t="s">
         <v>139</v>
       </c>
       <c r="G424" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/89c4bb4f45a0182fc00a1b86b13241a5.html","web")</f>
         <v>0</v>
       </c>
       <c r="H424" s="0" t="s">
-        <v>840</v>
+        <v>1114</v>
       </c>
       <c r="I424" s="0" t="s">
-        <v>18</v>
+        <v>1115</v>
       </c>
       <c r="J424" s="0" t="s">
-        <v>841</v>
+        <v>1125</v>
       </c>
       <c r="K424" s="0" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="s">
-        <v>1112</v>
+        <v>854</v>
       </c>
       <c r="B425" s="0" t="s">
-        <v>842</v>
+        <v>1126</v>
       </c>
       <c r="C425" s="0" t="s">
         <v>23</v>
@@ -18216,34 +18389,33 @@
         <v>137</v>
       </c>
       <c r="E425" s="0" t="s">
-        <v>843</v>
+        <v>1127</v>
       </c>
       <c r="F425" s="0" t="s">
         <v>139</v>
       </c>
       <c r="G425" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2d38bda3114d03f7543b8af88aadd03a.html","web")</f>
         <v>0</v>
       </c>
       <c r="H425" s="0" t="s">
-        <v>844</v>
+        <v>1114</v>
       </c>
       <c r="I425" s="0" t="s">
-        <v>18</v>
+        <v>1115</v>
       </c>
       <c r="J425" s="0" t="s">
-        <v>845</v>
+        <v>1128</v>
       </c>
       <c r="K425" s="0" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>1112</v>
+        <v>854</v>
       </c>
       <c r="B426" s="0" t="s">
-        <v>846</v>
+        <v>1129</v>
       </c>
       <c r="C426" s="0" t="s">
         <v>23</v>
@@ -18252,34 +18424,33 @@
         <v>137</v>
       </c>
       <c r="E426" s="0" t="s">
-        <v>847</v>
+        <v>1130</v>
       </c>
       <c r="F426" s="0" t="s">
         <v>139</v>
       </c>
       <c r="G426" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/93723bb54a2c43450d75403102e618ac.html","web")</f>
         <v>0</v>
       </c>
       <c r="H426" s="0" t="s">
-        <v>848</v>
+        <v>1114</v>
       </c>
       <c r="I426" s="0" t="s">
-        <v>18</v>
+        <v>1115</v>
       </c>
       <c r="J426" s="0" t="s">
-        <v>849</v>
+        <v>1131</v>
       </c>
       <c r="K426" s="0" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
-        <v>1112</v>
+        <v>854</v>
       </c>
       <c r="B427" s="0" t="s">
-        <v>1124</v>
+        <v>1132</v>
       </c>
       <c r="C427" s="0" t="s">
         <v>23</v>
@@ -18288,1399 +18459,1314 @@
         <v>137</v>
       </c>
       <c r="E427" s="0" t="s">
-        <v>1125</v>
+        <v>1133</v>
       </c>
       <c r="F427" s="0" t="s">
         <v>139</v>
       </c>
       <c r="G427" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/15fea217c64dbec48b115765548b89ae.html","web")</f>
         <v>0</v>
       </c>
       <c r="H427" s="0" t="s">
-        <v>1126</v>
+        <v>1114</v>
       </c>
       <c r="I427" s="0" t="s">
-        <v>18</v>
+        <v>1115</v>
       </c>
       <c r="J427" s="0" t="s">
-        <v>1127</v>
+        <v>1134</v>
       </c>
       <c r="K427" s="0" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
-        <v>1112</v>
+        <v>854</v>
       </c>
       <c r="B428" s="0" t="s">
-        <v>1129</v>
+        <v>1135</v>
       </c>
       <c r="C428" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D428" s="0" t="s">
-        <v>1130</v>
+        <v>345</v>
       </c>
       <c r="E428" s="0" t="s">
-        <v>1131</v>
+        <v>1136</v>
       </c>
       <c r="F428" s="0" t="s">
-        <v>171</v>
+        <v>509</v>
       </c>
       <c r="G428" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/374e24b1cf7c24eb75126ea6e39ac478.html","web")</f>
         <v>0</v>
       </c>
       <c r="H428" s="0" t="s">
-        <v>940</v>
+        <v>1114</v>
       </c>
       <c r="I428" s="0" t="s">
-        <v>18</v>
+        <v>1115</v>
       </c>
       <c r="J428" s="0" t="s">
-        <v>1132</v>
+        <v>1137</v>
       </c>
       <c r="K428" s="0" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
-        <v>1112</v>
+        <v>854</v>
       </c>
       <c r="B429" s="0" t="s">
-        <v>1133</v>
+        <v>1138</v>
       </c>
       <c r="C429" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D429" s="0" t="s">
-        <v>1134</v>
+        <v>345</v>
       </c>
       <c r="E429" s="0" t="s">
-        <v>1135</v>
+        <v>1139</v>
       </c>
       <c r="F429" s="0" t="s">
-        <v>171</v>
+        <v>509</v>
       </c>
       <c r="G429" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1e93ae651487e683206b923c11fd6db1.html","web")</f>
         <v>0</v>
       </c>
       <c r="H429" s="0" t="s">
-        <v>940</v>
+        <v>1114</v>
       </c>
       <c r="I429" s="0" t="s">
-        <v>18</v>
+        <v>1115</v>
       </c>
       <c r="J429" s="0" t="s">
-        <v>1136</v>
+        <v>1140</v>
       </c>
       <c r="K429" s="0" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
-        <v>1112</v>
+        <v>854</v>
       </c>
       <c r="B430" s="0" t="s">
-        <v>1137</v>
+        <v>1141</v>
       </c>
       <c r="C430" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D430" s="0" t="s">
-        <v>1138</v>
+        <v>33</v>
       </c>
       <c r="E430" s="0" t="s">
-        <v>1139</v>
+        <v>1142</v>
       </c>
       <c r="F430" s="0" t="s">
-        <v>171</v>
+        <v>23</v>
       </c>
       <c r="G430" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9289080901a39eba6ade178d596795a.html","web")</f>
         <v>0</v>
       </c>
       <c r="H430" s="0" t="s">
-        <v>940</v>
+        <v>1114</v>
       </c>
       <c r="I430" s="0" t="s">
-        <v>18</v>
+        <v>1115</v>
       </c>
       <c r="J430" s="0" t="s">
-        <v>1140</v>
+        <v>1143</v>
       </c>
       <c r="K430" s="0" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="s">
-        <v>1112</v>
+        <v>854</v>
       </c>
       <c r="B431" s="0" t="s">
-        <v>1141</v>
+        <v>1144</v>
       </c>
       <c r="C431" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D431" s="0" t="s">
-        <v>1142</v>
+        <v>33</v>
       </c>
       <c r="E431" s="0" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="F431" s="0" t="s">
-        <v>171</v>
+        <v>23</v>
       </c>
       <c r="G431" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b28e47214f0b71847c966828df0837ff.html","web")</f>
         <v>0</v>
       </c>
       <c r="H431" s="0" t="s">
-        <v>940</v>
+        <v>1114</v>
       </c>
       <c r="I431" s="0" t="s">
-        <v>18</v>
+        <v>1115</v>
       </c>
       <c r="J431" s="0" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="K431" s="0" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
-        <v>1112</v>
+        <v>854</v>
       </c>
       <c r="B432" s="0" t="s">
-        <v>1145</v>
+        <v>1147</v>
       </c>
       <c r="C432" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D432" s="0" t="s">
-        <v>1146</v>
+        <v>33</v>
       </c>
       <c r="E432" s="0" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="F432" s="0" t="s">
-        <v>171</v>
+        <v>509</v>
       </c>
       <c r="G432" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2ca96cd5a4e83feb0d493bf9aa1a5b59.html","web")</f>
         <v>0</v>
       </c>
       <c r="H432" s="0" t="s">
-        <v>940</v>
+        <v>1114</v>
       </c>
       <c r="I432" s="0" t="s">
-        <v>18</v>
+        <v>1115</v>
       </c>
       <c r="J432" s="0" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="K432" s="0" t="s">
-        <v>1149</v>
-      </c>
-    </row>
-    <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="0" t="s">
-        <v>1112</v>
-      </c>
-      <c r="B433" s="0" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="0" t="s">
         <v>1150</v>
       </c>
-      <c r="C433" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D433" s="0" t="s">
+      <c r="B435" s="0" t="s">
         <v>1151</v>
       </c>
-      <c r="E433" s="0" t="s">
-        <v>1152</v>
-      </c>
-      <c r="F433" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="G433" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/351c26a0f5a0cefa8f1183f2f12e1aa3.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H433" s="0" t="s">
-        <v>940</v>
-      </c>
-      <c r="I433" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J433" s="0" t="s">
-        <v>1153</v>
-      </c>
-      <c r="K433" s="0" t="s">
-        <v>1149</v>
-      </c>
-    </row>
-    <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="0" t="s">
-        <v>1112</v>
-      </c>
-      <c r="B434" s="0" t="s">
-        <v>1154</v>
-      </c>
-      <c r="C434" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D434" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E434" s="0" t="s">
-        <v>1155</v>
-      </c>
-      <c r="F434" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="G434" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/df06d844bd95ddd2f0f62f54941c4b88.html","web")</f>
-        <v>0</v>
-      </c>
-      <c r="H434" s="0" t="s">
-        <v>940</v>
-      </c>
-      <c r="I434" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J434" s="0" t="s">
-        <v>1156</v>
-      </c>
-      <c r="K434" s="0" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="0" t="s">
-        <v>1112</v>
-      </c>
-      <c r="B435" s="0" t="s">
-        <v>1158</v>
-      </c>
       <c r="C435" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D435" s="0" t="s">
         <v>137</v>
       </c>
       <c r="E435" s="0" t="s">
-        <v>1159</v>
+        <v>1152</v>
       </c>
       <c r="F435" s="0" t="s">
-        <v>139</v>
+        <v>509</v>
       </c>
       <c r="G435" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fb5bd0286cdca991d0f67c498513f602.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154d00de9ab9aff72373a673df10946a.html","web")</f>
         <v>0</v>
       </c>
       <c r="H435" s="0" t="s">
-        <v>940</v>
+        <v>797</v>
       </c>
       <c r="I435" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J435" s="0" t="s">
-        <v>1160</v>
+        <v>1153</v>
       </c>
       <c r="K435" s="0" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="436" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="0" t="s">
-        <v>1112</v>
+        <v>1150</v>
       </c>
       <c r="B436" s="0" t="s">
-        <v>1161</v>
+        <v>1155</v>
       </c>
       <c r="C436" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D436" s="0" t="s">
-        <v>137</v>
+        <v>1156</v>
       </c>
       <c r="E436" s="0" t="s">
-        <v>1162</v>
+        <v>1157</v>
       </c>
       <c r="F436" s="0" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="G436" s="0" t="n">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/091b217c2450d012fb2e192dee04053f.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59136b72-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>0</v>
       </c>
       <c r="H436" s="0" t="s">
-        <v>940</v>
+        <v>1158</v>
       </c>
       <c r="I436" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J436" s="0" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="K436" s="0" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A437" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B437" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="C437" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D437" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E437" s="0" t="s">
+        <v>839</v>
+      </c>
+      <c r="F437" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G437" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/89c4bb4f45a0182fc00a1b86b13241a5.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H437" s="0" t="s">
+        <v>840</v>
+      </c>
+      <c r="I437" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J437" s="0" t="s">
+        <v>841</v>
+      </c>
+      <c r="K437" s="0" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A438" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B438" s="0" t="s">
+        <v>842</v>
+      </c>
+      <c r="C438" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D438" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E438" s="0" t="s">
+        <v>843</v>
+      </c>
+      <c r="F438" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G438" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2d38bda3114d03f7543b8af88aadd03a.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H438" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="I438" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J438" s="0" t="s">
+        <v>845</v>
+      </c>
+      <c r="K438" s="0" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A439" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B439" s="0" t="s">
+        <v>846</v>
+      </c>
+      <c r="C439" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D439" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E439" s="0" t="s">
+        <v>847</v>
+      </c>
+      <c r="F439" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G439" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/93723bb54a2c43450d75403102e618ac.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H439" s="0" t="s">
+        <v>848</v>
+      </c>
+      <c r="I439" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J439" s="0" t="s">
+        <v>849</v>
+      </c>
+      <c r="K439" s="0" t="s">
+        <v>1161</v>
+      </c>
+    </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B440" s="0" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C440" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D440" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E440" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F440" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G440" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/15fea217c64dbec48b115765548b89ae.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H440" s="0" t="s">
         <v>1164</v>
       </c>
-      <c r="B440" s="0" t="s">
+      <c r="I440" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J440" s="0" t="s">
         <v>1165</v>
       </c>
-      <c r="C440" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D440" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E440" s="0" t="s">
+      <c r="K440" s="0" t="s">
         <v>1166</v>
       </c>
-      <c r="F440" s="0" t="s">
+    </row>
+    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A441" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B441" s="0" t="s">
         <v>1167</v>
       </c>
-      <c r="G440" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H440" s="2" t="s">
+      <c r="C441" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D441" s="0" t="s">
         <v>1168</v>
       </c>
-      <c r="I440" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="J440" s="0" t="s">
+      <c r="E441" s="0" t="s">
         <v>1169</v>
       </c>
-      <c r="K440" s="0" t="s">
+      <c r="F441" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G441" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/374e24b1cf7c24eb75126ea6e39ac478.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H441" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="I441" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J441" s="0" t="s">
         <v>1170</v>
       </c>
-    </row>
-    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="K441" s="0" t="s">
+        <v>1012</v>
+      </c>
+    </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B442" s="0" t="s">
         <v>1171</v>
       </c>
-      <c r="B442" s="0" t="s">
+      <c r="C442" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D442" s="0" t="s">
         <v>1172</v>
       </c>
-      <c r="C442" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D442" s="0" t="s">
+      <c r="E442" s="0" t="s">
         <v>1173</v>
       </c>
-      <c r="E442" s="0" t="s">
+      <c r="F442" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G442" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1e93ae651487e683206b923c11fd6db1.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H442" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="I442" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J442" s="0" t="s">
         <v>1174</v>
       </c>
-      <c r="F442" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="G442" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H442" s="2" t="s">
-        <v>1168</v>
-      </c>
-      <c r="I442" s="0" t="s">
+      <c r="K442" s="0" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B443" s="0" t="s">
         <v>1175</v>
       </c>
-      <c r="J442" s="0" t="s">
+      <c r="C443" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D443" s="0" t="s">
         <v>1176</v>
       </c>
-      <c r="K442" s="0" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E443" s="0" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F443" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G443" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e9289080901a39eba6ade178d596795a.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H443" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="I443" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J443" s="0" t="s">
+        <v>1178</v>
+      </c>
+      <c r="K443" s="0" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A444" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B444" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C444" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D444" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E444" s="0" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F444" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G444" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b28e47214f0b71847c966828df0837ff.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H444" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="I444" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J444" s="0" t="s">
+        <v>1182</v>
+      </c>
+      <c r="K444" s="0" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A445" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B445" s="0" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C445" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D445" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E445" s="0" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F445" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G445" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2ca96cd5a4e83feb0d493bf9aa1a5b59.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H445" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="I445" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J445" s="0" t="s">
+        <v>1186</v>
+      </c>
+      <c r="K445" s="0" t="s">
+        <v>1187</v>
+      </c>
+    </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B446" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C446" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D446" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E446" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F446" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G446" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/351c26a0f5a0cefa8f1183f2f12e1aa3.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H446" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="I446" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J446" s="0" t="s">
+        <v>1191</v>
+      </c>
+      <c r="K446" s="0" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A447" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B447" s="0" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C447" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D447" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E447" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F447" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G447" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/df06d844bd95ddd2f0f62f54941c4b88.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H447" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="I447" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J447" s="0" t="s">
+        <v>1194</v>
+      </c>
+      <c r="K447" s="0" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A448" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B448" s="0" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C448" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D448" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E448" s="0" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F448" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G448" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fb5bd0286cdca991d0f67c498513f602.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H448" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="I448" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J448" s="0" t="s">
+        <v>1198</v>
+      </c>
+      <c r="K448" s="0" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A449" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B449" s="0" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C449" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D449" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E449" s="0" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F449" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G449" s="0" t="n">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/091b217c2450d012fb2e192dee04053f.html","web")</f>
+        <v>0</v>
+      </c>
+      <c r="H449" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="I449" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J449" s="0" t="s">
+        <v>1201</v>
+      </c>
+      <c r="K449" s="0" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A453" s="0" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B453" s="0" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C453" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D453" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E453" s="0" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F453" s="0" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G453" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H453" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="I453" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="J453" s="0" t="s">
+        <v>1207</v>
+      </c>
+      <c r="K453" s="0" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A455" s="0" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B455" s="0" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C455" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D455" s="0" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E455" s="0" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F455" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G455" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H455" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="I455" s="0" t="s">
+        <v>1213</v>
+      </c>
+      <c r="J455" s="0" t="s">
+        <v>1214</v>
+      </c>
+      <c r="K455" s="0" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A459" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="B446" s="0" t="s">
-        <v>1177</v>
-      </c>
-      <c r="C446" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D446" s="0" t="s">
+      <c r="B459" s="0" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C459" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D459" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="E446" s="0" t="s">
-        <v>1178</v>
-      </c>
-      <c r="F446" s="0" t="s">
+      <c r="E459" s="0" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F459" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="G446" s="0" t="str">
+      <c r="G459" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H446" s="0" t="s">
-        <v>1179</v>
-      </c>
-      <c r="I446" s="0" t="s">
+      <c r="H459" s="0" t="s">
+        <v>1217</v>
+      </c>
+      <c r="I459" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="J446" s="0" t="s">
-        <v>1178</v>
-      </c>
-      <c r="K446" s="0" t="s">
+      <c r="J459" s="0" t="s">
+        <v>1216</v>
+      </c>
+      <c r="K459" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A447" s="0" t="s">
+    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A460" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="B447" s="0" t="s">
-        <v>1180</v>
-      </c>
-      <c r="C447" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D447" s="0" t="s">
+      <c r="B460" s="0" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C460" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D460" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="E447" s="0" t="s">
-        <v>1181</v>
-      </c>
-      <c r="F447" s="0" t="s">
+      <c r="E460" s="0" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F460" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="G447" s="0" t="str">
+      <c r="G460" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154ab10964742eaff37de9cc5beef39c.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H447" s="0" t="s">
-        <v>1182</v>
-      </c>
-      <c r="I447" s="0" t="s">
+      <c r="H460" s="0" t="s">
+        <v>1220</v>
+      </c>
+      <c r="I460" s="0" t="s">
         <v>603</v>
       </c>
-      <c r="J447" s="0" t="s">
-        <v>1183</v>
-      </c>
-      <c r="K447" s="0" t="s">
+      <c r="J460" s="0" t="s">
+        <v>1221</v>
+      </c>
+      <c r="K460" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A448" s="0" t="s">
+    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A461" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="B448" s="0" t="s">
-        <v>1184</v>
-      </c>
-      <c r="C448" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D448" s="0" t="s">
-        <v>1185</v>
-      </c>
-      <c r="E448" s="0" t="s">
-        <v>1186</v>
-      </c>
-      <c r="F448" s="0" t="s">
-        <v>1187</v>
-      </c>
-      <c r="G448" s="0" t="str">
+      <c r="B461" s="0" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C461" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D461" s="0" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E461" s="0" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F461" s="0" t="s">
+        <v>1225</v>
+      </c>
+      <c r="G461" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/21ef5e4c-b894-11e6-a189-5404a60d96b5.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H448" s="0" t="s">
-        <v>1188</v>
-      </c>
-      <c r="I448" s="0" t="s">
+      <c r="H461" s="0" t="s">
+        <v>1226</v>
+      </c>
+      <c r="I461" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="J448" s="0" t="s">
-        <v>1189</v>
-      </c>
-      <c r="K448" s="0" t="s">
+      <c r="J461" s="0" t="s">
+        <v>1227</v>
+      </c>
+      <c r="K461" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="0" t="s">
+    <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A462" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="B449" s="0" t="s">
-        <v>1190</v>
-      </c>
-      <c r="C449" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D449" s="0" t="s">
-        <v>1185</v>
-      </c>
-      <c r="E449" s="0" t="s">
-        <v>1191</v>
-      </c>
-      <c r="F449" s="0" t="s">
-        <v>1192</v>
-      </c>
-      <c r="G449" s="0" t="str">
+      <c r="B462" s="0" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C462" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D462" s="0" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E462" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="F462" s="0" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G462" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2260e24c-b894-11e6-a189-5404a60d96b5.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H449" s="0" t="s">
-        <v>1188</v>
-      </c>
-      <c r="I449" s="0" t="s">
+      <c r="H462" s="0" t="s">
+        <v>1226</v>
+      </c>
+      <c r="I462" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="J449" s="0" t="s">
-        <v>1193</v>
-      </c>
-      <c r="K449" s="0" t="s">
+      <c r="J462" s="0" t="s">
+        <v>1231</v>
+      </c>
+      <c r="K462" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A450" s="0" t="s">
+    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A463" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="B450" s="0" t="s">
-        <v>1194</v>
-      </c>
-      <c r="C450" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D450" s="0" t="s">
+      <c r="B463" s="0" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C463" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D463" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="E450" s="0" t="s">
-        <v>1195</v>
-      </c>
-      <c r="F450" s="0" t="s">
+      <c r="E463" s="0" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F463" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="G450" s="0" t="str">
+      <c r="G463" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc1b9e3073d751143fe8ab63ca9fcc45.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H450" s="0" t="s">
-        <v>1196</v>
-      </c>
-      <c r="I450" s="0" t="s">
+      <c r="H463" s="0" t="s">
+        <v>1234</v>
+      </c>
+      <c r="I463" s="0" t="s">
         <v>603</v>
       </c>
-      <c r="J450" s="0" t="s">
-        <v>1197</v>
-      </c>
-      <c r="K450" s="0" t="s">
+      <c r="J463" s="0" t="s">
+        <v>1235</v>
+      </c>
+      <c r="K463" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A451" s="0" t="s">
+    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A464" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="B451" s="0" t="s">
-        <v>1198</v>
-      </c>
-      <c r="C451" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D451" s="0" t="s">
+      <c r="B464" s="0" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C464" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D464" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="E451" s="0" t="s">
-        <v>1199</v>
-      </c>
-      <c r="F451" s="0" t="s">
+      <c r="E464" s="0" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F464" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="G451" s="0" t="str">
+      <c r="G464" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5e49c0b73ac161d5e5dd05173416c400.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H451" s="0" t="s">
-        <v>1200</v>
-      </c>
-      <c r="I451" s="0" t="s">
+      <c r="H464" s="0" t="s">
+        <v>1238</v>
+      </c>
+      <c r="I464" s="0" t="s">
         <v>603</v>
       </c>
-      <c r="J451" s="0" t="s">
-        <v>1201</v>
-      </c>
-      <c r="K451" s="0" t="s">
+      <c r="J464" s="0" t="s">
+        <v>1239</v>
+      </c>
+      <c r="K464" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A452" s="0" t="s">
+    <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A465" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="B452" s="0" t="s">
-        <v>1202</v>
-      </c>
-      <c r="C452" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D452" s="0" t="s">
+      <c r="B465" s="0" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C465" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D465" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="E452" s="0" t="s">
-        <v>1203</v>
-      </c>
-      <c r="F452" s="0" t="s">
+      <c r="E465" s="0" t="s">
+        <v>1241</v>
+      </c>
+      <c r="F465" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="G452" s="0" t="str">
+      <c r="G465" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/299fb9d19040c4aa3862644286261ad2.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H452" s="0" t="s">
-        <v>1204</v>
-      </c>
-      <c r="I452" s="0" t="s">
+      <c r="H465" s="0" t="s">
+        <v>1242</v>
+      </c>
+      <c r="I465" s="0" t="s">
         <v>603</v>
       </c>
-      <c r="J452" s="0" t="s">
+      <c r="J465" s="0" t="s">
+        <v>1243</v>
+      </c>
+      <c r="K465" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A467" s="0" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B467" s="0" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C467" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D467" s="0" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E467" s="0" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F467" s="0" t="s">
         <v>1205</v>
       </c>
-      <c r="K452" s="0" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A454" s="0" t="s">
-        <v>1206</v>
-      </c>
-      <c r="B454" s="0" t="s">
-        <v>1207</v>
-      </c>
-      <c r="C454" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D454" s="0" t="s">
-        <v>1173</v>
-      </c>
-      <c r="E454" s="0" t="s">
-        <v>1208</v>
-      </c>
-      <c r="F454" s="0" t="s">
-        <v>1167</v>
-      </c>
-      <c r="G454" s="0" t="str">
+      <c r="G467" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/865d0e00-53e6-11e6-b524-5404a60d96b5.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H454" s="2" t="s">
-        <v>1168</v>
-      </c>
-      <c r="I454" s="0" t="s">
+      <c r="H467" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="I467" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="J454" s="0" t="s">
-        <v>1209</v>
-      </c>
-      <c r="K454" s="0" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A455" s="0" t="s">
-        <v>1206</v>
-      </c>
-      <c r="B455" s="0" t="s">
-        <v>1210</v>
-      </c>
-      <c r="C455" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D455" s="0" t="s">
-        <v>1211</v>
-      </c>
-      <c r="E455" s="0" t="s">
-        <v>1212</v>
-      </c>
-      <c r="F455" s="0" t="s">
+      <c r="J467" s="0" t="s">
+        <v>1247</v>
+      </c>
+      <c r="K467" s="0" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A468" s="0" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B468" s="0" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C468" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D468" s="0" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E468" s="0" t="s">
+        <v>1250</v>
+      </c>
+      <c r="F468" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="G455" s="0" t="str">
+      <c r="G468" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a1d2e309c6f25017442ad6c79c4f9eca.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H455" s="2" t="s">
-        <v>1168</v>
-      </c>
-      <c r="I455" s="0" t="s">
+      <c r="H468" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="I468" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="J455" s="0" t="s">
-        <v>1213</v>
-      </c>
-      <c r="K455" s="0" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A456" s="0" t="s">
-        <v>1206</v>
-      </c>
-      <c r="B456" s="0" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C456" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D456" s="0" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E456" s="0" t="s">
-        <v>1216</v>
-      </c>
-      <c r="F456" s="0" t="s">
+      <c r="J468" s="0" t="s">
+        <v>1251</v>
+      </c>
+      <c r="K468" s="0" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A469" s="0" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B469" s="0" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C469" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D469" s="0" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E469" s="0" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F469" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="G456" s="0" t="str">
+      <c r="G469" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e5de4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H456" s="2" t="s">
-        <v>1168</v>
-      </c>
-      <c r="I456" s="0" t="s">
+      <c r="H469" s="2" t="s">
+        <v>1206</v>
+      </c>
+      <c r="I469" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="J456" s="0" t="s">
-        <v>1217</v>
-      </c>
-      <c r="K456" s="0" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A458" s="0" t="s">
+      <c r="J469" s="0" t="s">
+        <v>1255</v>
+      </c>
+      <c r="K469" s="0" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B458" s="0" t="s">
+      <c r="B471" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="C458" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D458" s="0" t="s">
-        <v>1218</v>
-      </c>
-      <c r="E458" s="0" t="s">
+      <c r="C471" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D471" s="0" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E471" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="F458" s="0" t="s">
+      <c r="F471" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="G458" s="0" t="str">
+      <c r="G471" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bcfeacf77d49ef51a6ee66a1ab0ebcb4.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H458" s="0" t="s">
-        <v>1219</v>
-      </c>
-      <c r="I458" s="0" t="s">
+      <c r="H471" s="0" t="s">
+        <v>1257</v>
+      </c>
+      <c r="I471" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="J458" s="0" t="s">
+      <c r="J471" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="K458" s="0" t="s">
+      <c r="K471" s="0" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A459" s="0" t="s">
+    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B459" s="0" t="s">
+      <c r="B472" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="C459" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D459" s="0" t="s">
-        <v>1218</v>
-      </c>
-      <c r="E459" s="0" t="s">
+      <c r="C472" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D472" s="0" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E472" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="F459" s="0" t="s">
+      <c r="F472" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="G459" s="0" t="str">
+      <c r="G472" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c323f38340e4846931ad4891232d839d.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H459" s="0" t="s">
-        <v>1219</v>
-      </c>
-      <c r="I459" s="0" t="s">
+      <c r="H472" s="0" t="s">
+        <v>1257</v>
+      </c>
+      <c r="I472" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="J459" s="0" t="s">
+      <c r="J472" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="K459" s="0" t="s">
+      <c r="K472" s="0" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A460" s="0" t="s">
+    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B460" s="0" t="s">
+      <c r="B473" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="C460" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D460" s="0" t="s">
-        <v>1218</v>
-      </c>
-      <c r="E460" s="0" t="s">
+      <c r="C473" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D473" s="0" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E473" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="F460" s="0" t="s">
+      <c r="F473" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="G460" s="0" t="str">
+      <c r="G473" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c432bfbfc0e7f4403f91af39736ff61c.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H460" s="0" t="s">
-        <v>1219</v>
-      </c>
-      <c r="I460" s="0" t="s">
+      <c r="H473" s="0" t="s">
+        <v>1257</v>
+      </c>
+      <c r="I473" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="J460" s="0" t="s">
+      <c r="J473" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="K460" s="0" t="s">
+      <c r="K473" s="0" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A461" s="0" t="s">
+    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B461" s="0" t="s">
+      <c r="B474" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="C461" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D461" s="0" t="s">
-        <v>1218</v>
-      </c>
-      <c r="E461" s="0" t="s">
+      <c r="C474" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D474" s="0" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E474" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="F461" s="0" t="s">
+      <c r="F474" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="G461" s="0" t="str">
+      <c r="G474" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/eb9ac643cd9c73cae960d6d2db7b901d.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H461" s="0" t="s">
-        <v>1219</v>
-      </c>
-      <c r="I461" s="0" t="s">
+      <c r="H474" s="0" t="s">
+        <v>1257</v>
+      </c>
+      <c r="I474" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="J461" s="0" t="s">
+      <c r="J474" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="K461" s="0" t="s">
+      <c r="K474" s="0" t="s">
         <v>703</v>
-      </c>
-    </row>
-    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A463" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B463" s="0" t="s">
-        <v>1220</v>
-      </c>
-      <c r="C463" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D463" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E463" s="0" t="s">
-        <v>1221</v>
-      </c>
-      <c r="F463" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="G463" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/712494ba-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H463" s="0" t="s">
-        <v>1222</v>
-      </c>
-      <c r="I463" s="0" t="s">
-        <v>1223</v>
-      </c>
-      <c r="J463" s="0" t="s">
-        <v>1224</v>
-      </c>
-      <c r="K463" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A464" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B464" s="0" t="s">
-        <v>1226</v>
-      </c>
-      <c r="C464" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D464" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E464" s="0" t="s">
-        <v>1227</v>
-      </c>
-      <c r="F464" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="G464" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913462e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H464" s="0" t="s">
-        <v>1228</v>
-      </c>
-      <c r="I464" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J464" s="0" t="s">
-        <v>1230</v>
-      </c>
-      <c r="K464" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A465" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B465" s="0" t="s">
-        <v>1231</v>
-      </c>
-      <c r="C465" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D465" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E465" s="0" t="s">
-        <v>1232</v>
-      </c>
-      <c r="F465" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="G465" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917ca14-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H465" s="0" t="s">
-        <v>1233</v>
-      </c>
-      <c r="I465" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J465" s="0" t="s">
-        <v>1234</v>
-      </c>
-      <c r="K465" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A466" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B466" s="0" t="s">
-        <v>1235</v>
-      </c>
-      <c r="C466" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D466" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E466" s="0" t="s">
-        <v>1236</v>
-      </c>
-      <c r="F466" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="G466" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f541a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H466" s="0" t="s">
-        <v>1233</v>
-      </c>
-      <c r="I466" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J466" s="0" t="s">
-        <v>1237</v>
-      </c>
-      <c r="K466" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A467" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B467" s="0" t="s">
-        <v>1238</v>
-      </c>
-      <c r="C467" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D467" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E467" s="0" t="s">
-        <v>1239</v>
-      </c>
-      <c r="F467" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="G467" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59171af6-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H467" s="0" t="s">
-        <v>1233</v>
-      </c>
-      <c r="I467" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J467" s="0" t="s">
-        <v>1240</v>
-      </c>
-      <c r="K467" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A468" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B468" s="0" t="s">
-        <v>1241</v>
-      </c>
-      <c r="C468" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D468" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E468" s="0" t="s">
-        <v>1242</v>
-      </c>
-      <c r="F468" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="G468" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591768a8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H468" s="0" t="s">
-        <v>1243</v>
-      </c>
-      <c r="I468" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J468" s="0" t="s">
-        <v>1244</v>
-      </c>
-      <c r="K468" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A469" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B469" s="0" t="s">
-        <v>1245</v>
-      </c>
-      <c r="C469" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D469" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E469" s="0" t="s">
-        <v>1246</v>
-      </c>
-      <c r="F469" s="0" t="s">
-        <v>1247</v>
-      </c>
-      <c r="G469" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e05c4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H469" s="0" t="s">
-        <v>1243</v>
-      </c>
-      <c r="I469" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J469" s="0" t="s">
-        <v>1248</v>
-      </c>
-      <c r="K469" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A470" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B470" s="0" t="s">
-        <v>1249</v>
-      </c>
-      <c r="C470" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D470" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E470" s="0" t="s">
-        <v>1250</v>
-      </c>
-      <c r="F470" s="0" t="s">
-        <v>1247</v>
-      </c>
-      <c r="G470" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e034e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H470" s="0" t="s">
-        <v>1243</v>
-      </c>
-      <c r="I470" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J470" s="0" t="s">
-        <v>1251</v>
-      </c>
-      <c r="K470" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A471" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B471" s="0" t="s">
-        <v>1252</v>
-      </c>
-      <c r="C471" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D471" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E471" s="0" t="s">
-        <v>1253</v>
-      </c>
-      <c r="F471" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="G471" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59148822-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H471" s="0" t="s">
-        <v>1243</v>
-      </c>
-      <c r="I471" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J471" s="0" t="s">
-        <v>1254</v>
-      </c>
-      <c r="K471" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A472" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B472" s="0" t="s">
-        <v>1255</v>
-      </c>
-      <c r="C472" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D472" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E472" s="0" t="s">
-        <v>1256</v>
-      </c>
-      <c r="F472" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="G472" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591313de-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H472" s="0" t="s">
-        <v>1243</v>
-      </c>
-      <c r="I472" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J472" s="0" t="s">
-        <v>1257</v>
-      </c>
-      <c r="K472" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A473" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B473" s="0" t="s">
-        <v>1258</v>
-      </c>
-      <c r="C473" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D473" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E473" s="0" t="s">
-        <v>1259</v>
-      </c>
-      <c r="F473" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="G473" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e536c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H473" s="0" t="s">
-        <v>1260</v>
-      </c>
-      <c r="I473" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J473" s="0" t="s">
-        <v>1261</v>
-      </c>
-      <c r="K473" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A474" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B474" s="0" t="s">
-        <v>1262</v>
-      </c>
-      <c r="C474" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D474" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E474" s="0" t="s">
-        <v>1263</v>
-      </c>
-      <c r="F474" s="0" t="s">
-        <v>509</v>
-      </c>
-      <c r="G474" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590eaf60-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H474" s="0" t="s">
-        <v>1264</v>
-      </c>
-      <c r="I474" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J474" s="0" t="s">
-        <v>1265</v>
-      </c>
-      <c r="K474" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="0" t="s">
-        <v>793</v>
-      </c>
-      <c r="B475" s="0" t="s">
-        <v>904</v>
-      </c>
-      <c r="C475" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D475" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E475" s="0" t="s">
-        <v>1266</v>
-      </c>
-      <c r="F475" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G475" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913c4dc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H475" s="0" t="s">
-        <v>1243</v>
-      </c>
-      <c r="I475" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J475" s="0" t="s">
-        <v>907</v>
-      </c>
-      <c r="K475" s="0" t="s">
-        <v>1225</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19688,7 +19774,7 @@
         <v>793</v>
       </c>
       <c r="B476" s="0" t="s">
-        <v>1267</v>
+        <v>1258</v>
       </c>
       <c r="C476" s="0" t="s">
         <v>23</v>
@@ -19697,26 +19783,26 @@
         <v>137</v>
       </c>
       <c r="E476" s="0" t="s">
-        <v>1268</v>
+        <v>1259</v>
       </c>
       <c r="F476" s="0" t="s">
-        <v>23</v>
+        <v>243</v>
       </c>
       <c r="G476" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e3260-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/712494ba-c7b6-11e6-bb2a-ac72891c3257.html","web")</f>
         <v>web</v>
       </c>
       <c r="H476" s="0" t="s">
-        <v>1269</v>
+        <v>1260</v>
       </c>
       <c r="I476" s="0" t="s">
-        <v>1229</v>
+        <v>1261</v>
       </c>
       <c r="J476" s="0" t="s">
-        <v>1270</v>
+        <v>1262</v>
       </c>
       <c r="K476" s="0" t="s">
-        <v>1225</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19724,7 +19810,7 @@
         <v>793</v>
       </c>
       <c r="B477" s="0" t="s">
-        <v>1271</v>
+        <v>1264</v>
       </c>
       <c r="C477" s="0" t="s">
         <v>23</v>
@@ -19733,26 +19819,26 @@
         <v>137</v>
       </c>
       <c r="E477" s="0" t="s">
-        <v>1272</v>
+        <v>1265</v>
       </c>
       <c r="F477" s="0" t="s">
-        <v>23</v>
+        <v>243</v>
       </c>
       <c r="G477" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917ed1e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913462e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
       <c r="H477" s="0" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="I477" s="0" t="s">
-        <v>1229</v>
+        <v>1267</v>
       </c>
       <c r="J477" s="0" t="s">
-        <v>1273</v>
+        <v>1268</v>
       </c>
       <c r="K477" s="0" t="s">
-        <v>1225</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19760,7 +19846,7 @@
         <v>793</v>
       </c>
       <c r="B478" s="0" t="s">
-        <v>225</v>
+        <v>1269</v>
       </c>
       <c r="C478" s="0" t="s">
         <v>23</v>
@@ -19769,48 +19855,496 @@
         <v>137</v>
       </c>
       <c r="E478" s="0" t="s">
+        <v>1270</v>
+      </c>
+      <c r="F478" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G478" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917ca14-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H478" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="I478" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J478" s="0" t="s">
+        <v>1272</v>
+      </c>
+      <c r="K478" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B479" s="0" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C479" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D479" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E479" s="0" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F479" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G479" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f541a-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H479" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="I479" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J479" s="0" t="s">
+        <v>1275</v>
+      </c>
+      <c r="K479" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B480" s="0" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C480" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D480" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E480" s="0" t="s">
+        <v>1277</v>
+      </c>
+      <c r="F480" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G480" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59171af6-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H480" s="0" t="s">
+        <v>1271</v>
+      </c>
+      <c r="I480" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J480" s="0" t="s">
+        <v>1278</v>
+      </c>
+      <c r="K480" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A481" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B481" s="0" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C481" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D481" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E481" s="0" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F481" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G481" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591768a8-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H481" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="I481" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J481" s="0" t="s">
+        <v>1282</v>
+      </c>
+      <c r="K481" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B482" s="0" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C482" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D482" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E482" s="0" t="s">
+        <v>1284</v>
+      </c>
+      <c r="F482" s="0" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G482" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e05c4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H482" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="I482" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J482" s="0" t="s">
+        <v>1286</v>
+      </c>
+      <c r="K482" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A483" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B483" s="0" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C483" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D483" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E483" s="0" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F483" s="0" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G483" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e034e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H483" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="I483" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J483" s="0" t="s">
+        <v>1289</v>
+      </c>
+      <c r="K483" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A484" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B484" s="0" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C484" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D484" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E484" s="0" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F484" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="G484" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/59148822-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H484" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="I484" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J484" s="0" t="s">
+        <v>1292</v>
+      </c>
+      <c r="K484" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A485" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B485" s="0" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C485" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D485" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E485" s="0" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F485" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="G485" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/591313de-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H485" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="I485" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J485" s="0" t="s">
+        <v>1295</v>
+      </c>
+      <c r="K485" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A486" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B486" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C486" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D486" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E486" s="0" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F486" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="G486" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e536c-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H486" s="0" t="s">
+        <v>1298</v>
+      </c>
+      <c r="I486" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J486" s="0" t="s">
+        <v>1299</v>
+      </c>
+      <c r="K486" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A487" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B487" s="0" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C487" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D487" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E487" s="0" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F487" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="G487" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590eaf60-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H487" s="0" t="s">
+        <v>1302</v>
+      </c>
+      <c r="I487" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J487" s="0" t="s">
+        <v>1303</v>
+      </c>
+      <c r="K487" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A488" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B488" s="0" t="s">
+        <v>904</v>
+      </c>
+      <c r="C488" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D488" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E488" s="0" t="s">
+        <v>1304</v>
+      </c>
+      <c r="F488" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G488" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913c4dc-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H488" s="0" t="s">
+        <v>1281</v>
+      </c>
+      <c r="I488" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J488" s="0" t="s">
+        <v>907</v>
+      </c>
+      <c r="K488" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A489" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B489" s="0" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C489" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D489" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E489" s="0" t="s">
+        <v>1306</v>
+      </c>
+      <c r="F489" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G489" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590e3260-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H489" s="0" t="s">
+        <v>1307</v>
+      </c>
+      <c r="I489" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J489" s="0" t="s">
+        <v>1308</v>
+      </c>
+      <c r="K489" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A490" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B490" s="0" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C490" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D490" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E490" s="0" t="s">
+        <v>1310</v>
+      </c>
+      <c r="F490" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G490" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917ed1e-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H490" s="0" t="s">
+        <v>1307</v>
+      </c>
+      <c r="I490" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J490" s="0" t="s">
+        <v>1311</v>
+      </c>
+      <c r="K490" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A491" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="B491" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C491" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D491" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E491" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="F478" s="0" t="s">
+      <c r="F491" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="G478" s="0" t="str">
+      <c r="G491" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51e0588121783d77407236e0d2eb5d14.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H478" s="0" t="s">
-        <v>1269</v>
-      </c>
-      <c r="I478" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="J478" s="0" t="s">
+      <c r="H491" s="0" t="s">
+        <v>1307</v>
+      </c>
+      <c r="I491" s="0" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J491" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="K478" s="0" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="K491" s="0" t="s">
+        <v>1263</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Add Emon ec550aer to the ignored file #342.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4759" uniqueCount="1405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4769" uniqueCount="1411">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -4052,6 +4052,24 @@
   </si>
   <si>
     <t xml:space="preserve">aerosol optical depth at 550 nm due to stratospheric volcanic aerosols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ec550aer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude latitude alevel time lambda550nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerosol extinction coefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Though available for 6hrLev  tm5 code name = ec550aer this variable is not available for Emon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerosol Extinction at 550nm</t>
   </si>
   <si>
     <t xml:space="preserve">E6hrZ</t>
@@ -4364,8 +4382,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C492" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H508" activeCellId="0" sqref="H508:I523"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B484" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H504" activeCellId="0" sqref="H504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4379,7 +4397,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -20863,146 +20881,112 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A504" s="0" t="s">
+    <row r="504" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="B504" s="3" t="s">
         <v>1344</v>
       </c>
-      <c r="B504" s="0" t="s">
+      <c r="C504" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D504" s="3" t="s">
         <v>1345</v>
       </c>
-      <c r="C504" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D504" s="0" t="s">
+      <c r="E504" s="3" t="s">
         <v>1346</v>
       </c>
-      <c r="E504" s="0" t="s">
+      <c r="F504" s="3" t="s">
         <v>1347</v>
       </c>
-      <c r="F504" s="0" t="s">
+      <c r="G504" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/be9cffbb781e32b0bc311b22fa5c0322.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H504" s="3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="I504" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="J504" s="3" t="s">
+        <v>1349</v>
+      </c>
+      <c r="K504" s="3" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A506" s="0" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B506" s="0" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C506" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D506" s="0" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E506" s="0" t="s">
+        <v>1353</v>
+      </c>
+      <c r="F506" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="G504" s="0" t="str">
+      <c r="G506" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590d64f2-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H504" s="4" t="s">
+      <c r="H506" s="4" t="s">
         <v>1335</v>
       </c>
-      <c r="I504" s="4" t="s">
+      <c r="I506" s="4" t="s">
         <v>682</v>
       </c>
-      <c r="J504" s="0" t="s">
-        <v>1348</v>
-      </c>
-      <c r="K504" s="0" t="s">
+      <c r="J506" s="0" t="s">
+        <v>1354</v>
+      </c>
+      <c r="K506" s="0" t="s">
         <v>1337</v>
       </c>
     </row>
-    <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A505" s="0" t="s">
-        <v>1344</v>
-      </c>
-      <c r="B505" s="0" t="s">
-        <v>1349</v>
-      </c>
-      <c r="C505" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D505" s="0" t="s">
-        <v>1346</v>
-      </c>
-      <c r="E505" s="0" t="s">
+    <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A507" s="0" t="s">
         <v>1350</v>
       </c>
-      <c r="F505" s="0" t="s">
+      <c r="B507" s="0" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C507" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D507" s="0" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E507" s="0" t="s">
+        <v>1356</v>
+      </c>
+      <c r="F507" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="G505" s="0" t="str">
+      <c r="G507" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5913d0c6-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H505" s="4" t="s">
+      <c r="H507" s="4" t="s">
         <v>1335</v>
       </c>
-      <c r="I505" s="4" t="s">
+      <c r="I507" s="4" t="s">
         <v>682</v>
       </c>
-      <c r="J505" s="0" t="s">
-        <v>1351</v>
-      </c>
-      <c r="K505" s="0" t="s">
+      <c r="J507" s="0" t="s">
+        <v>1357</v>
+      </c>
+      <c r="K507" s="0" t="s">
         <v>1337</v>
-      </c>
-    </row>
-    <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A508" s="0" t="s">
-        <v>890</v>
-      </c>
-      <c r="B508" s="0" t="s">
-        <v>1352</v>
-      </c>
-      <c r="C508" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D508" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="E508" s="0" t="s">
-        <v>1353</v>
-      </c>
-      <c r="F508" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="G508" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H508" s="3" t="s">
-        <v>1354</v>
-      </c>
-      <c r="I508" s="3" t="s">
-        <v>1355</v>
-      </c>
-      <c r="J508" s="0" t="s">
-        <v>1356</v>
-      </c>
-      <c r="K508" s="0" t="s">
-        <v>1357</v>
-      </c>
-    </row>
-    <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A509" s="0" t="s">
-        <v>890</v>
-      </c>
-      <c r="B509" s="0" t="s">
-        <v>1358</v>
-      </c>
-      <c r="C509" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D509" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="E509" s="0" t="s">
-        <v>1359</v>
-      </c>
-      <c r="F509" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="G509" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H509" s="3" t="s">
-        <v>1360</v>
-      </c>
-      <c r="I509" s="3" t="s">
-        <v>1012</v>
-      </c>
-      <c r="J509" s="0" t="s">
-        <v>1361</v>
-      </c>
-      <c r="K509" s="0" t="s">
-        <v>1357</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21010,7 +20994,7 @@
         <v>890</v>
       </c>
       <c r="B510" s="0" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
       <c r="C510" s="0" t="s">
         <v>31</v>
@@ -21019,25 +21003,25 @@
         <v>171</v>
       </c>
       <c r="E510" s="0" t="s">
+        <v>1359</v>
+      </c>
+      <c r="F510" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="G510" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H510" s="3" t="s">
+        <v>1360</v>
+      </c>
+      <c r="I510" s="3" t="s">
+        <v>1361</v>
+      </c>
+      <c r="J510" s="0" t="s">
+        <v>1362</v>
+      </c>
+      <c r="K510" s="0" t="s">
         <v>1363</v>
-      </c>
-      <c r="F510" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="G510" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H510" s="3" t="s">
-        <v>1364</v>
-      </c>
-      <c r="I510" s="3" t="s">
-        <v>1012</v>
-      </c>
-      <c r="J510" s="0" t="s">
-        <v>1365</v>
-      </c>
-      <c r="K510" s="0" t="s">
-        <v>1357</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21045,7 +21029,7 @@
         <v>890</v>
       </c>
       <c r="B511" s="0" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="C511" s="0" t="s">
         <v>31</v>
@@ -21054,25 +21038,25 @@
         <v>171</v>
       </c>
       <c r="E511" s="0" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="F511" s="0" t="s">
-        <v>173</v>
+        <v>278</v>
       </c>
       <c r="G511" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H511" s="3" t="s">
-        <v>1364</v>
+        <v>1366</v>
       </c>
       <c r="I511" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="J511" s="0" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="K511" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21080,7 +21064,7 @@
         <v>890</v>
       </c>
       <c r="B512" s="0" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="C512" s="0" t="s">
         <v>31</v>
@@ -21089,7 +21073,7 @@
         <v>171</v>
       </c>
       <c r="E512" s="0" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="F512" s="0" t="s">
         <v>173</v>
@@ -21098,7 +21082,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="3" t="s">
-        <v>1364</v>
+        <v>1370</v>
       </c>
       <c r="I512" s="3" t="s">
         <v>1012</v>
@@ -21107,7 +21091,7 @@
         <v>1371</v>
       </c>
       <c r="K512" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21133,16 +21117,16 @@
         <v>0</v>
       </c>
       <c r="H513" s="3" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="I513" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="J513" s="0" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="K513" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21150,7 +21134,7 @@
         <v>890</v>
       </c>
       <c r="B514" s="0" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="C514" s="0" t="s">
         <v>31</v>
@@ -21159,25 +21143,25 @@
         <v>171</v>
       </c>
       <c r="E514" s="0" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="F514" s="0" t="s">
-        <v>1378</v>
+        <v>173</v>
       </c>
       <c r="G514" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H514" s="3" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="I514" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="J514" s="0" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="K514" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21185,7 +21169,7 @@
         <v>890</v>
       </c>
       <c r="B515" s="0" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="C515" s="0" t="s">
         <v>31</v>
@@ -21194,25 +21178,25 @@
         <v>171</v>
       </c>
       <c r="E515" s="0" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="F515" s="0" t="s">
-        <v>1378</v>
+        <v>173</v>
       </c>
       <c r="G515" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H515" s="3" t="s">
-        <v>1374</v>
+        <v>1380</v>
       </c>
       <c r="I515" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="J515" s="0" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="K515" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21220,7 +21204,7 @@
         <v>890</v>
       </c>
       <c r="B516" s="0" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="C516" s="0" t="s">
         <v>31</v>
@@ -21229,16 +21213,16 @@
         <v>171</v>
       </c>
       <c r="E516" s="0" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F516" s="0" t="s">
         <v>1384</v>
       </c>
-      <c r="F516" s="0" t="s">
-        <v>894</v>
-      </c>
       <c r="G516" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H516" s="3" t="s">
-        <v>1374</v>
+        <v>1380</v>
       </c>
       <c r="I516" s="3" t="s">
         <v>1012</v>
@@ -21247,7 +21231,7 @@
         <v>1385</v>
       </c>
       <c r="K516" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21267,13 +21251,13 @@
         <v>1387</v>
       </c>
       <c r="F517" s="0" t="s">
-        <v>894</v>
+        <v>1384</v>
       </c>
       <c r="G517" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H517" s="3" t="s">
-        <v>1374</v>
+        <v>1380</v>
       </c>
       <c r="I517" s="3" t="s">
         <v>1012</v>
@@ -21282,7 +21266,7 @@
         <v>1388</v>
       </c>
       <c r="K517" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21308,16 +21292,16 @@
         <v>0</v>
       </c>
       <c r="H518" s="3" t="s">
-        <v>1391</v>
+        <v>1380</v>
       </c>
       <c r="I518" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="J518" s="0" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="K518" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21325,7 +21309,7 @@
         <v>890</v>
       </c>
       <c r="B519" s="0" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="C519" s="0" t="s">
         <v>31</v>
@@ -21334,7 +21318,7 @@
         <v>171</v>
       </c>
       <c r="E519" s="0" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="F519" s="0" t="s">
         <v>894</v>
@@ -21343,16 +21327,16 @@
         <v>0</v>
       </c>
       <c r="H519" s="3" t="s">
-        <v>1395</v>
+        <v>1380</v>
       </c>
       <c r="I519" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="J519" s="0" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="K519" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21360,7 +21344,7 @@
         <v>890</v>
       </c>
       <c r="B520" s="0" t="s">
-        <v>1005</v>
+        <v>1395</v>
       </c>
       <c r="C520" s="0" t="s">
         <v>31</v>
@@ -21369,25 +21353,25 @@
         <v>171</v>
       </c>
       <c r="E520" s="0" t="s">
+        <v>1396</v>
+      </c>
+      <c r="F520" s="0" t="s">
+        <v>894</v>
+      </c>
+      <c r="G520" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H520" s="3" t="s">
         <v>1397</v>
-      </c>
-      <c r="F520" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G520" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H520" s="3" t="s">
-        <v>1374</v>
       </c>
       <c r="I520" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="J520" s="0" t="s">
-        <v>1008</v>
+        <v>1398</v>
       </c>
       <c r="K520" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21395,7 +21379,7 @@
         <v>890</v>
       </c>
       <c r="B521" s="0" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="C521" s="0" t="s">
         <v>31</v>
@@ -21404,25 +21388,25 @@
         <v>171</v>
       </c>
       <c r="E521" s="0" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="F521" s="0" t="s">
-        <v>31</v>
+        <v>894</v>
       </c>
       <c r="G521" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H521" s="3" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="I521" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="J521" s="0" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="K521" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21430,7 +21414,7 @@
         <v>890</v>
       </c>
       <c r="B522" s="0" t="s">
-        <v>1402</v>
+        <v>1005</v>
       </c>
       <c r="C522" s="0" t="s">
         <v>31</v>
@@ -21442,22 +21426,22 @@
         <v>1403</v>
       </c>
       <c r="F522" s="0" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G522" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H522" s="3" t="s">
-        <v>1400</v>
+        <v>1380</v>
       </c>
       <c r="I522" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="J522" s="0" t="s">
-        <v>1404</v>
+        <v>1008</v>
       </c>
       <c r="K522" s="0" t="s">
-        <v>1357</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21465,7 +21449,7 @@
         <v>890</v>
       </c>
       <c r="B523" s="0" t="s">
-        <v>260</v>
+        <v>1404</v>
       </c>
       <c r="C523" s="0" t="s">
         <v>31</v>
@@ -21474,29 +21458,97 @@
         <v>171</v>
       </c>
       <c r="E523" s="0" t="s">
-        <v>261</v>
+        <v>1405</v>
       </c>
       <c r="F523" s="0" t="s">
-        <v>262</v>
+        <v>31</v>
       </c>
       <c r="G523" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H523" s="3" t="s">
-        <v>1400</v>
+        <v>1406</v>
       </c>
       <c r="I523" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="J523" s="0" t="s">
+        <v>1407</v>
+      </c>
+      <c r="K523" s="0" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A524" s="0" t="s">
+        <v>890</v>
+      </c>
+      <c r="B524" s="0" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C524" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D524" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E524" s="0" t="s">
+        <v>1409</v>
+      </c>
+      <c r="F524" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G524" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H524" s="3" t="s">
+        <v>1406</v>
+      </c>
+      <c r="I524" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="J524" s="0" t="s">
+        <v>1410</v>
+      </c>
+      <c r="K524" s="0" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A525" s="0" t="s">
+        <v>890</v>
+      </c>
+      <c r="B525" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="C525" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D525" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E525" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="F525" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="G525" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H525" s="3" t="s">
+        <v>1406</v>
+      </c>
+      <c r="I525" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="J525" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="K523" s="0" t="s">
-        <v>1357</v>
-      </c>
-    </row>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="K525" s="0" t="s">
+        <v>1363</v>
+      </c>
+    </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add the block of CFsubhr variables (cl--fco2nat) to the list of ignored. Also add the manual instructon for this #374.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9747" uniqueCount="1533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10237" uniqueCount="1721">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -4619,6 +4619,570 @@
   </si>
   <si>
     <t xml:space="preserve">Temperature of upper boundary of the liquid ocean, including temperatures below sea-ice and floating ice shelves.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage Cloud Cover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 248.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage cloud cover, including both large-scale and convective cloud.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass Fraction of Cloud Liquid Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 246.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes both large-scale and convective cloud. Calculate as the mass of cloud liquid water in the grid cell divided by the mass of air (including the water in all phases) in the grid cells. Precipitating hydrometeors are included ONLY if the precipitating hydrometeors affect the calculation of radiative transfer in model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass Fraction of Cloud Ice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 247.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes both large-scale and convective cloud. This is calculated as the mass of cloud ice in the grid cell divided by the mass of air (including the water in all phases) in the grid cell. It includes precipitating hydrometeors ONLY if the precipitating hydrometeors affect the calculation of radiative transfer in model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 130.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastward Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 131.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zonal wind (positive in a eastward direction).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">va</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northward Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 132.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meridional wind (positive in a northward direction).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific Humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 133.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific humidity is the mass fraction of water vapor in (moist) air.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative Humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 157.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omega (=dp/dt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pa s-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 135.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omega (vertical velocity in pressure coordinates, positive downwards)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geopotential Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 129.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geopotential is the sum of the specific gravitational potential energy relative to the geoid and the specific centripetal potential energy. Geopotential height is the geopotential divided by the standard acceleration due to gravity. It is numerically similar to the altitude (or geometric height) and not to the quantity with standard name height, which is relative to the surface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pfull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure at Model Full-Levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 54.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air pressure on model levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tm5 code name = phalf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site time1 height2m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Near-Surface Air Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 167.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">near-surface (usually, 2 meter) air temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 139.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature of the lower boundary of the atmosphere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sea Level Pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 151.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Air Pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tm5 code name = ps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surface pressure (not mean sea-level pressure), 2-D field to calculate the 3-D pressure field from hybrid coordinates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site time1 height10m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastward Near-Surface Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 165.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastward component of the near-surface (usually, 10 meters)  wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northward Near-Surface Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 166.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northward component of the near surface wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfcWind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Near-Surface Wind Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 214.128, expression = sqrt(sqr(var165)+sqr(var166))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">near-surface (usually, 10 meters) wind speed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Near-Surface Relative Humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 80.129, expression = 100.*exp(17.62*((var168-273.15)/(var168-30.03)-(var167-273.15)/(var167-30.03)))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">huss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Near-Surface Specific Humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 81.129, expression = 1./(1.+1.608*(var134*exp(-17.62*(var168-273.15)/(var168-30.03))/611.-1.))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Near-surface (usually, 2 meter) specific humidity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 228.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">includes both liquid and solid phases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prsn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snowfall Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 144.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At surface; includes precipitation of all forms of water in the solid phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convective Precipitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 143.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convective precipitation at surface; includes both liquid and solid phases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evspsbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaporation Including Sublimation and Transpiration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 182.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaporation at surface (also known as evapotranspiration): flux of water into the atmosphere due to conversion of both liquid and solid phases to vapor (from underlying surface and vegetation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Snow and Ice Sublimation Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 44.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The snow and ice sublimation flux is the loss of snow and ice mass per unit area from the surface resulting from their direct conversion to water vapor that enters the atmosphere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tauu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Downward Eastward Wind Stress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 180.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downward eastward wind stress at the surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tauv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Downward Northward Wind Stress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 181.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downward northward wind stress at the surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Upward Latent Heat Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 147.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Upward Sensible Heat Flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 146.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The surface sensible heat flux, also called turbulent heat flux, is the exchange of heat between the surface and the air by motion of air.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rlds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Downwelling Longwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 175.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The surface called 'surface' means the lower boundary of the atmosphere. 'longwave' means longwave radiation. Downwelling radiation is radiation from above. It does not mean 'net downward'. When thought of as being incident on a surface, a radiative flux is sometimes called 'irradiance'. In addition, it is identical with the quantity measured by a cosine-collector light-meter and sometimes called 'vector irradiance'. In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rlus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Upwelling Longwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 96.129, expression = var177-var175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Downwelling Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 169.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface solar irradiance for UV calculations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Upwelling Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 95.129, expression = var176-var169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsdscs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Downwelling Clear-Sky Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 102.129, expression = var210-var176+var169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface solar irradiance clear sky for UV calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsuscs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Upwelling Clear-Sky Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Upwelling Clear-sky Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rldscs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Downwelling Clear-Sky Longwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 104.129, expression = var211-var177+var175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface downwelling clear-sky longwave radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsdt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOA Incident Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 212.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shortwave radiation incident at the top of the atmosphere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOA Outgoing Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 97.129, expression = var178-var212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at the top of the atmosphere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rlut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOA Outgoing Longwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 179.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at the top of the atmosphere (to be compared with satellite measurements)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rlutcs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOA Outgoing Clear-Sky Longwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 209.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upwelling clear-sky longwave radiation at top of atmosphere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsutcs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOA Outgoing Clear-Sky Shortwave Radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 103.129, expression = var208-var212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculated in the absence of clouds.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Vapor Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 137.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vertically integrated through the atmospheric column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Cloud Cover Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 164.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total cloud area fraction for the whole atmospheric column, as seen from the surface or the top of the atmosphere. Includes both large-scale and convective cloud.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clwvi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condensed Water Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 116.129, expression = var78+var79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass of condensed (liquid + ice) water in the column divided by the area of the column (not just the area of the cloudy portion of the column). Includes precipitating hydrometeors ONLY if the precipitating hydrometeors affect the calculation of radiative transfer in model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clivi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Water Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 79.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mass of ice water in the column divided by the area of the column (not just the area of the cloudy portion of the column). Includes precipitating frozen hydrometeors ONLY if the precipitating hydrometeor affects the calculation of radiative transfer in model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rtmt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Downward Radiative Flux at Top of Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ifs code name = 98.129, expression = var178+var179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Downward Radiative Flux at Top of Model : I.e., at the top of that portion of the atmosphere where dynamics are explicitly treated by the model. This is reported only if it differs from the net downward radiative flux at the top of the atmosphere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fco2antt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carbon Mass Flux into Atmosphere Due to All Anthropogenic Emissions of CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lpjg code name = fco2antt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is requested only for the emission-driven coupled carbon climate model runs.  Does not include natural fire sources but, includes all anthropogenic sources, including fossil fuel use, cement production, agricultural burning, and sources associated with anthropogenic land use change excluding forest regrowth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fco2nat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Carbon Mass Flux into the Atmosphere Due to Natural Sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lpjg code name = fco2nat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is what the atmosphere sees (on its own grid).  This field should be equivalent to the combined natural fluxes of carbon  that account for natural exchanges between the atmosphere and land (nep) or ocean (fgco2) reservoirs.</t>
   </si>
 </sst>
 </file>
@@ -4746,10 +5310,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1029"/>
+  <dimension ref="A1:K1080"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A997" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A967" activeCellId="0" sqref="967:1030"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1049" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1017" activeCellId="1" sqref="1031:1080 A1017"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4763,7 +5327,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -39868,6 +40432,1771 @@
     </row>
     <row r="1029" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1030" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1031" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1032" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1032" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1032" s="0" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C1032" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1032" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1032" s="0" t="s">
+        <v>1534</v>
+      </c>
+      <c r="F1032" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1032" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e0ecf1c1305c1bdc69bee0e7ba1e2e03.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1032" s="0" t="s">
+        <v>1535</v>
+      </c>
+      <c r="I1032" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1032" s="0" t="s">
+        <v>1536</v>
+      </c>
+      <c r="K1032" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1033" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1033" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1033" s="0" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C1033" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1033" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1033" s="0" t="s">
+        <v>1538</v>
+      </c>
+      <c r="F1033" s="0" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G1033" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b2b3318a73839edfafa9d46864aadc.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1033" s="0" t="s">
+        <v>1539</v>
+      </c>
+      <c r="I1033" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1033" s="0" t="s">
+        <v>1540</v>
+      </c>
+      <c r="K1033" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1034" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1034" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1034" s="0" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C1034" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1034" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1034" s="0" t="s">
+        <v>1542</v>
+      </c>
+      <c r="F1034" s="0" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G1034" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/dd916e3e2eca18cda5d9f81749d0c91c.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1034" s="0" t="s">
+        <v>1543</v>
+      </c>
+      <c r="I1034" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1034" s="0" t="s">
+        <v>1544</v>
+      </c>
+      <c r="K1034" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1035" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1035" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1035" s="0" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C1035" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1035" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1035" s="0" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F1035" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="G1035" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b9c3eb96337c69c1c4a5aab1317f5563.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1035" s="0" t="s">
+        <v>1547</v>
+      </c>
+      <c r="I1035" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1035" s="0" t="s">
+        <v>1546</v>
+      </c>
+      <c r="K1035" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1036" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1036" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1036" s="0" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C1036" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1036" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1036" s="0" t="s">
+        <v>1549</v>
+      </c>
+      <c r="F1036" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="G1036" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/21db90c0a12448299f855fdab60930d4.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1036" s="0" t="s">
+        <v>1550</v>
+      </c>
+      <c r="I1036" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1036" s="0" t="s">
+        <v>1551</v>
+      </c>
+      <c r="K1036" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1037" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1037" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1037" s="0" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C1037" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1037" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1037" s="0" t="s">
+        <v>1553</v>
+      </c>
+      <c r="F1037" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="G1037" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2dedcb347c18e132a2f4d625abf94585.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1037" s="0" t="s">
+        <v>1554</v>
+      </c>
+      <c r="I1037" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1037" s="0" t="s">
+        <v>1555</v>
+      </c>
+      <c r="K1037" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1038" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1038" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1038" s="0" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C1038" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1038" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1038" s="0" t="s">
+        <v>1557</v>
+      </c>
+      <c r="F1038" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1038" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53f4724d228998d54191c73352532ce3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1038" s="0" t="s">
+        <v>1558</v>
+      </c>
+      <c r="I1038" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1038" s="0" t="s">
+        <v>1559</v>
+      </c>
+      <c r="K1038" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1039" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1039" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1039" s="0" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C1039" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1039" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1039" s="0" t="s">
+        <v>1561</v>
+      </c>
+      <c r="F1039" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1039" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3cc6766c2d001a58d18dfe7f60fd5e66.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1039" s="0" t="s">
+        <v>1562</v>
+      </c>
+      <c r="I1039" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1039" s="0" t="s">
+        <v>999</v>
+      </c>
+      <c r="K1039" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1040" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1040" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1040" s="0" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C1040" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1040" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1040" s="0" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F1040" s="0" t="s">
+        <v>1565</v>
+      </c>
+      <c r="G1040" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51fb29dd55442361fa9c5dbe23aca9c6.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1040" s="0" t="s">
+        <v>1566</v>
+      </c>
+      <c r="I1040" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1040" s="0" t="s">
+        <v>1567</v>
+      </c>
+      <c r="K1040" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1041" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1041" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1041" s="0" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C1041" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1041" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1041" s="0" t="s">
+        <v>1569</v>
+      </c>
+      <c r="F1041" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1041" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/28e774ec0ecd561a6a3d437e6c443a6b.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1041" s="0" t="s">
+        <v>1570</v>
+      </c>
+      <c r="I1041" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1041" s="0" t="s">
+        <v>1571</v>
+      </c>
+      <c r="K1041" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1042" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1042" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1042" s="0" t="s">
+        <v>1572</v>
+      </c>
+      <c r="C1042" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1042" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1042" s="0" t="s">
+        <v>1573</v>
+      </c>
+      <c r="F1042" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G1042" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7a107875bd58c5e655e8f87152a3bad7.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1042" s="0" t="s">
+        <v>1574</v>
+      </c>
+      <c r="I1042" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1042" s="0" t="s">
+        <v>1575</v>
+      </c>
+      <c r="K1042" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1043" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1043" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1043" s="0" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C1043" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1043" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="E1043" s="0" t="s">
+        <v>1524</v>
+      </c>
+      <c r="F1043" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G1043" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154ab10964742eaff37de9cc5beef39c.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1043" s="0" t="s">
+        <v>1576</v>
+      </c>
+      <c r="I1043" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1043" s="0" t="s">
+        <v>1527</v>
+      </c>
+      <c r="K1043" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1044" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1044" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1044" s="0" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C1044" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1044" s="0" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E1044" s="0" t="s">
+        <v>1579</v>
+      </c>
+      <c r="F1044" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="G1044" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5c4978e802ba55d5a298cf1b3bdc2b3a.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1044" s="0" t="s">
+        <v>1580</v>
+      </c>
+      <c r="I1044" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1044" s="0" t="s">
+        <v>1581</v>
+      </c>
+      <c r="K1044" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1045" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1045" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1045" s="0" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C1045" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1045" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1045" s="0" t="s">
+        <v>1583</v>
+      </c>
+      <c r="F1045" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="G1045" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90c49fce92dc1f21647dad07d1342843.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1045" s="0" t="s">
+        <v>1584</v>
+      </c>
+      <c r="I1045" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1045" s="0" t="s">
+        <v>1585</v>
+      </c>
+      <c r="K1045" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1046" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1046" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1046" s="0" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C1046" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1046" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1046" s="0" t="s">
+        <v>1587</v>
+      </c>
+      <c r="F1046" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G1046" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3d23c359f44d6a153c4dcab9e07d7cb6.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1046" s="0" t="s">
+        <v>1588</v>
+      </c>
+      <c r="I1046" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1046" s="0" t="s">
+        <v>1587</v>
+      </c>
+      <c r="K1046" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1047" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1047" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1047" s="0" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C1047" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1047" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1047" s="0" t="s">
+        <v>1590</v>
+      </c>
+      <c r="F1047" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G1047" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8c9504d28596e05586c8e193082ac617.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1047" s="0" t="s">
+        <v>1591</v>
+      </c>
+      <c r="I1047" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1047" s="0" t="s">
+        <v>1592</v>
+      </c>
+      <c r="K1047" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1048" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1048" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1048" s="0" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C1048" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1048" s="0" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E1048" s="0" t="s">
+        <v>1595</v>
+      </c>
+      <c r="F1048" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="G1048" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e72b243a2a1c8691ab0168d8b62534c2.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1048" s="0" t="s">
+        <v>1596</v>
+      </c>
+      <c r="I1048" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1048" s="0" t="s">
+        <v>1597</v>
+      </c>
+      <c r="K1048" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1049" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1049" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1049" s="0" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C1049" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1049" s="0" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E1049" s="0" t="s">
+        <v>1599</v>
+      </c>
+      <c r="F1049" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="G1049" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b1cd51f370e346ecb20f1e80cb6ea4.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1049" s="0" t="s">
+        <v>1600</v>
+      </c>
+      <c r="I1049" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1049" s="0" t="s">
+        <v>1601</v>
+      </c>
+      <c r="K1049" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1050" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1050" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1050" s="0" t="s">
+        <v>1602</v>
+      </c>
+      <c r="C1050" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1050" s="0" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E1050" s="0" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F1050" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="G1050" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4b97609a32d53dff5b8e73729e4f258b.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1050" s="0" t="s">
+        <v>1604</v>
+      </c>
+      <c r="I1050" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1050" s="0" t="s">
+        <v>1605</v>
+      </c>
+      <c r="K1050" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1051" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1051" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1051" s="0" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C1051" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1051" s="0" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E1051" s="0" t="s">
+        <v>1607</v>
+      </c>
+      <c r="F1051" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1051" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c75f684ec69602e9de82b48e53afb2cc.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1051" s="0" t="s">
+        <v>1608</v>
+      </c>
+      <c r="I1051" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1051" s="0" t="s">
+        <v>999</v>
+      </c>
+      <c r="K1051" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1052" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1052" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1052" s="0" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C1052" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1052" s="0" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E1052" s="0" t="s">
+        <v>1610</v>
+      </c>
+      <c r="F1052" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1052" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ebfefc2ab8716ef597b128171b275945.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1052" s="0" t="s">
+        <v>1611</v>
+      </c>
+      <c r="I1052" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1052" s="0" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K1052" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1053" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1053" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1053" s="0" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C1053" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1053" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1053" s="0" t="s">
+        <v>1614</v>
+      </c>
+      <c r="F1053" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1053" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/62f26742cf240c1b5169a5cd511196b6.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1053" s="0" t="s">
+        <v>1615</v>
+      </c>
+      <c r="I1053" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1053" s="0" t="s">
+        <v>1616</v>
+      </c>
+      <c r="K1053" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1054" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1054" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1054" s="0" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C1054" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1054" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1054" s="0" t="s">
+        <v>1618</v>
+      </c>
+      <c r="F1054" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1054" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/051919eddec810e292c883205c944ceb.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1054" s="0" t="s">
+        <v>1619</v>
+      </c>
+      <c r="I1054" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1054" s="0" t="s">
+        <v>1620</v>
+      </c>
+      <c r="K1054" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1055" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1055" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1055" s="0" t="s">
+        <v>1621</v>
+      </c>
+      <c r="C1055" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1055" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1055" s="0" t="s">
+        <v>1622</v>
+      </c>
+      <c r="F1055" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1055" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/aa2bea81f238ad8f2c35a7e16ad97801.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1055" s="0" t="s">
+        <v>1623</v>
+      </c>
+      <c r="I1055" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1055" s="0" t="s">
+        <v>1624</v>
+      </c>
+      <c r="K1055" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1056" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1056" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1056" s="0" t="s">
+        <v>1625</v>
+      </c>
+      <c r="C1056" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1056" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1056" s="0" t="s">
+        <v>1626</v>
+      </c>
+      <c r="F1056" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1056" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/089961a3af4d54d5fb045cf3750e760c.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1056" s="0" t="s">
+        <v>1627</v>
+      </c>
+      <c r="I1056" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1056" s="0" t="s">
+        <v>1628</v>
+      </c>
+      <c r="K1056" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1057" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1057" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1057" s="0" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C1057" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1057" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1057" s="0" t="s">
+        <v>1630</v>
+      </c>
+      <c r="F1057" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1057" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3a8e1636a31c82fbdd9a1ae45ab3be7d.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1057" s="0" t="s">
+        <v>1631</v>
+      </c>
+      <c r="I1057" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1057" s="0" t="s">
+        <v>1632</v>
+      </c>
+      <c r="K1057" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1058" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1058" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1058" s="0" t="s">
+        <v>1633</v>
+      </c>
+      <c r="C1058" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1058" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1058" s="0" t="s">
+        <v>1634</v>
+      </c>
+      <c r="F1058" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G1058" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3abb7c5b4c4650e9d17a8439004aebea.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1058" s="0" t="s">
+        <v>1635</v>
+      </c>
+      <c r="I1058" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1058" s="0" t="s">
+        <v>1636</v>
+      </c>
+      <c r="K1058" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1059" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1059" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1059" s="0" t="s">
+        <v>1637</v>
+      </c>
+      <c r="C1059" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1059" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1059" s="0" t="s">
+        <v>1638</v>
+      </c>
+      <c r="F1059" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G1059" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bd10cebbde1593b65e5220911f9a997c.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1059" s="0" t="s">
+        <v>1639</v>
+      </c>
+      <c r="I1059" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1059" s="0" t="s">
+        <v>1640</v>
+      </c>
+      <c r="K1059" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1060" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1060" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1060" s="0" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C1060" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1060" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1060" s="0" t="s">
+        <v>1642</v>
+      </c>
+      <c r="F1060" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1060" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/95cbf6ac889c8fe7d92e20e8c34960d1.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1060" s="0" t="s">
+        <v>1643</v>
+      </c>
+      <c r="I1060" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1060" s="0" t="s">
+        <v>1220</v>
+      </c>
+      <c r="K1060" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1061" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1061" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1061" s="0" t="s">
+        <v>1644</v>
+      </c>
+      <c r="C1061" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1061" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1061" s="0" t="s">
+        <v>1645</v>
+      </c>
+      <c r="F1061" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1061" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a13ed886b17e20cdae8b89b9ff8e4610.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1061" s="0" t="s">
+        <v>1646</v>
+      </c>
+      <c r="I1061" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1061" s="0" t="s">
+        <v>1647</v>
+      </c>
+      <c r="K1061" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1062" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1062" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1062" s="0" t="s">
+        <v>1648</v>
+      </c>
+      <c r="C1062" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1062" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1062" s="0" t="s">
+        <v>1649</v>
+      </c>
+      <c r="F1062" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1062" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70d7d6fc0e9c2f14624a0270bf2b99b9.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1062" s="0" t="s">
+        <v>1650</v>
+      </c>
+      <c r="I1062" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1062" s="0" t="s">
+        <v>1651</v>
+      </c>
+      <c r="K1062" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1063" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1063" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1063" s="0" t="s">
+        <v>1652</v>
+      </c>
+      <c r="C1063" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1063" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1063" s="0" t="s">
+        <v>1653</v>
+      </c>
+      <c r="F1063" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1063" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/89027ee0079acb709750ddeac1c08899.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1063" s="0" t="s">
+        <v>1654</v>
+      </c>
+      <c r="I1063" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1063" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="K1063" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1064" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1064" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1064" s="0" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C1064" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1064" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1064" s="0" t="s">
+        <v>1656</v>
+      </c>
+      <c r="F1064" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1064" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e7b9f984d3bba15daccaaa18039a85d.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1064" s="0" t="s">
+        <v>1657</v>
+      </c>
+      <c r="I1064" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1064" s="0" t="s">
+        <v>1658</v>
+      </c>
+      <c r="K1064" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1065" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1065" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1065" s="0" t="s">
+        <v>1659</v>
+      </c>
+      <c r="C1065" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1065" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1065" s="0" t="s">
+        <v>1660</v>
+      </c>
+      <c r="F1065" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1065" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70bf79db957daa3b82413da949233ac7.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1065" s="0" t="s">
+        <v>1661</v>
+      </c>
+      <c r="I1065" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1065" s="0" t="s">
+        <v>1226</v>
+      </c>
+      <c r="K1065" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1066" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1066" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1066" s="0" t="s">
+        <v>1662</v>
+      </c>
+      <c r="C1066" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1066" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1066" s="0" t="s">
+        <v>1663</v>
+      </c>
+      <c r="F1066" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1066" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d0a35d5c99a0aa93ad4069cfe83bf748.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1066" s="0" t="s">
+        <v>1664</v>
+      </c>
+      <c r="I1066" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1066" s="0" t="s">
+        <v>1665</v>
+      </c>
+      <c r="K1066" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1067" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1067" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1067" s="0" t="s">
+        <v>1666</v>
+      </c>
+      <c r="C1067" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1067" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1067" s="0" t="s">
+        <v>1667</v>
+      </c>
+      <c r="F1067" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1067" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e2.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1067" s="0" t="s">
+        <v>1661</v>
+      </c>
+      <c r="I1067" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1067" s="0" t="s">
+        <v>1668</v>
+      </c>
+      <c r="K1067" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1068" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1068" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1068" s="0" t="s">
+        <v>1669</v>
+      </c>
+      <c r="C1068" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1068" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1068" s="0" t="s">
+        <v>1670</v>
+      </c>
+      <c r="F1068" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1068" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7b2d1e1a3ece1169d8ac61af4b758ed2.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1068" s="0" t="s">
+        <v>1671</v>
+      </c>
+      <c r="I1068" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1068" s="0" t="s">
+        <v>1672</v>
+      </c>
+      <c r="K1068" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1069" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1069" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1069" s="0" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C1069" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1069" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1069" s="0" t="s">
+        <v>1674</v>
+      </c>
+      <c r="F1069" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1069" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a21e250a10f96b1c1ad6d742206a157e.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1069" s="0" t="s">
+        <v>1675</v>
+      </c>
+      <c r="I1069" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1069" s="0" t="s">
+        <v>1676</v>
+      </c>
+      <c r="K1069" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1070" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1070" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1070" s="0" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C1070" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1070" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1070" s="0" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F1070" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1070" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b907fef85d4c9571a9457ee1b259bb8f.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1070" s="0" t="s">
+        <v>1679</v>
+      </c>
+      <c r="I1070" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1070" s="0" t="s">
+        <v>1680</v>
+      </c>
+      <c r="K1070" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1071" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1071" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1071" s="0" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C1071" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1071" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1071" s="0" t="s">
+        <v>1682</v>
+      </c>
+      <c r="F1071" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1071" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/63345d9732c72b97ca395f24ce2d6642.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1071" s="0" t="s">
+        <v>1683</v>
+      </c>
+      <c r="I1071" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1071" s="0" t="s">
+        <v>1684</v>
+      </c>
+      <c r="K1071" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1072" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1072" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1072" s="0" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C1072" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1072" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1072" s="0" t="s">
+        <v>1686</v>
+      </c>
+      <c r="F1072" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1072" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/921b8b8f6620826567d9324314c70410.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1072" s="0" t="s">
+        <v>1687</v>
+      </c>
+      <c r="I1072" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1072" s="0" t="s">
+        <v>1688</v>
+      </c>
+      <c r="K1072" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1073" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1073" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1073" s="0" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C1073" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1073" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1073" s="0" t="s">
+        <v>1690</v>
+      </c>
+      <c r="F1073" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1073" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/12e0369ff0ba1a6f1a84e0d9565d4b07.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1073" s="0" t="s">
+        <v>1691</v>
+      </c>
+      <c r="I1073" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1073" s="0" t="s">
+        <v>1692</v>
+      </c>
+      <c r="K1073" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1074" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1074" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1074" s="0" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C1074" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1074" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1074" s="0" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F1074" s="0" t="s">
+        <v>965</v>
+      </c>
+      <c r="G1074" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fc637f1c75e58be8a6e4112411a00f36.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1074" s="0" t="s">
+        <v>1695</v>
+      </c>
+      <c r="I1074" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1074" s="0" t="s">
+        <v>1696</v>
+      </c>
+      <c r="K1074" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1075" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1075" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1075" s="0" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C1075" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1075" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1075" s="0" t="s">
+        <v>1698</v>
+      </c>
+      <c r="F1075" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1075" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7c2249d424dde72f8616d42870a9d425.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1075" s="0" t="s">
+        <v>1699</v>
+      </c>
+      <c r="I1075" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1075" s="0" t="s">
+        <v>1700</v>
+      </c>
+      <c r="K1075" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1076" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1076" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1076" s="0" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C1076" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1076" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1076" s="0" t="s">
+        <v>1702</v>
+      </c>
+      <c r="F1076" s="0" t="s">
+        <v>965</v>
+      </c>
+      <c r="G1076" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/80a1dd605b563e9f09c718a5ba9cb9cc.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1076" s="0" t="s">
+        <v>1703</v>
+      </c>
+      <c r="I1076" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1076" s="0" t="s">
+        <v>1704</v>
+      </c>
+      <c r="K1076" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1077" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1077" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1077" s="0" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C1077" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1077" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1077" s="0" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F1077" s="0" t="s">
+        <v>965</v>
+      </c>
+      <c r="G1077" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/73c496f5669cc122cf1cddfe4df2a27a.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1077" s="0" t="s">
+        <v>1707</v>
+      </c>
+      <c r="I1077" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1077" s="0" t="s">
+        <v>1708</v>
+      </c>
+      <c r="K1077" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1078" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1078" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1078" s="0" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C1078" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1078" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1078" s="0" t="s">
+        <v>1710</v>
+      </c>
+      <c r="F1078" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1078" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/26328c46dfcc65d454b6fd4c52ccb48f.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1078" s="0" t="s">
+        <v>1711</v>
+      </c>
+      <c r="I1078" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1078" s="0" t="s">
+        <v>1712</v>
+      </c>
+      <c r="K1078" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1079" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1079" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1079" s="0" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C1079" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1079" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1079" s="0" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F1079" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1079" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc1b9e3073d751143fe8ab63ca9fcc45.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1079" s="0" t="s">
+        <v>1715</v>
+      </c>
+      <c r="I1079" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1079" s="0" t="s">
+        <v>1716</v>
+      </c>
+      <c r="K1079" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1080" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1080" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1080" s="0" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C1080" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1080" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1080" s="0" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F1080" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1080" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/299fb9d19040c4aa3862644286261ad2.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1080" s="0" t="s">
+        <v>1719</v>
+      </c>
+      <c r="I1080" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1080" s="0" t="s">
+        <v>1720</v>
+      </c>
+      <c r="K1080" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Revert "Add the block of CFsubhr variables (cl--fco2nat) to the list of ignored. Also add the manual instructon for this #374."
This reverts commit 6f0dd646e56ec758f81ba8e30a68b9eb3d268d50.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10237" uniqueCount="1721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9747" uniqueCount="1533">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -4619,570 +4619,6 @@
   </si>
   <si>
     <t xml:space="preserve">Temperature of upper boundary of the liquid ocean, including temperatures below sea-ice and floating ice shelves.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage Cloud Cover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 248.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage cloud cover, including both large-scale and convective cloud.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Fraction of Cloud Liquid Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 246.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Includes both large-scale and convective cloud. Calculate as the mass of cloud liquid water in the grid cell divided by the mass of air (including the water in all phases) in the grid cells. Precipitating hydrometeors are included ONLY if the precipitating hydrometeors affect the calculation of radiative transfer in model.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Fraction of Cloud Ice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 247.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Includes both large-scale and convective cloud. This is calculated as the mass of cloud ice in the grid cell divided by the mass of air (including the water in all phases) in the grid cell. It includes precipitating hydrometeors ONLY if the precipitating hydrometeors affect the calculation of radiative transfer in model.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 130.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastward Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 131.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zonal wind (positive in a eastward direction).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">va</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northward Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 132.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meridional wind (positive in a northward direction).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specific Humidity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 133.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specific humidity is the mass fraction of water vapor in (moist) air.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relative Humidity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 157.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omega (=dp/dt)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pa s-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 135.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omega (vertical velocity in pressure coordinates, positive downwards)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geopotential Height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 129.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geopotential is the sum of the specific gravitational potential energy relative to the geoid and the specific centripetal potential energy. Geopotential height is the geopotential divided by the standard acceleration due to gravity. It is numerically similar to the altitude (or geometric height) and not to the quantity with standard name height, which is relative to the surface.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pfull</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressure at Model Full-Levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 54.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air pressure on model levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tm5 code name = phalf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site time1 height2m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near-Surface Air Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 167.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">near-surface (usually, 2 meter) air temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 139.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature of the lower boundary of the atmosphere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">psl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sea Level Pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 151.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Air Pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tm5 code name = ps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">surface pressure (not mean sea-level pressure), 2-D field to calculate the 3-D pressure field from hybrid coordinates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">site time1 height10m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastward Near-Surface Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 165.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastward component of the near-surface (usually, 10 meters)  wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northward Near-Surface Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 166.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northward component of the near surface wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sfcWind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near-Surface Wind Speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 214.128, expression = sqrt(sqr(var165)+sqr(var166))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">near-surface (usually, 10 meters) wind speed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near-Surface Relative Humidity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 80.129, expression = 100.*exp(17.62*((var168-273.15)/(var168-30.03)-(var167-273.15)/(var167-30.03)))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">huss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near-Surface Specific Humidity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 81.129, expression = 1./(1.+1.608*(var134*exp(-17.62*(var168-273.15)/(var168-30.03))/611.-1.))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near-surface (usually, 2 meter) specific humidity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precipitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 228.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">includes both liquid and solid phases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prsn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snowfall Flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 144.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At surface; includes precipitation of all forms of water in the solid phase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convective Precipitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 143.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convective precipitation at surface; includes both liquid and solid phases.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">evspsbl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evaporation Including Sublimation and Transpiration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 182.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evaporation at surface (also known as evapotranspiration): flux of water into the atmosphere due to conversion of both liquid and solid phases to vapor (from underlying surface and vegetation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sbl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Snow and Ice Sublimation Flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 44.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The snow and ice sublimation flux is the loss of snow and ice mass per unit area from the surface resulting from their direct conversion to water vapor that enters the atmosphere.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tauu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Downward Eastward Wind Stress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 180.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Downward eastward wind stress at the surface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tauv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Downward Northward Wind Stress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 181.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Downward northward wind stress at the surface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hfls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Upward Latent Heat Flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 147.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hfss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Upward Sensible Heat Flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 146.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The surface sensible heat flux, also called turbulent heat flux, is the exchange of heat between the surface and the air by motion of air.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rlds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Downwelling Longwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 175.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The surface called 'surface' means the lower boundary of the atmosphere. 'longwave' means longwave radiation. Downwelling radiation is radiation from above. It does not mean 'net downward'. When thought of as being incident on a surface, a radiative flux is sometimes called 'irradiance'. In addition, it is identical with the quantity measured by a cosine-collector light-meter and sometimes called 'vector irradiance'. In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rlus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Upwelling Longwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 96.129, expression = var177-var175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Downwelling Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 169.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface solar irradiance for UV calculations.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Upwelling Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 95.129, expression = var176-var169</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsdscs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Downwelling Clear-Sky Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 102.129, expression = var210-var176+var169</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface solar irradiance clear sky for UV calculations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsuscs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Upwelling Clear-Sky Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Upwelling Clear-sky Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rldscs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Downwelling Clear-Sky Longwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 104.129, expression = var211-var177+var175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface downwelling clear-sky longwave radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsdt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOA Incident Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 212.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shortwave radiation incident at the top of the atmosphere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOA Outgoing Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 97.129, expression = var178-var212</t>
-  </si>
-  <si>
-    <t xml:space="preserve">at the top of the atmosphere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rlut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOA Outgoing Longwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 179.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">at the top of the atmosphere (to be compared with satellite measurements)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rlutcs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOA Outgoing Clear-Sky Longwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 209.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upwelling clear-sky longwave radiation at top of atmosphere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rsutcs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOA Outgoing Clear-Sky Shortwave Radiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 103.129, expression = var208-var212</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculated in the absence of clouds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Vapor Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 137.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vertically integrated through the atmospheric column</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Cloud Cover Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 164.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total cloud area fraction for the whole atmospheric column, as seen from the surface or the top of the atmosphere. Includes both large-scale and convective cloud.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clwvi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condensed Water Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 116.129, expression = var78+var79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass of condensed (liquid + ice) water in the column divided by the area of the column (not just the area of the cloudy portion of the column). Includes precipitating hydrometeors ONLY if the precipitating hydrometeors affect the calculation of radiative transfer in model.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clivi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ice Water Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 79.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mass of ice water in the column divided by the area of the column (not just the area of the cloudy portion of the column). Includes precipitating frozen hydrometeors ONLY if the precipitating hydrometeor affects the calculation of radiative transfer in model.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rtmt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Net Downward Radiative Flux at Top of Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifs code name = 98.129, expression = var178+var179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Net Downward Radiative Flux at Top of Model : I.e., at the top of that portion of the atmosphere where dynamics are explicitly treated by the model. This is reported only if it differs from the net downward radiative flux at the top of the atmosphere.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fco2antt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carbon Mass Flux into Atmosphere Due to All Anthropogenic Emissions of CO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lpjg code name = fco2antt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is requested only for the emission-driven coupled carbon climate model runs.  Does not include natural fire sources but, includes all anthropogenic sources, including fossil fuel use, cement production, agricultural burning, and sources associated with anthropogenic land use change excluding forest regrowth.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fco2nat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surface Carbon Mass Flux into the Atmosphere Due to Natural Sources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lpjg code name = fco2nat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is what the atmosphere sees (on its own grid).  This field should be equivalent to the combined natural fluxes of carbon  that account for natural exchanges between the atmosphere and land (nep) or ocean (fgco2) reservoirs.</t>
   </si>
 </sst>
 </file>
@@ -5310,10 +4746,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1080"/>
+  <dimension ref="A1:K1029"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1049" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1017" activeCellId="1" sqref="1031:1080 A1017"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A997" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A967" activeCellId="0" sqref="967:1030"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5327,7 +4763,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="200.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
@@ -40432,1771 +39868,6 @@
     </row>
     <row r="1029" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1030" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1031" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1032" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1032" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1032" s="0" t="s">
-        <v>1533</v>
-      </c>
-      <c r="C1032" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1032" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1032" s="0" t="s">
-        <v>1534</v>
-      </c>
-      <c r="F1032" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1032" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e0ecf1c1305c1bdc69bee0e7ba1e2e03.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1032" s="0" t="s">
-        <v>1535</v>
-      </c>
-      <c r="I1032" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1032" s="0" t="s">
-        <v>1536</v>
-      </c>
-      <c r="K1032" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1033" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1033" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1033" s="0" t="s">
-        <v>1537</v>
-      </c>
-      <c r="C1033" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1033" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1033" s="0" t="s">
-        <v>1538</v>
-      </c>
-      <c r="F1033" s="0" t="s">
-        <v>1036</v>
-      </c>
-      <c r="G1033" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b2b3318a73839edfafa9d46864aadc.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1033" s="0" t="s">
-        <v>1539</v>
-      </c>
-      <c r="I1033" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1033" s="0" t="s">
-        <v>1540</v>
-      </c>
-      <c r="K1033" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1034" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1034" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1034" s="0" t="s">
-        <v>1541</v>
-      </c>
-      <c r="C1034" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1034" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1034" s="0" t="s">
-        <v>1542</v>
-      </c>
-      <c r="F1034" s="0" t="s">
-        <v>1036</v>
-      </c>
-      <c r="G1034" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/dd916e3e2eca18cda5d9f81749d0c91c.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1034" s="0" t="s">
-        <v>1543</v>
-      </c>
-      <c r="I1034" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1034" s="0" t="s">
-        <v>1544</v>
-      </c>
-      <c r="K1034" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1035" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1035" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1035" s="0" t="s">
-        <v>1545</v>
-      </c>
-      <c r="C1035" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1035" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1035" s="0" t="s">
-        <v>1546</v>
-      </c>
-      <c r="F1035" s="0" t="s">
-        <v>838</v>
-      </c>
-      <c r="G1035" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b9c3eb96337c69c1c4a5aab1317f5563.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1035" s="0" t="s">
-        <v>1547</v>
-      </c>
-      <c r="I1035" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1035" s="0" t="s">
-        <v>1546</v>
-      </c>
-      <c r="K1035" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1036" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1036" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1036" s="0" t="s">
-        <v>1548</v>
-      </c>
-      <c r="C1036" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1036" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1036" s="0" t="s">
-        <v>1549</v>
-      </c>
-      <c r="F1036" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="G1036" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/21db90c0a12448299f855fdab60930d4.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1036" s="0" t="s">
-        <v>1550</v>
-      </c>
-      <c r="I1036" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1036" s="0" t="s">
-        <v>1551</v>
-      </c>
-      <c r="K1036" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1037" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1037" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1037" s="0" t="s">
-        <v>1552</v>
-      </c>
-      <c r="C1037" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1037" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1037" s="0" t="s">
-        <v>1553</v>
-      </c>
-      <c r="F1037" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="G1037" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2dedcb347c18e132a2f4d625abf94585.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1037" s="0" t="s">
-        <v>1554</v>
-      </c>
-      <c r="I1037" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1037" s="0" t="s">
-        <v>1555</v>
-      </c>
-      <c r="K1037" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1038" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1038" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1038" s="0" t="s">
-        <v>1556</v>
-      </c>
-      <c r="C1038" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1038" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1038" s="0" t="s">
-        <v>1557</v>
-      </c>
-      <c r="F1038" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1038" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53f4724d228998d54191c73352532ce3.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1038" s="0" t="s">
-        <v>1558</v>
-      </c>
-      <c r="I1038" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1038" s="0" t="s">
-        <v>1559</v>
-      </c>
-      <c r="K1038" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1039" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1039" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1039" s="0" t="s">
-        <v>1560</v>
-      </c>
-      <c r="C1039" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1039" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1039" s="0" t="s">
-        <v>1561</v>
-      </c>
-      <c r="F1039" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1039" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3cc6766c2d001a58d18dfe7f60fd5e66.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1039" s="0" t="s">
-        <v>1562</v>
-      </c>
-      <c r="I1039" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1039" s="0" t="s">
-        <v>999</v>
-      </c>
-      <c r="K1039" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1040" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1040" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1040" s="0" t="s">
-        <v>1563</v>
-      </c>
-      <c r="C1040" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1040" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1040" s="0" t="s">
-        <v>1564</v>
-      </c>
-      <c r="F1040" s="0" t="s">
-        <v>1565</v>
-      </c>
-      <c r="G1040" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51fb29dd55442361fa9c5dbe23aca9c6.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1040" s="0" t="s">
-        <v>1566</v>
-      </c>
-      <c r="I1040" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1040" s="0" t="s">
-        <v>1567</v>
-      </c>
-      <c r="K1040" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1041" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1041" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1041" s="0" t="s">
-        <v>1568</v>
-      </c>
-      <c r="C1041" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1041" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1041" s="0" t="s">
-        <v>1569</v>
-      </c>
-      <c r="F1041" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1041" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/28e774ec0ecd561a6a3d437e6c443a6b.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1041" s="0" t="s">
-        <v>1570</v>
-      </c>
-      <c r="I1041" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1041" s="0" t="s">
-        <v>1571</v>
-      </c>
-      <c r="K1041" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1042" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1042" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1042" s="0" t="s">
-        <v>1572</v>
-      </c>
-      <c r="C1042" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1042" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1042" s="0" t="s">
-        <v>1573</v>
-      </c>
-      <c r="F1042" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="G1042" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7a107875bd58c5e655e8f87152a3bad7.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1042" s="0" t="s">
-        <v>1574</v>
-      </c>
-      <c r="I1042" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1042" s="0" t="s">
-        <v>1575</v>
-      </c>
-      <c r="K1042" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1043" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1043" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1043" s="0" t="s">
-        <v>1522</v>
-      </c>
-      <c r="C1043" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1043" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="E1043" s="0" t="s">
-        <v>1524</v>
-      </c>
-      <c r="F1043" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="G1043" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154ab10964742eaff37de9cc5beef39c.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1043" s="0" t="s">
-        <v>1576</v>
-      </c>
-      <c r="I1043" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1043" s="0" t="s">
-        <v>1527</v>
-      </c>
-      <c r="K1043" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1044" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1044" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1044" s="0" t="s">
-        <v>1577</v>
-      </c>
-      <c r="C1044" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1044" s="0" t="s">
-        <v>1578</v>
-      </c>
-      <c r="E1044" s="0" t="s">
-        <v>1579</v>
-      </c>
-      <c r="F1044" s="0" t="s">
-        <v>838</v>
-      </c>
-      <c r="G1044" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5c4978e802ba55d5a298cf1b3bdc2b3a.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1044" s="0" t="s">
-        <v>1580</v>
-      </c>
-      <c r="I1044" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1044" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="K1044" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1045" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1045" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1045" s="0" t="s">
-        <v>1582</v>
-      </c>
-      <c r="C1045" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1045" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1045" s="0" t="s">
-        <v>1583</v>
-      </c>
-      <c r="F1045" s="0" t="s">
-        <v>838</v>
-      </c>
-      <c r="G1045" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90c49fce92dc1f21647dad07d1342843.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1045" s="0" t="s">
-        <v>1584</v>
-      </c>
-      <c r="I1045" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1045" s="0" t="s">
-        <v>1585</v>
-      </c>
-      <c r="K1045" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1046" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1046" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1046" s="0" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C1046" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1046" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1046" s="0" t="s">
-        <v>1587</v>
-      </c>
-      <c r="F1046" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="G1046" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3d23c359f44d6a153c4dcab9e07d7cb6.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1046" s="0" t="s">
-        <v>1588</v>
-      </c>
-      <c r="I1046" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1046" s="0" t="s">
-        <v>1587</v>
-      </c>
-      <c r="K1046" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1047" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1047" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1047" s="0" t="s">
-        <v>1589</v>
-      </c>
-      <c r="C1047" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1047" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1047" s="0" t="s">
-        <v>1590</v>
-      </c>
-      <c r="F1047" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="G1047" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8c9504d28596e05586c8e193082ac617.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1047" s="0" t="s">
-        <v>1591</v>
-      </c>
-      <c r="I1047" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1047" s="0" t="s">
-        <v>1592</v>
-      </c>
-      <c r="K1047" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1048" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1048" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1048" s="0" t="s">
-        <v>1593</v>
-      </c>
-      <c r="C1048" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1048" s="0" t="s">
-        <v>1594</v>
-      </c>
-      <c r="E1048" s="0" t="s">
-        <v>1595</v>
-      </c>
-      <c r="F1048" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="G1048" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e72b243a2a1c8691ab0168d8b62534c2.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1048" s="0" t="s">
-        <v>1596</v>
-      </c>
-      <c r="I1048" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1048" s="0" t="s">
-        <v>1597</v>
-      </c>
-      <c r="K1048" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1049" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1049" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1049" s="0" t="s">
-        <v>1598</v>
-      </c>
-      <c r="C1049" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1049" s="0" t="s">
-        <v>1594</v>
-      </c>
-      <c r="E1049" s="0" t="s">
-        <v>1599</v>
-      </c>
-      <c r="F1049" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="G1049" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b1cd51f370e346ecb20f1e80cb6ea4.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1049" s="0" t="s">
-        <v>1600</v>
-      </c>
-      <c r="I1049" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1049" s="0" t="s">
-        <v>1601</v>
-      </c>
-      <c r="K1049" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1050" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1050" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1050" s="0" t="s">
-        <v>1602</v>
-      </c>
-      <c r="C1050" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1050" s="0" t="s">
-        <v>1594</v>
-      </c>
-      <c r="E1050" s="0" t="s">
-        <v>1603</v>
-      </c>
-      <c r="F1050" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="G1050" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4b97609a32d53dff5b8e73729e4f258b.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1050" s="0" t="s">
-        <v>1604</v>
-      </c>
-      <c r="I1050" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1050" s="0" t="s">
-        <v>1605</v>
-      </c>
-      <c r="K1050" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1051" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1051" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1051" s="0" t="s">
-        <v>1606</v>
-      </c>
-      <c r="C1051" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1051" s="0" t="s">
-        <v>1578</v>
-      </c>
-      <c r="E1051" s="0" t="s">
-        <v>1607</v>
-      </c>
-      <c r="F1051" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1051" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c75f684ec69602e9de82b48e53afb2cc.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1051" s="0" t="s">
-        <v>1608</v>
-      </c>
-      <c r="I1051" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1051" s="0" t="s">
-        <v>999</v>
-      </c>
-      <c r="K1051" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1052" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1052" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1052" s="0" t="s">
-        <v>1609</v>
-      </c>
-      <c r="C1052" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1052" s="0" t="s">
-        <v>1578</v>
-      </c>
-      <c r="E1052" s="0" t="s">
-        <v>1610</v>
-      </c>
-      <c r="F1052" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1052" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ebfefc2ab8716ef597b128171b275945.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1052" s="0" t="s">
-        <v>1611</v>
-      </c>
-      <c r="I1052" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1052" s="0" t="s">
-        <v>1612</v>
-      </c>
-      <c r="K1052" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1053" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1053" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1053" s="0" t="s">
-        <v>1613</v>
-      </c>
-      <c r="C1053" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1053" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1053" s="0" t="s">
-        <v>1614</v>
-      </c>
-      <c r="F1053" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1053" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/62f26742cf240c1b5169a5cd511196b6.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1053" s="0" t="s">
-        <v>1615</v>
-      </c>
-      <c r="I1053" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1053" s="0" t="s">
-        <v>1616</v>
-      </c>
-      <c r="K1053" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1054" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1054" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1054" s="0" t="s">
-        <v>1617</v>
-      </c>
-      <c r="C1054" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1054" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1054" s="0" t="s">
-        <v>1618</v>
-      </c>
-      <c r="F1054" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1054" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/051919eddec810e292c883205c944ceb.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1054" s="0" t="s">
-        <v>1619</v>
-      </c>
-      <c r="I1054" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1054" s="0" t="s">
-        <v>1620</v>
-      </c>
-      <c r="K1054" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1055" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1055" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1055" s="0" t="s">
-        <v>1621</v>
-      </c>
-      <c r="C1055" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1055" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1055" s="0" t="s">
-        <v>1622</v>
-      </c>
-      <c r="F1055" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1055" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/aa2bea81f238ad8f2c35a7e16ad97801.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1055" s="0" t="s">
-        <v>1623</v>
-      </c>
-      <c r="I1055" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1055" s="0" t="s">
-        <v>1624</v>
-      </c>
-      <c r="K1055" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1056" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1056" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1056" s="0" t="s">
-        <v>1625</v>
-      </c>
-      <c r="C1056" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1056" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1056" s="0" t="s">
-        <v>1626</v>
-      </c>
-      <c r="F1056" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1056" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/089961a3af4d54d5fb045cf3750e760c.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1056" s="0" t="s">
-        <v>1627</v>
-      </c>
-      <c r="I1056" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1056" s="0" t="s">
-        <v>1628</v>
-      </c>
-      <c r="K1056" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1057" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1057" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1057" s="0" t="s">
-        <v>1629</v>
-      </c>
-      <c r="C1057" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1057" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1057" s="0" t="s">
-        <v>1630</v>
-      </c>
-      <c r="F1057" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1057" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3a8e1636a31c82fbdd9a1ae45ab3be7d.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1057" s="0" t="s">
-        <v>1631</v>
-      </c>
-      <c r="I1057" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1057" s="0" t="s">
-        <v>1632</v>
-      </c>
-      <c r="K1057" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1058" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1058" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1058" s="0" t="s">
-        <v>1633</v>
-      </c>
-      <c r="C1058" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1058" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1058" s="0" t="s">
-        <v>1634</v>
-      </c>
-      <c r="F1058" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="G1058" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3abb7c5b4c4650e9d17a8439004aebea.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1058" s="0" t="s">
-        <v>1635</v>
-      </c>
-      <c r="I1058" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1058" s="0" t="s">
-        <v>1636</v>
-      </c>
-      <c r="K1058" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1059" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1059" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1059" s="0" t="s">
-        <v>1637</v>
-      </c>
-      <c r="C1059" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1059" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1059" s="0" t="s">
-        <v>1638</v>
-      </c>
-      <c r="F1059" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="G1059" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bd10cebbde1593b65e5220911f9a997c.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1059" s="0" t="s">
-        <v>1639</v>
-      </c>
-      <c r="I1059" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1059" s="0" t="s">
-        <v>1640</v>
-      </c>
-      <c r="K1059" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1060" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1060" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1060" s="0" t="s">
-        <v>1641</v>
-      </c>
-      <c r="C1060" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1060" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1060" s="0" t="s">
-        <v>1642</v>
-      </c>
-      <c r="F1060" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1060" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/95cbf6ac889c8fe7d92e20e8c34960d1.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1060" s="0" t="s">
-        <v>1643</v>
-      </c>
-      <c r="I1060" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1060" s="0" t="s">
-        <v>1220</v>
-      </c>
-      <c r="K1060" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1061" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1061" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1061" s="0" t="s">
-        <v>1644</v>
-      </c>
-      <c r="C1061" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1061" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1061" s="0" t="s">
-        <v>1645</v>
-      </c>
-      <c r="F1061" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1061" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a13ed886b17e20cdae8b89b9ff8e4610.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1061" s="0" t="s">
-        <v>1646</v>
-      </c>
-      <c r="I1061" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1061" s="0" t="s">
-        <v>1647</v>
-      </c>
-      <c r="K1061" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1062" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1062" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1062" s="0" t="s">
-        <v>1648</v>
-      </c>
-      <c r="C1062" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1062" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1062" s="0" t="s">
-        <v>1649</v>
-      </c>
-      <c r="F1062" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1062" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70d7d6fc0e9c2f14624a0270bf2b99b9.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1062" s="0" t="s">
-        <v>1650</v>
-      </c>
-      <c r="I1062" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1062" s="0" t="s">
-        <v>1651</v>
-      </c>
-      <c r="K1062" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1063" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1063" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1063" s="0" t="s">
-        <v>1652</v>
-      </c>
-      <c r="C1063" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1063" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1063" s="0" t="s">
-        <v>1653</v>
-      </c>
-      <c r="F1063" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1063" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/89027ee0079acb709750ddeac1c08899.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1063" s="0" t="s">
-        <v>1654</v>
-      </c>
-      <c r="I1063" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1063" s="0" t="s">
-        <v>1229</v>
-      </c>
-      <c r="K1063" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1064" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1064" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1064" s="0" t="s">
-        <v>1655</v>
-      </c>
-      <c r="C1064" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1064" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1064" s="0" t="s">
-        <v>1656</v>
-      </c>
-      <c r="F1064" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1064" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e7b9f984d3bba15daccaaa18039a85d.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1064" s="0" t="s">
-        <v>1657</v>
-      </c>
-      <c r="I1064" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1064" s="0" t="s">
-        <v>1658</v>
-      </c>
-      <c r="K1064" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1065" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1065" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1065" s="0" t="s">
-        <v>1659</v>
-      </c>
-      <c r="C1065" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1065" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1065" s="0" t="s">
-        <v>1660</v>
-      </c>
-      <c r="F1065" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1065" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70bf79db957daa3b82413da949233ac7.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1065" s="0" t="s">
-        <v>1661</v>
-      </c>
-      <c r="I1065" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1065" s="0" t="s">
-        <v>1226</v>
-      </c>
-      <c r="K1065" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1066" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1066" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1066" s="0" t="s">
-        <v>1662</v>
-      </c>
-      <c r="C1066" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1066" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1066" s="0" t="s">
-        <v>1663</v>
-      </c>
-      <c r="F1066" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1066" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d0a35d5c99a0aa93ad4069cfe83bf748.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1066" s="0" t="s">
-        <v>1664</v>
-      </c>
-      <c r="I1066" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1066" s="0" t="s">
-        <v>1665</v>
-      </c>
-      <c r="K1066" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1067" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1067" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1067" s="0" t="s">
-        <v>1666</v>
-      </c>
-      <c r="C1067" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1067" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1067" s="0" t="s">
-        <v>1667</v>
-      </c>
-      <c r="F1067" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1067" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e2.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1067" s="0" t="s">
-        <v>1661</v>
-      </c>
-      <c r="I1067" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1067" s="0" t="s">
-        <v>1668</v>
-      </c>
-      <c r="K1067" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1068" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1068" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1068" s="0" t="s">
-        <v>1669</v>
-      </c>
-      <c r="C1068" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1068" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1068" s="0" t="s">
-        <v>1670</v>
-      </c>
-      <c r="F1068" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1068" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7b2d1e1a3ece1169d8ac61af4b758ed2.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1068" s="0" t="s">
-        <v>1671</v>
-      </c>
-      <c r="I1068" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1068" s="0" t="s">
-        <v>1672</v>
-      </c>
-      <c r="K1068" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1069" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1069" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1069" s="0" t="s">
-        <v>1673</v>
-      </c>
-      <c r="C1069" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1069" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1069" s="0" t="s">
-        <v>1674</v>
-      </c>
-      <c r="F1069" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1069" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a21e250a10f96b1c1ad6d742206a157e.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1069" s="0" t="s">
-        <v>1675</v>
-      </c>
-      <c r="I1069" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1069" s="0" t="s">
-        <v>1676</v>
-      </c>
-      <c r="K1069" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1070" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1070" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1070" s="0" t="s">
-        <v>1677</v>
-      </c>
-      <c r="C1070" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1070" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1070" s="0" t="s">
-        <v>1678</v>
-      </c>
-      <c r="F1070" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1070" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b907fef85d4c9571a9457ee1b259bb8f.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1070" s="0" t="s">
-        <v>1679</v>
-      </c>
-      <c r="I1070" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1070" s="0" t="s">
-        <v>1680</v>
-      </c>
-      <c r="K1070" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1071" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1071" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1071" s="0" t="s">
-        <v>1681</v>
-      </c>
-      <c r="C1071" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1071" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1071" s="0" t="s">
-        <v>1682</v>
-      </c>
-      <c r="F1071" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1071" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/63345d9732c72b97ca395f24ce2d6642.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1071" s="0" t="s">
-        <v>1683</v>
-      </c>
-      <c r="I1071" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1071" s="0" t="s">
-        <v>1684</v>
-      </c>
-      <c r="K1071" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1072" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1072" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1072" s="0" t="s">
-        <v>1685</v>
-      </c>
-      <c r="C1072" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1072" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1072" s="0" t="s">
-        <v>1686</v>
-      </c>
-      <c r="F1072" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1072" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/921b8b8f6620826567d9324314c70410.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1072" s="0" t="s">
-        <v>1687</v>
-      </c>
-      <c r="I1072" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1072" s="0" t="s">
-        <v>1688</v>
-      </c>
-      <c r="K1072" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1073" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1073" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1073" s="0" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C1073" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1073" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1073" s="0" t="s">
-        <v>1690</v>
-      </c>
-      <c r="F1073" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1073" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/12e0369ff0ba1a6f1a84e0d9565d4b07.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1073" s="0" t="s">
-        <v>1691</v>
-      </c>
-      <c r="I1073" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1073" s="0" t="s">
-        <v>1692</v>
-      </c>
-      <c r="K1073" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1074" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1074" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1074" s="0" t="s">
-        <v>1693</v>
-      </c>
-      <c r="C1074" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1074" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1074" s="0" t="s">
-        <v>1694</v>
-      </c>
-      <c r="F1074" s="0" t="s">
-        <v>965</v>
-      </c>
-      <c r="G1074" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fc637f1c75e58be8a6e4112411a00f36.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1074" s="0" t="s">
-        <v>1695</v>
-      </c>
-      <c r="I1074" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1074" s="0" t="s">
-        <v>1696</v>
-      </c>
-      <c r="K1074" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1075" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1075" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1075" s="0" t="s">
-        <v>1697</v>
-      </c>
-      <c r="C1075" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1075" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1075" s="0" t="s">
-        <v>1698</v>
-      </c>
-      <c r="F1075" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1075" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7c2249d424dde72f8616d42870a9d425.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1075" s="0" t="s">
-        <v>1699</v>
-      </c>
-      <c r="I1075" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1075" s="0" t="s">
-        <v>1700</v>
-      </c>
-      <c r="K1075" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1076" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1076" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1076" s="0" t="s">
-        <v>1701</v>
-      </c>
-      <c r="C1076" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1076" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1076" s="0" t="s">
-        <v>1702</v>
-      </c>
-      <c r="F1076" s="0" t="s">
-        <v>965</v>
-      </c>
-      <c r="G1076" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/80a1dd605b563e9f09c718a5ba9cb9cc.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1076" s="0" t="s">
-        <v>1703</v>
-      </c>
-      <c r="I1076" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1076" s="0" t="s">
-        <v>1704</v>
-      </c>
-      <c r="K1076" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1077" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1077" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1077" s="0" t="s">
-        <v>1705</v>
-      </c>
-      <c r="C1077" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1077" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1077" s="0" t="s">
-        <v>1706</v>
-      </c>
-      <c r="F1077" s="0" t="s">
-        <v>965</v>
-      </c>
-      <c r="G1077" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/73c496f5669cc122cf1cddfe4df2a27a.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1077" s="0" t="s">
-        <v>1707</v>
-      </c>
-      <c r="I1077" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1077" s="0" t="s">
-        <v>1708</v>
-      </c>
-      <c r="K1077" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1078" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1078" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1078" s="0" t="s">
-        <v>1709</v>
-      </c>
-      <c r="C1078" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1078" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1078" s="0" t="s">
-        <v>1710</v>
-      </c>
-      <c r="F1078" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1078" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/26328c46dfcc65d454b6fd4c52ccb48f.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1078" s="0" t="s">
-        <v>1711</v>
-      </c>
-      <c r="I1078" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1078" s="0" t="s">
-        <v>1712</v>
-      </c>
-      <c r="K1078" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1079" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1079" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1079" s="0" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C1079" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1079" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1079" s="0" t="s">
-        <v>1714</v>
-      </c>
-      <c r="F1079" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1079" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc1b9e3073d751143fe8ab63ca9fcc45.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1079" s="0" t="s">
-        <v>1715</v>
-      </c>
-      <c r="I1079" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1079" s="0" t="s">
-        <v>1716</v>
-      </c>
-      <c r="K1079" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1080" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1080" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1080" s="0" t="s">
-        <v>1717</v>
-      </c>
-      <c r="C1080" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1080" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1080" s="0" t="s">
-        <v>1718</v>
-      </c>
-      <c r="F1080" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1080" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/299fb9d19040c4aa3862644286261ad2.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1080" s="0" t="s">
-        <v>1719</v>
-      </c>
-      <c r="I1080" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1080" s="0" t="s">
-        <v>1720</v>
-      </c>
-      <c r="K1080" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Correcting the current changes which cause the ignoring of 3hr tos in all cases #393, the 3hr tos for the AMIP run #389 should become part of the preferences file.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10237" uniqueCount="1721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10227" uniqueCount="1716">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -4604,21 +4604,6 @@
   </si>
   <si>
     <t xml:space="preserve">Air pressure on model half-levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sea Surface Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">degC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The 3hr tos for an AMIP run needs to be taken from NEMO. The confusing thing here is that the request asks for tos from the ocean grid cell. Therefore ignore this variable for this table for AMIP? #389</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature of upper boundary of the liquid ocean, including temperatures below sea-ice and floating ice shelves.</t>
   </si>
   <si>
     <t xml:space="preserve">cl</t>
@@ -5310,10 +5295,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1080"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1049" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1017" activeCellId="1" sqref="1031:1080 A1017"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A269" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B284" activeCellId="0" sqref="B284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -40394,51 +40379,86 @@
       </c>
     </row>
     <row r="1027" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1028" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1028" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="B1028" s="3" t="s">
+    <row r="1028" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1029" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1030" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1030" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1030" s="0" t="s">
         <v>1528</v>
       </c>
-      <c r="C1028" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1028" s="3" t="s">
-        <v>873</v>
-      </c>
-      <c r="E1028" s="3" t="s">
+      <c r="C1030" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1030" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1030" s="0" t="s">
         <v>1529</v>
       </c>
-      <c r="F1028" s="3" t="s">
+      <c r="F1030" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1030" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e0ecf1c1305c1bdc69bee0e7ba1e2e03.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1030" s="0" t="s">
         <v>1530</v>
       </c>
-      <c r="G1028" s="3" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/0e5d376315a376cd2b1e37f440fe43d3.html","web")</f>
+      <c r="I1030" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J1030" s="0" t="s">
+        <v>1531</v>
+      </c>
+      <c r="K1030" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1031" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1031" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1031" s="0" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C1031" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1031" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1031" s="0" t="s">
+        <v>1533</v>
+      </c>
+      <c r="F1031" s="0" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G1031" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b2b3318a73839edfafa9d46864aadc.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1028" s="3" t="s">
-        <v>1531</v>
-      </c>
-      <c r="I1028" s="3" t="s">
+      <c r="H1031" s="0" t="s">
+        <v>1534</v>
+      </c>
+      <c r="I1031" s="0" t="s">
         <v>1526</v>
       </c>
-      <c r="J1028" s="3" t="s">
-        <v>1532</v>
-      </c>
-      <c r="K1028" s="3" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="1029" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1030" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1031" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="J1031" s="0" t="s">
+        <v>1535</v>
+      </c>
+      <c r="K1031" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
     <row r="1032" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1032" s="0" t="s">
         <v>303</v>
       </c>
       <c r="B1032" s="0" t="s">
-        <v>1533</v>
+        <v>1536</v>
       </c>
       <c r="C1032" s="0" t="s">
         <v>31</v>
@@ -40447,23 +40467,23 @@
         <v>334</v>
       </c>
       <c r="E1032" s="0" t="s">
-        <v>1534</v>
+        <v>1537</v>
       </c>
       <c r="F1032" s="0" t="s">
-        <v>24</v>
+        <v>1036</v>
       </c>
       <c r="G1032" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e0ecf1c1305c1bdc69bee0e7ba1e2e03.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/dd916e3e2eca18cda5d9f81749d0c91c.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1032" s="0" t="s">
-        <v>1535</v>
+        <v>1538</v>
       </c>
       <c r="I1032" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1032" s="0" t="s">
-        <v>1536</v>
+        <v>1539</v>
       </c>
       <c r="K1032" s="0" t="s">
         <v>305</v>
@@ -40474,7 +40494,7 @@
         <v>303</v>
       </c>
       <c r="B1033" s="0" t="s">
-        <v>1537</v>
+        <v>1540</v>
       </c>
       <c r="C1033" s="0" t="s">
         <v>31</v>
@@ -40483,23 +40503,23 @@
         <v>334</v>
       </c>
       <c r="E1033" s="0" t="s">
-        <v>1538</v>
+        <v>1541</v>
       </c>
       <c r="F1033" s="0" t="s">
-        <v>1036</v>
+        <v>838</v>
       </c>
       <c r="G1033" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b2b3318a73839edfafa9d46864aadc.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b9c3eb96337c69c1c4a5aab1317f5563.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1033" s="0" t="s">
-        <v>1539</v>
+        <v>1542</v>
       </c>
       <c r="I1033" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1033" s="0" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="K1033" s="0" t="s">
         <v>305</v>
@@ -40510,7 +40530,7 @@
         <v>303</v>
       </c>
       <c r="B1034" s="0" t="s">
-        <v>1541</v>
+        <v>1543</v>
       </c>
       <c r="C1034" s="0" t="s">
         <v>31</v>
@@ -40519,23 +40539,23 @@
         <v>334</v>
       </c>
       <c r="E1034" s="0" t="s">
-        <v>1542</v>
+        <v>1544</v>
       </c>
       <c r="F1034" s="0" t="s">
-        <v>1036</v>
+        <v>252</v>
       </c>
       <c r="G1034" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/dd916e3e2eca18cda5d9f81749d0c91c.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/21db90c0a12448299f855fdab60930d4.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1034" s="0" t="s">
-        <v>1543</v>
+        <v>1545</v>
       </c>
       <c r="I1034" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1034" s="0" t="s">
-        <v>1544</v>
+        <v>1546</v>
       </c>
       <c r="K1034" s="0" t="s">
         <v>305</v>
@@ -40546,7 +40566,7 @@
         <v>303</v>
       </c>
       <c r="B1035" s="0" t="s">
-        <v>1545</v>
+        <v>1547</v>
       </c>
       <c r="C1035" s="0" t="s">
         <v>31</v>
@@ -40555,23 +40575,23 @@
         <v>334</v>
       </c>
       <c r="E1035" s="0" t="s">
-        <v>1546</v>
+        <v>1548</v>
       </c>
       <c r="F1035" s="0" t="s">
-        <v>838</v>
+        <v>252</v>
       </c>
       <c r="G1035" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b9c3eb96337c69c1c4a5aab1317f5563.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2dedcb347c18e132a2f4d625abf94585.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1035" s="0" t="s">
-        <v>1547</v>
+        <v>1549</v>
       </c>
       <c r="I1035" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1035" s="0" t="s">
-        <v>1546</v>
+        <v>1550</v>
       </c>
       <c r="K1035" s="0" t="s">
         <v>305</v>
@@ -40582,7 +40602,7 @@
         <v>303</v>
       </c>
       <c r="B1036" s="0" t="s">
-        <v>1548</v>
+        <v>1551</v>
       </c>
       <c r="C1036" s="0" t="s">
         <v>31</v>
@@ -40591,23 +40611,23 @@
         <v>334</v>
       </c>
       <c r="E1036" s="0" t="s">
-        <v>1549</v>
+        <v>1552</v>
       </c>
       <c r="F1036" s="0" t="s">
-        <v>252</v>
+        <v>31</v>
       </c>
       <c r="G1036" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/21db90c0a12448299f855fdab60930d4.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53f4724d228998d54191c73352532ce3.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1036" s="0" t="s">
-        <v>1550</v>
+        <v>1553</v>
       </c>
       <c r="I1036" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1036" s="0" t="s">
-        <v>1551</v>
+        <v>1554</v>
       </c>
       <c r="K1036" s="0" t="s">
         <v>305</v>
@@ -40618,7 +40638,7 @@
         <v>303</v>
       </c>
       <c r="B1037" s="0" t="s">
-        <v>1552</v>
+        <v>1555</v>
       </c>
       <c r="C1037" s="0" t="s">
         <v>31</v>
@@ -40627,23 +40647,23 @@
         <v>334</v>
       </c>
       <c r="E1037" s="0" t="s">
-        <v>1553</v>
+        <v>1556</v>
       </c>
       <c r="F1037" s="0" t="s">
-        <v>252</v>
+        <v>24</v>
       </c>
       <c r="G1037" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2dedcb347c18e132a2f4d625abf94585.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3cc6766c2d001a58d18dfe7f60fd5e66.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1037" s="0" t="s">
-        <v>1554</v>
+        <v>1557</v>
       </c>
       <c r="I1037" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1037" s="0" t="s">
-        <v>1555</v>
+        <v>999</v>
       </c>
       <c r="K1037" s="0" t="s">
         <v>305</v>
@@ -40654,7 +40674,7 @@
         <v>303</v>
       </c>
       <c r="B1038" s="0" t="s">
-        <v>1556</v>
+        <v>1558</v>
       </c>
       <c r="C1038" s="0" t="s">
         <v>31</v>
@@ -40663,23 +40683,23 @@
         <v>334</v>
       </c>
       <c r="E1038" s="0" t="s">
-        <v>1557</v>
+        <v>1559</v>
       </c>
       <c r="F1038" s="0" t="s">
-        <v>31</v>
+        <v>1560</v>
       </c>
       <c r="G1038" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53f4724d228998d54191c73352532ce3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51fb29dd55442361fa9c5dbe23aca9c6.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1038" s="0" t="s">
-        <v>1558</v>
+        <v>1561</v>
       </c>
       <c r="I1038" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1038" s="0" t="s">
-        <v>1559</v>
+        <v>1562</v>
       </c>
       <c r="K1038" s="0" t="s">
         <v>305</v>
@@ -40690,7 +40710,7 @@
         <v>303</v>
       </c>
       <c r="B1039" s="0" t="s">
-        <v>1560</v>
+        <v>1563</v>
       </c>
       <c r="C1039" s="0" t="s">
         <v>31</v>
@@ -40699,23 +40719,23 @@
         <v>334</v>
       </c>
       <c r="E1039" s="0" t="s">
-        <v>1561</v>
+        <v>1564</v>
       </c>
       <c r="F1039" s="0" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G1039" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3cc6766c2d001a58d18dfe7f60fd5e66.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/28e774ec0ecd561a6a3d437e6c443a6b.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1039" s="0" t="s">
-        <v>1562</v>
+        <v>1565</v>
       </c>
       <c r="I1039" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1039" s="0" t="s">
-        <v>999</v>
+        <v>1566</v>
       </c>
       <c r="K1039" s="0" t="s">
         <v>305</v>
@@ -40726,7 +40746,7 @@
         <v>303</v>
       </c>
       <c r="B1040" s="0" t="s">
-        <v>1563</v>
+        <v>1567</v>
       </c>
       <c r="C1040" s="0" t="s">
         <v>31</v>
@@ -40735,23 +40755,23 @@
         <v>334</v>
       </c>
       <c r="E1040" s="0" t="s">
-        <v>1564</v>
+        <v>1568</v>
       </c>
       <c r="F1040" s="0" t="s">
-        <v>1565</v>
+        <v>219</v>
       </c>
       <c r="G1040" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51fb29dd55442361fa9c5dbe23aca9c6.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7a107875bd58c5e655e8f87152a3bad7.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1040" s="0" t="s">
-        <v>1566</v>
+        <v>1569</v>
       </c>
       <c r="I1040" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1040" s="0" t="s">
-        <v>1567</v>
+        <v>1570</v>
       </c>
       <c r="K1040" s="0" t="s">
         <v>305</v>
@@ -40762,32 +40782,32 @@
         <v>303</v>
       </c>
       <c r="B1041" s="0" t="s">
-        <v>1568</v>
+        <v>1522</v>
       </c>
       <c r="C1041" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D1041" s="0" t="s">
-        <v>334</v>
+        <v>304</v>
       </c>
       <c r="E1041" s="0" t="s">
-        <v>1569</v>
+        <v>1524</v>
       </c>
       <c r="F1041" s="0" t="s">
-        <v>16</v>
+        <v>219</v>
       </c>
       <c r="G1041" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/28e774ec0ecd561a6a3d437e6c443a6b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154ab10964742eaff37de9cc5beef39c.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1041" s="0" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="I1041" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1041" s="0" t="s">
-        <v>1571</v>
+        <v>1527</v>
       </c>
       <c r="K1041" s="0" t="s">
         <v>305</v>
@@ -40804,26 +40824,26 @@
         <v>31</v>
       </c>
       <c r="D1042" s="0" t="s">
-        <v>334</v>
+        <v>1573</v>
       </c>
       <c r="E1042" s="0" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="F1042" s="0" t="s">
-        <v>219</v>
+        <v>838</v>
       </c>
       <c r="G1042" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7a107875bd58c5e655e8f87152a3bad7.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5c4978e802ba55d5a298cf1b3bdc2b3a.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1042" s="0" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="I1042" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1042" s="0" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="K1042" s="0" t="s">
         <v>305</v>
@@ -40834,32 +40854,32 @@
         <v>303</v>
       </c>
       <c r="B1043" s="0" t="s">
-        <v>1522</v>
+        <v>1577</v>
       </c>
       <c r="C1043" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D1043" s="0" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
       <c r="E1043" s="0" t="s">
-        <v>1524</v>
+        <v>1578</v>
       </c>
       <c r="F1043" s="0" t="s">
-        <v>219</v>
+        <v>838</v>
       </c>
       <c r="G1043" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154ab10964742eaff37de9cc5beef39c.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90c49fce92dc1f21647dad07d1342843.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1043" s="0" t="s">
-        <v>1576</v>
+        <v>1579</v>
       </c>
       <c r="I1043" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1043" s="0" t="s">
-        <v>1527</v>
+        <v>1580</v>
       </c>
       <c r="K1043" s="0" t="s">
         <v>305</v>
@@ -40870,32 +40890,32 @@
         <v>303</v>
       </c>
       <c r="B1044" s="0" t="s">
-        <v>1577</v>
+        <v>1581</v>
       </c>
       <c r="C1044" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D1044" s="0" t="s">
-        <v>1578</v>
+        <v>367</v>
       </c>
       <c r="E1044" s="0" t="s">
-        <v>1579</v>
+        <v>1582</v>
       </c>
       <c r="F1044" s="0" t="s">
-        <v>838</v>
+        <v>219</v>
       </c>
       <c r="G1044" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5c4978e802ba55d5a298cf1b3bdc2b3a.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3d23c359f44d6a153c4dcab9e07d7cb6.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1044" s="0" t="s">
-        <v>1580</v>
+        <v>1583</v>
       </c>
       <c r="I1044" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1044" s="0" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="K1044" s="0" t="s">
         <v>305</v>
@@ -40906,7 +40926,7 @@
         <v>303</v>
       </c>
       <c r="B1045" s="0" t="s">
-        <v>1582</v>
+        <v>1584</v>
       </c>
       <c r="C1045" s="0" t="s">
         <v>31</v>
@@ -40915,23 +40935,23 @@
         <v>367</v>
       </c>
       <c r="E1045" s="0" t="s">
-        <v>1583</v>
+        <v>1585</v>
       </c>
       <c r="F1045" s="0" t="s">
-        <v>838</v>
+        <v>219</v>
       </c>
       <c r="G1045" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90c49fce92dc1f21647dad07d1342843.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8c9504d28596e05586c8e193082ac617.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1045" s="0" t="s">
-        <v>1584</v>
+        <v>1586</v>
       </c>
       <c r="I1045" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1045" s="0" t="s">
-        <v>1585</v>
+        <v>1587</v>
       </c>
       <c r="K1045" s="0" t="s">
         <v>305</v>
@@ -40942,32 +40962,32 @@
         <v>303</v>
       </c>
       <c r="B1046" s="0" t="s">
-        <v>1586</v>
+        <v>1588</v>
       </c>
       <c r="C1046" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D1046" s="0" t="s">
-        <v>367</v>
+        <v>1589</v>
       </c>
       <c r="E1046" s="0" t="s">
-        <v>1587</v>
+        <v>1590</v>
       </c>
       <c r="F1046" s="0" t="s">
-        <v>219</v>
+        <v>252</v>
       </c>
       <c r="G1046" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3d23c359f44d6a153c4dcab9e07d7cb6.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e72b243a2a1c8691ab0168d8b62534c2.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1046" s="0" t="s">
-        <v>1588</v>
+        <v>1591</v>
       </c>
       <c r="I1046" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1046" s="0" t="s">
-        <v>1587</v>
+        <v>1592</v>
       </c>
       <c r="K1046" s="0" t="s">
         <v>305</v>
@@ -40978,32 +40998,32 @@
         <v>303</v>
       </c>
       <c r="B1047" s="0" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C1047" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1047" s="0" t="s">
         <v>1589</v>
       </c>
-      <c r="C1047" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1047" s="0" t="s">
-        <v>367</v>
-      </c>
       <c r="E1047" s="0" t="s">
-        <v>1590</v>
+        <v>1594</v>
       </c>
       <c r="F1047" s="0" t="s">
-        <v>219</v>
+        <v>252</v>
       </c>
       <c r="G1047" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8c9504d28596e05586c8e193082ac617.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b1cd51f370e346ecb20f1e80cb6ea4.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1047" s="0" t="s">
-        <v>1591</v>
+        <v>1595</v>
       </c>
       <c r="I1047" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1047" s="0" t="s">
-        <v>1592</v>
+        <v>1596</v>
       </c>
       <c r="K1047" s="0" t="s">
         <v>305</v>
@@ -41014,32 +41034,32 @@
         <v>303</v>
       </c>
       <c r="B1048" s="0" t="s">
-        <v>1593</v>
+        <v>1597</v>
       </c>
       <c r="C1048" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D1048" s="0" t="s">
-        <v>1594</v>
+        <v>1589</v>
       </c>
       <c r="E1048" s="0" t="s">
-        <v>1595</v>
+        <v>1598</v>
       </c>
       <c r="F1048" s="0" t="s">
         <v>252</v>
       </c>
       <c r="G1048" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e72b243a2a1c8691ab0168d8b62534c2.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4b97609a32d53dff5b8e73729e4f258b.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1048" s="0" t="s">
-        <v>1596</v>
+        <v>1599</v>
       </c>
       <c r="I1048" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1048" s="0" t="s">
-        <v>1597</v>
+        <v>1600</v>
       </c>
       <c r="K1048" s="0" t="s">
         <v>305</v>
@@ -41050,32 +41070,32 @@
         <v>303</v>
       </c>
       <c r="B1049" s="0" t="s">
-        <v>1598</v>
+        <v>1601</v>
       </c>
       <c r="C1049" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D1049" s="0" t="s">
-        <v>1594</v>
+        <v>1573</v>
       </c>
       <c r="E1049" s="0" t="s">
-        <v>1599</v>
+        <v>1602</v>
       </c>
       <c r="F1049" s="0" t="s">
-        <v>252</v>
+        <v>24</v>
       </c>
       <c r="G1049" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b1cd51f370e346ecb20f1e80cb6ea4.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c75f684ec69602e9de82b48e53afb2cc.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1049" s="0" t="s">
-        <v>1600</v>
+        <v>1603</v>
       </c>
       <c r="I1049" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1049" s="0" t="s">
-        <v>1601</v>
+        <v>999</v>
       </c>
       <c r="K1049" s="0" t="s">
         <v>305</v>
@@ -41086,32 +41106,32 @@
         <v>303</v>
       </c>
       <c r="B1050" s="0" t="s">
-        <v>1602</v>
+        <v>1604</v>
       </c>
       <c r="C1050" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D1050" s="0" t="s">
-        <v>1594</v>
+        <v>1573</v>
       </c>
       <c r="E1050" s="0" t="s">
-        <v>1603</v>
+        <v>1605</v>
       </c>
       <c r="F1050" s="0" t="s">
-        <v>252</v>
+        <v>31</v>
       </c>
       <c r="G1050" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4b97609a32d53dff5b8e73729e4f258b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ebfefc2ab8716ef597b128171b275945.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1050" s="0" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="I1050" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1050" s="0" t="s">
-        <v>1605</v>
+        <v>1607</v>
       </c>
       <c r="K1050" s="0" t="s">
         <v>305</v>
@@ -41122,32 +41142,32 @@
         <v>303</v>
       </c>
       <c r="B1051" s="0" t="s">
-        <v>1606</v>
+        <v>1608</v>
       </c>
       <c r="C1051" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D1051" s="0" t="s">
-        <v>1578</v>
+        <v>367</v>
       </c>
       <c r="E1051" s="0" t="s">
-        <v>1607</v>
+        <v>1609</v>
       </c>
       <c r="F1051" s="0" t="s">
-        <v>24</v>
+        <v>196</v>
       </c>
       <c r="G1051" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c75f684ec69602e9de82b48e53afb2cc.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/62f26742cf240c1b5169a5cd511196b6.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1051" s="0" t="s">
-        <v>1608</v>
+        <v>1610</v>
       </c>
       <c r="I1051" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1051" s="0" t="s">
-        <v>999</v>
+        <v>1611</v>
       </c>
       <c r="K1051" s="0" t="s">
         <v>305</v>
@@ -41158,32 +41178,32 @@
         <v>303</v>
       </c>
       <c r="B1052" s="0" t="s">
-        <v>1609</v>
+        <v>1612</v>
       </c>
       <c r="C1052" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D1052" s="0" t="s">
-        <v>1578</v>
+        <v>367</v>
       </c>
       <c r="E1052" s="0" t="s">
-        <v>1610</v>
+        <v>1613</v>
       </c>
       <c r="F1052" s="0" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="G1052" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ebfefc2ab8716ef597b128171b275945.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/051919eddec810e292c883205c944ceb.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1052" s="0" t="s">
-        <v>1611</v>
+        <v>1614</v>
       </c>
       <c r="I1052" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1052" s="0" t="s">
-        <v>1612</v>
+        <v>1615</v>
       </c>
       <c r="K1052" s="0" t="s">
         <v>305</v>
@@ -41194,7 +41214,7 @@
         <v>303</v>
       </c>
       <c r="B1053" s="0" t="s">
-        <v>1613</v>
+        <v>1616</v>
       </c>
       <c r="C1053" s="0" t="s">
         <v>31</v>
@@ -41203,23 +41223,23 @@
         <v>367</v>
       </c>
       <c r="E1053" s="0" t="s">
-        <v>1614</v>
+        <v>1617</v>
       </c>
       <c r="F1053" s="0" t="s">
         <v>196</v>
       </c>
       <c r="G1053" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/62f26742cf240c1b5169a5cd511196b6.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/aa2bea81f238ad8f2c35a7e16ad97801.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1053" s="0" t="s">
-        <v>1615</v>
+        <v>1618</v>
       </c>
       <c r="I1053" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1053" s="0" t="s">
-        <v>1616</v>
+        <v>1619</v>
       </c>
       <c r="K1053" s="0" t="s">
         <v>305</v>
@@ -41230,7 +41250,7 @@
         <v>303</v>
       </c>
       <c r="B1054" s="0" t="s">
-        <v>1617</v>
+        <v>1620</v>
       </c>
       <c r="C1054" s="0" t="s">
         <v>31</v>
@@ -41239,23 +41259,23 @@
         <v>367</v>
       </c>
       <c r="E1054" s="0" t="s">
-        <v>1618</v>
+        <v>1621</v>
       </c>
       <c r="F1054" s="0" t="s">
         <v>196</v>
       </c>
       <c r="G1054" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/051919eddec810e292c883205c944ceb.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/089961a3af4d54d5fb045cf3750e760c.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1054" s="0" t="s">
-        <v>1619</v>
+        <v>1622</v>
       </c>
       <c r="I1054" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1054" s="0" t="s">
-        <v>1620</v>
+        <v>1623</v>
       </c>
       <c r="K1054" s="0" t="s">
         <v>305</v>
@@ -41266,7 +41286,7 @@
         <v>303</v>
       </c>
       <c r="B1055" s="0" t="s">
-        <v>1621</v>
+        <v>1624</v>
       </c>
       <c r="C1055" s="0" t="s">
         <v>31</v>
@@ -41275,23 +41295,23 @@
         <v>367</v>
       </c>
       <c r="E1055" s="0" t="s">
-        <v>1622</v>
+        <v>1625</v>
       </c>
       <c r="F1055" s="0" t="s">
         <v>196</v>
       </c>
       <c r="G1055" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/aa2bea81f238ad8f2c35a7e16ad97801.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3a8e1636a31c82fbdd9a1ae45ab3be7d.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1055" s="0" t="s">
-        <v>1623</v>
+        <v>1626</v>
       </c>
       <c r="I1055" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1055" s="0" t="s">
-        <v>1624</v>
+        <v>1627</v>
       </c>
       <c r="K1055" s="0" t="s">
         <v>305</v>
@@ -41302,7 +41322,7 @@
         <v>303</v>
       </c>
       <c r="B1056" s="0" t="s">
-        <v>1625</v>
+        <v>1628</v>
       </c>
       <c r="C1056" s="0" t="s">
         <v>31</v>
@@ -41311,23 +41331,23 @@
         <v>367</v>
       </c>
       <c r="E1056" s="0" t="s">
-        <v>1626</v>
+        <v>1629</v>
       </c>
       <c r="F1056" s="0" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="G1056" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/089961a3af4d54d5fb045cf3750e760c.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3abb7c5b4c4650e9d17a8439004aebea.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1056" s="0" t="s">
-        <v>1627</v>
+        <v>1630</v>
       </c>
       <c r="I1056" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1056" s="0" t="s">
-        <v>1628</v>
+        <v>1631</v>
       </c>
       <c r="K1056" s="0" t="s">
         <v>305</v>
@@ -41338,7 +41358,7 @@
         <v>303</v>
       </c>
       <c r="B1057" s="0" t="s">
-        <v>1629</v>
+        <v>1632</v>
       </c>
       <c r="C1057" s="0" t="s">
         <v>31</v>
@@ -41347,23 +41367,23 @@
         <v>367</v>
       </c>
       <c r="E1057" s="0" t="s">
-        <v>1630</v>
+        <v>1633</v>
       </c>
       <c r="F1057" s="0" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="G1057" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3a8e1636a31c82fbdd9a1ae45ab3be7d.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bd10cebbde1593b65e5220911f9a997c.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1057" s="0" t="s">
-        <v>1631</v>
+        <v>1634</v>
       </c>
       <c r="I1057" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1057" s="0" t="s">
-        <v>1632</v>
+        <v>1635</v>
       </c>
       <c r="K1057" s="0" t="s">
         <v>305</v>
@@ -41374,7 +41394,7 @@
         <v>303</v>
       </c>
       <c r="B1058" s="0" t="s">
-        <v>1633</v>
+        <v>1636</v>
       </c>
       <c r="C1058" s="0" t="s">
         <v>31</v>
@@ -41383,23 +41403,23 @@
         <v>367</v>
       </c>
       <c r="E1058" s="0" t="s">
-        <v>1634</v>
+        <v>1637</v>
       </c>
       <c r="F1058" s="0" t="s">
-        <v>219</v>
+        <v>308</v>
       </c>
       <c r="G1058" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3abb7c5b4c4650e9d17a8439004aebea.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/95cbf6ac889c8fe7d92e20e8c34960d1.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1058" s="0" t="s">
-        <v>1635</v>
+        <v>1638</v>
       </c>
       <c r="I1058" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1058" s="0" t="s">
-        <v>1636</v>
+        <v>1220</v>
       </c>
       <c r="K1058" s="0" t="s">
         <v>305</v>
@@ -41410,7 +41430,7 @@
         <v>303</v>
       </c>
       <c r="B1059" s="0" t="s">
-        <v>1637</v>
+        <v>1639</v>
       </c>
       <c r="C1059" s="0" t="s">
         <v>31</v>
@@ -41419,23 +41439,23 @@
         <v>367</v>
       </c>
       <c r="E1059" s="0" t="s">
-        <v>1638</v>
+        <v>1640</v>
       </c>
       <c r="F1059" s="0" t="s">
-        <v>219</v>
+        <v>308</v>
       </c>
       <c r="G1059" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bd10cebbde1593b65e5220911f9a997c.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a13ed886b17e20cdae8b89b9ff8e4610.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1059" s="0" t="s">
-        <v>1639</v>
+        <v>1641</v>
       </c>
       <c r="I1059" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1059" s="0" t="s">
-        <v>1640</v>
+        <v>1642</v>
       </c>
       <c r="K1059" s="0" t="s">
         <v>305</v>
@@ -41446,7 +41466,7 @@
         <v>303</v>
       </c>
       <c r="B1060" s="0" t="s">
-        <v>1641</v>
+        <v>1643</v>
       </c>
       <c r="C1060" s="0" t="s">
         <v>31</v>
@@ -41455,23 +41475,23 @@
         <v>367</v>
       </c>
       <c r="E1060" s="0" t="s">
-        <v>1642</v>
+        <v>1644</v>
       </c>
       <c r="F1060" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1060" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/95cbf6ac889c8fe7d92e20e8c34960d1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70d7d6fc0e9c2f14624a0270bf2b99b9.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1060" s="0" t="s">
-        <v>1643</v>
+        <v>1645</v>
       </c>
       <c r="I1060" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1060" s="0" t="s">
-        <v>1220</v>
+        <v>1646</v>
       </c>
       <c r="K1060" s="0" t="s">
         <v>305</v>
@@ -41482,7 +41502,7 @@
         <v>303</v>
       </c>
       <c r="B1061" s="0" t="s">
-        <v>1644</v>
+        <v>1647</v>
       </c>
       <c r="C1061" s="0" t="s">
         <v>31</v>
@@ -41491,23 +41511,23 @@
         <v>367</v>
       </c>
       <c r="E1061" s="0" t="s">
-        <v>1645</v>
+        <v>1648</v>
       </c>
       <c r="F1061" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1061" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a13ed886b17e20cdae8b89b9ff8e4610.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/89027ee0079acb709750ddeac1c08899.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1061" s="0" t="s">
-        <v>1646</v>
+        <v>1649</v>
       </c>
       <c r="I1061" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1061" s="0" t="s">
-        <v>1647</v>
+        <v>1229</v>
       </c>
       <c r="K1061" s="0" t="s">
         <v>305</v>
@@ -41518,7 +41538,7 @@
         <v>303</v>
       </c>
       <c r="B1062" s="0" t="s">
-        <v>1648</v>
+        <v>1650</v>
       </c>
       <c r="C1062" s="0" t="s">
         <v>31</v>
@@ -41527,23 +41547,23 @@
         <v>367</v>
       </c>
       <c r="E1062" s="0" t="s">
-        <v>1649</v>
+        <v>1651</v>
       </c>
       <c r="F1062" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1062" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70d7d6fc0e9c2f14624a0270bf2b99b9.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e7b9f984d3bba15daccaaa18039a85d.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1062" s="0" t="s">
-        <v>1650</v>
+        <v>1652</v>
       </c>
       <c r="I1062" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1062" s="0" t="s">
-        <v>1651</v>
+        <v>1653</v>
       </c>
       <c r="K1062" s="0" t="s">
         <v>305</v>
@@ -41554,7 +41574,7 @@
         <v>303</v>
       </c>
       <c r="B1063" s="0" t="s">
-        <v>1652</v>
+        <v>1654</v>
       </c>
       <c r="C1063" s="0" t="s">
         <v>31</v>
@@ -41563,23 +41583,23 @@
         <v>367</v>
       </c>
       <c r="E1063" s="0" t="s">
-        <v>1653</v>
+        <v>1655</v>
       </c>
       <c r="F1063" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1063" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/89027ee0079acb709750ddeac1c08899.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70bf79db957daa3b82413da949233ac7.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1063" s="0" t="s">
-        <v>1654</v>
+        <v>1656</v>
       </c>
       <c r="I1063" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1063" s="0" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
       <c r="K1063" s="0" t="s">
         <v>305</v>
@@ -41590,7 +41610,7 @@
         <v>303</v>
       </c>
       <c r="B1064" s="0" t="s">
-        <v>1655</v>
+        <v>1657</v>
       </c>
       <c r="C1064" s="0" t="s">
         <v>31</v>
@@ -41599,23 +41619,23 @@
         <v>367</v>
       </c>
       <c r="E1064" s="0" t="s">
-        <v>1656</v>
+        <v>1658</v>
       </c>
       <c r="F1064" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1064" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e7b9f984d3bba15daccaaa18039a85d.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d0a35d5c99a0aa93ad4069cfe83bf748.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1064" s="0" t="s">
-        <v>1657</v>
+        <v>1659</v>
       </c>
       <c r="I1064" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1064" s="0" t="s">
-        <v>1658</v>
+        <v>1660</v>
       </c>
       <c r="K1064" s="0" t="s">
         <v>305</v>
@@ -41626,7 +41646,7 @@
         <v>303</v>
       </c>
       <c r="B1065" s="0" t="s">
-        <v>1659</v>
+        <v>1661</v>
       </c>
       <c r="C1065" s="0" t="s">
         <v>31</v>
@@ -41635,23 +41655,23 @@
         <v>367</v>
       </c>
       <c r="E1065" s="0" t="s">
-        <v>1660</v>
+        <v>1662</v>
       </c>
       <c r="F1065" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1065" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70bf79db957daa3b82413da949233ac7.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e2.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1065" s="0" t="s">
-        <v>1661</v>
+        <v>1656</v>
       </c>
       <c r="I1065" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1065" s="0" t="s">
-        <v>1226</v>
+        <v>1663</v>
       </c>
       <c r="K1065" s="0" t="s">
         <v>305</v>
@@ -41662,7 +41682,7 @@
         <v>303</v>
       </c>
       <c r="B1066" s="0" t="s">
-        <v>1662</v>
+        <v>1664</v>
       </c>
       <c r="C1066" s="0" t="s">
         <v>31</v>
@@ -41671,23 +41691,23 @@
         <v>367</v>
       </c>
       <c r="E1066" s="0" t="s">
-        <v>1663</v>
+        <v>1665</v>
       </c>
       <c r="F1066" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1066" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d0a35d5c99a0aa93ad4069cfe83bf748.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7b2d1e1a3ece1169d8ac61af4b758ed2.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1066" s="0" t="s">
-        <v>1664</v>
+        <v>1666</v>
       </c>
       <c r="I1066" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1066" s="0" t="s">
-        <v>1665</v>
+        <v>1667</v>
       </c>
       <c r="K1066" s="0" t="s">
         <v>305</v>
@@ -41698,7 +41718,7 @@
         <v>303</v>
       </c>
       <c r="B1067" s="0" t="s">
-        <v>1666</v>
+        <v>1668</v>
       </c>
       <c r="C1067" s="0" t="s">
         <v>31</v>
@@ -41707,23 +41727,23 @@
         <v>367</v>
       </c>
       <c r="E1067" s="0" t="s">
-        <v>1667</v>
+        <v>1669</v>
       </c>
       <c r="F1067" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1067" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e2.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a21e250a10f96b1c1ad6d742206a157e.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1067" s="0" t="s">
-        <v>1661</v>
+        <v>1670</v>
       </c>
       <c r="I1067" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1067" s="0" t="s">
-        <v>1668</v>
+        <v>1671</v>
       </c>
       <c r="K1067" s="0" t="s">
         <v>305</v>
@@ -41734,7 +41754,7 @@
         <v>303</v>
       </c>
       <c r="B1068" s="0" t="s">
-        <v>1669</v>
+        <v>1672</v>
       </c>
       <c r="C1068" s="0" t="s">
         <v>31</v>
@@ -41743,23 +41763,23 @@
         <v>367</v>
       </c>
       <c r="E1068" s="0" t="s">
-        <v>1670</v>
+        <v>1673</v>
       </c>
       <c r="F1068" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1068" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7b2d1e1a3ece1169d8ac61af4b758ed2.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b907fef85d4c9571a9457ee1b259bb8f.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1068" s="0" t="s">
-        <v>1671</v>
+        <v>1674</v>
       </c>
       <c r="I1068" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1068" s="0" t="s">
-        <v>1672</v>
+        <v>1675</v>
       </c>
       <c r="K1068" s="0" t="s">
         <v>305</v>
@@ -41770,7 +41790,7 @@
         <v>303</v>
       </c>
       <c r="B1069" s="0" t="s">
-        <v>1673</v>
+        <v>1676</v>
       </c>
       <c r="C1069" s="0" t="s">
         <v>31</v>
@@ -41779,23 +41799,23 @@
         <v>367</v>
       </c>
       <c r="E1069" s="0" t="s">
-        <v>1674</v>
+        <v>1677</v>
       </c>
       <c r="F1069" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1069" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a21e250a10f96b1c1ad6d742206a157e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/63345d9732c72b97ca395f24ce2d6642.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1069" s="0" t="s">
-        <v>1675</v>
+        <v>1678</v>
       </c>
       <c r="I1069" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1069" s="0" t="s">
-        <v>1676</v>
+        <v>1679</v>
       </c>
       <c r="K1069" s="0" t="s">
         <v>305</v>
@@ -41806,7 +41826,7 @@
         <v>303</v>
       </c>
       <c r="B1070" s="0" t="s">
-        <v>1677</v>
+        <v>1680</v>
       </c>
       <c r="C1070" s="0" t="s">
         <v>31</v>
@@ -41815,23 +41835,23 @@
         <v>367</v>
       </c>
       <c r="E1070" s="0" t="s">
-        <v>1678</v>
+        <v>1681</v>
       </c>
       <c r="F1070" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1070" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b907fef85d4c9571a9457ee1b259bb8f.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/921b8b8f6620826567d9324314c70410.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1070" s="0" t="s">
-        <v>1679</v>
+        <v>1682</v>
       </c>
       <c r="I1070" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1070" s="0" t="s">
-        <v>1680</v>
+        <v>1683</v>
       </c>
       <c r="K1070" s="0" t="s">
         <v>305</v>
@@ -41842,7 +41862,7 @@
         <v>303</v>
       </c>
       <c r="B1071" s="0" t="s">
-        <v>1681</v>
+        <v>1684</v>
       </c>
       <c r="C1071" s="0" t="s">
         <v>31</v>
@@ -41851,23 +41871,23 @@
         <v>367</v>
       </c>
       <c r="E1071" s="0" t="s">
-        <v>1682</v>
+        <v>1685</v>
       </c>
       <c r="F1071" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G1071" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/63345d9732c72b97ca395f24ce2d6642.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/12e0369ff0ba1a6f1a84e0d9565d4b07.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1071" s="0" t="s">
-        <v>1683</v>
+        <v>1686</v>
       </c>
       <c r="I1071" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1071" s="0" t="s">
-        <v>1684</v>
+        <v>1687</v>
       </c>
       <c r="K1071" s="0" t="s">
         <v>305</v>
@@ -41878,7 +41898,7 @@
         <v>303</v>
       </c>
       <c r="B1072" s="0" t="s">
-        <v>1685</v>
+        <v>1688</v>
       </c>
       <c r="C1072" s="0" t="s">
         <v>31</v>
@@ -41887,23 +41907,23 @@
         <v>367</v>
       </c>
       <c r="E1072" s="0" t="s">
-        <v>1686</v>
+        <v>1689</v>
       </c>
       <c r="F1072" s="0" t="s">
-        <v>308</v>
+        <v>965</v>
       </c>
       <c r="G1072" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/921b8b8f6620826567d9324314c70410.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fc637f1c75e58be8a6e4112411a00f36.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1072" s="0" t="s">
-        <v>1687</v>
+        <v>1690</v>
       </c>
       <c r="I1072" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1072" s="0" t="s">
-        <v>1688</v>
+        <v>1691</v>
       </c>
       <c r="K1072" s="0" t="s">
         <v>305</v>
@@ -41914,7 +41934,7 @@
         <v>303</v>
       </c>
       <c r="B1073" s="0" t="s">
-        <v>1689</v>
+        <v>1692</v>
       </c>
       <c r="C1073" s="0" t="s">
         <v>31</v>
@@ -41923,23 +41943,23 @@
         <v>367</v>
       </c>
       <c r="E1073" s="0" t="s">
-        <v>1690</v>
+        <v>1693</v>
       </c>
       <c r="F1073" s="0" t="s">
-        <v>308</v>
+        <v>24</v>
       </c>
       <c r="G1073" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/12e0369ff0ba1a6f1a84e0d9565d4b07.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7c2249d424dde72f8616d42870a9d425.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1073" s="0" t="s">
-        <v>1691</v>
+        <v>1694</v>
       </c>
       <c r="I1073" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1073" s="0" t="s">
-        <v>1692</v>
+        <v>1695</v>
       </c>
       <c r="K1073" s="0" t="s">
         <v>305</v>
@@ -41950,7 +41970,7 @@
         <v>303</v>
       </c>
       <c r="B1074" s="0" t="s">
-        <v>1693</v>
+        <v>1696</v>
       </c>
       <c r="C1074" s="0" t="s">
         <v>31</v>
@@ -41959,23 +41979,23 @@
         <v>367</v>
       </c>
       <c r="E1074" s="0" t="s">
-        <v>1694</v>
+        <v>1697</v>
       </c>
       <c r="F1074" s="0" t="s">
         <v>965</v>
       </c>
       <c r="G1074" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fc637f1c75e58be8a6e4112411a00f36.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/80a1dd605b563e9f09c718a5ba9cb9cc.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1074" s="0" t="s">
-        <v>1695</v>
+        <v>1698</v>
       </c>
       <c r="I1074" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1074" s="0" t="s">
-        <v>1696</v>
+        <v>1699</v>
       </c>
       <c r="K1074" s="0" t="s">
         <v>305</v>
@@ -41986,7 +42006,7 @@
         <v>303</v>
       </c>
       <c r="B1075" s="0" t="s">
-        <v>1697</v>
+        <v>1700</v>
       </c>
       <c r="C1075" s="0" t="s">
         <v>31</v>
@@ -41995,23 +42015,23 @@
         <v>367</v>
       </c>
       <c r="E1075" s="0" t="s">
-        <v>1698</v>
+        <v>1701</v>
       </c>
       <c r="F1075" s="0" t="s">
-        <v>24</v>
+        <v>965</v>
       </c>
       <c r="G1075" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7c2249d424dde72f8616d42870a9d425.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/73c496f5669cc122cf1cddfe4df2a27a.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1075" s="0" t="s">
-        <v>1699</v>
+        <v>1702</v>
       </c>
       <c r="I1075" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1075" s="0" t="s">
-        <v>1700</v>
+        <v>1703</v>
       </c>
       <c r="K1075" s="0" t="s">
         <v>305</v>
@@ -42022,7 +42042,7 @@
         <v>303</v>
       </c>
       <c r="B1076" s="0" t="s">
-        <v>1701</v>
+        <v>1704</v>
       </c>
       <c r="C1076" s="0" t="s">
         <v>31</v>
@@ -42031,23 +42051,23 @@
         <v>367</v>
       </c>
       <c r="E1076" s="0" t="s">
-        <v>1702</v>
+        <v>1705</v>
       </c>
       <c r="F1076" s="0" t="s">
-        <v>965</v>
+        <v>308</v>
       </c>
       <c r="G1076" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/80a1dd605b563e9f09c718a5ba9cb9cc.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/26328c46dfcc65d454b6fd4c52ccb48f.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1076" s="0" t="s">
-        <v>1703</v>
+        <v>1706</v>
       </c>
       <c r="I1076" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1076" s="0" t="s">
-        <v>1704</v>
+        <v>1707</v>
       </c>
       <c r="K1076" s="0" t="s">
         <v>305</v>
@@ -42058,7 +42078,7 @@
         <v>303</v>
       </c>
       <c r="B1077" s="0" t="s">
-        <v>1705</v>
+        <v>1708</v>
       </c>
       <c r="C1077" s="0" t="s">
         <v>31</v>
@@ -42067,23 +42087,23 @@
         <v>367</v>
       </c>
       <c r="E1077" s="0" t="s">
-        <v>1706</v>
+        <v>1709</v>
       </c>
       <c r="F1077" s="0" t="s">
-        <v>965</v>
+        <v>196</v>
       </c>
       <c r="G1077" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/73c496f5669cc122cf1cddfe4df2a27a.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc1b9e3073d751143fe8ab63ca9fcc45.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1077" s="0" t="s">
-        <v>1707</v>
+        <v>1710</v>
       </c>
       <c r="I1077" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1077" s="0" t="s">
-        <v>1708</v>
+        <v>1711</v>
       </c>
       <c r="K1077" s="0" t="s">
         <v>305</v>
@@ -42094,7 +42114,7 @@
         <v>303</v>
       </c>
       <c r="B1078" s="0" t="s">
-        <v>1709</v>
+        <v>1712</v>
       </c>
       <c r="C1078" s="0" t="s">
         <v>31</v>
@@ -42103,100 +42123,30 @@
         <v>367</v>
       </c>
       <c r="E1078" s="0" t="s">
-        <v>1710</v>
+        <v>1713</v>
       </c>
       <c r="F1078" s="0" t="s">
-        <v>308</v>
+        <v>196</v>
       </c>
       <c r="G1078" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/26328c46dfcc65d454b6fd4c52ccb48f.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/299fb9d19040c4aa3862644286261ad2.html","web")</f>
         <v>web</v>
       </c>
       <c r="H1078" s="0" t="s">
-        <v>1711</v>
+        <v>1714</v>
       </c>
       <c r="I1078" s="0" t="s">
         <v>1526</v>
       </c>
       <c r="J1078" s="0" t="s">
-        <v>1712</v>
+        <v>1715</v>
       </c>
       <c r="K1078" s="0" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="1079" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1079" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1079" s="0" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C1079" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1079" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1079" s="0" t="s">
-        <v>1714</v>
-      </c>
-      <c r="F1079" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1079" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc1b9e3073d751143fe8ab63ca9fcc45.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1079" s="0" t="s">
-        <v>1715</v>
-      </c>
-      <c r="I1079" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1079" s="0" t="s">
-        <v>1716</v>
-      </c>
-      <c r="K1079" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="1080" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1080" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1080" s="0" t="s">
-        <v>1717</v>
-      </c>
-      <c r="C1080" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1080" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1080" s="0" t="s">
-        <v>1718</v>
-      </c>
-      <c r="F1080" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1080" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/299fb9d19040c4aa3862644286261ad2.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H1080" s="0" t="s">
-        <v>1719</v>
-      </c>
-      <c r="I1080" s="0" t="s">
-        <v>1526</v>
-      </c>
-      <c r="J1080" s="0" t="s">
-        <v>1720</v>
-      </c>
-      <c r="K1080" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
The Ofx combinations with thkcello and masscello are added to the ignored list #249.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10197" uniqueCount="1714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10217" uniqueCount="1725">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -5162,6 +5162,39 @@
   </si>
   <si>
     <t xml:space="preserve">Carbon mass flux per unit area into atmosphere due to heterotrophic respiration on land (respiration by consumers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thkcello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ocean Model Cell Thickness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nemo code name = thkcello  but not constant in time in NEMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automatic, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Thickness' means the vertical extent of a layer. 'Cell' refers to a model grid-cell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMIP,DCPP,PAMIP,PMIP,VIACSAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">masscello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ocean Grid-Cell Mass per Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nemo code name = masscello  but not constant in time in NEMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracer grid-cell mass per unit area used for computing tracer budgets. For Boussinesq models with static ocean grid cell thickness, masscello = rhozero*thickcello, where thickcello is static cell thickness and rhozero is constant Boussinesq reference density. More generally, masscello is time dependent and reported as part of Omon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMIP,OMIP</t>
   </si>
 </sst>
 </file>
@@ -5291,8 +5324,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A926" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A941" activeCellId="0" sqref="A941"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1052" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1078" activeCellId="0" sqref="H1078"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42031,6 +42064,78 @@
         <v>968</v>
       </c>
     </row>
+    <row r="1078" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1078" s="3" t="s">
+        <v>946</v>
+      </c>
+      <c r="B1078" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C1078" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1078" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="E1078" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F1078" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1078" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5aea9677ebbb40076a0e0b3b11fdb46f.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1078" s="3" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I1078" s="3" t="s">
+        <v>1717</v>
+      </c>
+      <c r="J1078" s="3" t="s">
+        <v>1718</v>
+      </c>
+      <c r="K1078" s="3" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="1079" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1079" s="3" t="s">
+        <v>946</v>
+      </c>
+      <c r="B1079" s="3" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C1079" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1079" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="E1079" s="3" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F1079" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="G1079" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9122e7b627c429163fd0857dc366e14e.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1079" s="3" t="s">
+        <v>1722</v>
+      </c>
+      <c r="I1079" s="3" t="s">
+        <v>1717</v>
+      </c>
+      <c r="J1079" s="3" t="s">
+        <v>1723</v>
+      </c>
+      <c r="K1079" s="3" t="s">
+        <v>1724</v>
+      </c>
+    </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Moving the lpjg identified variable fHarvestToProduct to the pre-ignored and ignored list #445.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10237" uniqueCount="1725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10247" uniqueCount="1730">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -5219,6 +5219,21 @@
   </si>
   <si>
     <t xml:space="preserve">CMIP,OMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fHarvestToProduct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harvested Biomass That Goes into Product Pool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in LPJ-GUESS, see ec-earth issue 633-21 and ece2cmor3 issue 446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Warlind, Lars, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be it food or wood harvest, any carbon that is subsequently stored is reported here</t>
   </si>
 </sst>
 </file>
@@ -5349,7 +5364,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1055" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1083" activeCellId="0" sqref="B1083"/>
+      <selection pane="topLeft" activeCell="A1086" activeCellId="0" sqref="A1086"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42232,6 +42247,42 @@
         <v>716</v>
       </c>
     </row>
+    <row r="1086" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1086" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B1086" s="3" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1086" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1086" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1086" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="F1086" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1086" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a796-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1086" s="0" t="s">
+        <v>1727</v>
+      </c>
+      <c r="I1086" s="0" t="s">
+        <v>1728</v>
+      </c>
+      <c r="J1086" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="K1086" s="3" t="s">
+        <v>1031</v>
+      </c>
+    </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Moving the lpjg identified combination Eday mrros to the ignored list #445.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="B1083" authorId="0">
+    <comment ref="B1085" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10247" uniqueCount="1730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10257" uniqueCount="1735">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -5221,13 +5221,28 @@
     <t xml:space="preserve">CMIP,OMIP</t>
   </si>
   <si>
+    <t xml:space="preserve">mrros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface Runoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in LPJ-GUESS, see ec-earth issue 633-21 and ece2cmor3 issue 446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lars, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The total surface run off leaving the land portion of the grid cell (excluding drainage through the base of the soil model).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerChemMIP,C4MIP,CDRMIP,CFMIP,CMIP,FAFMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,LUMIP,PMIP,RFMIP,VIACSAB,VolMIP</t>
+  </si>
+  <si>
     <t xml:space="preserve">fHarvestToProduct</t>
   </si>
   <si>
     <t xml:space="preserve">Harvested Biomass That Goes into Product Pool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not available in LPJ-GUESS, see ec-earth issue 633-21 and ece2cmor3 issue 446</t>
   </si>
   <si>
     <t xml:space="preserve">David Warlind, Lars, Thomas</t>
@@ -5243,7 +5258,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5279,6 +5294,12 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5323,7 +5344,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5342,6 +5363,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -5363,8 +5388,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1055" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1086" activeCellId="0" sqref="A1086"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1058" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1083" activeCellId="0" sqref="1083:1083"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42175,116 +42200,157 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="1083" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1083" s="0" t="s">
+    <row r="1080" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1081" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1081" s="0" t="s">
+        <v>961</v>
+      </c>
+      <c r="B1081" s="3" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C1081" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1081" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1081" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="F1081" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1081" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/26a31ad76858198bd4d719aafeebe801.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1081" s="5" t="s">
+        <v>1727</v>
+      </c>
+      <c r="I1081" s="3" t="s">
+        <v>1728</v>
+      </c>
+      <c r="J1081" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="K1081" s="3" t="s">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="1082" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1082" s="0"/>
+    </row>
+    <row r="1083" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1083" s="0"/>
+    </row>
+    <row r="1085" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1085" s="0" t="s">
         <v>433</v>
       </c>
-      <c r="B1083" s="0" t="s">
+      <c r="B1085" s="0" t="s">
         <v>1478</v>
       </c>
-      <c r="C1083" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1083" s="0" t="s">
+      <c r="C1085" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1085" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="E1083" s="0" t="s">
+      <c r="E1085" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="F1083" s="0" t="s">
+      <c r="F1085" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="G1083" s="0" t="str">
+      <c r="G1085" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1083" s="0" t="s">
+      <c r="H1085" s="0" t="s">
         <v>1480</v>
       </c>
-      <c r="I1083" s="0" t="s">
+      <c r="I1085" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="J1083" s="0" t="s">
+      <c r="J1085" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="K1083" s="0" t="s">
+      <c r="K1085" s="0" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="1084" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1084" s="0" t="s">
+    <row r="1086" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1086" s="0" t="s">
         <v>912</v>
       </c>
-      <c r="B1084" s="0" t="s">
+      <c r="B1086" s="0" t="s">
         <v>1478</v>
       </c>
-      <c r="C1084" s="0" t="s">
+      <c r="C1086" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D1084" s="0" t="s">
+      <c r="D1086" s="0" t="s">
         <v>911</v>
       </c>
-      <c r="E1084" s="0" t="s">
+      <c r="E1086" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="F1084" s="0" t="s">
+      <c r="F1086" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="G1084" s="0" t="str">
+      <c r="G1086" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1084" s="0" t="s">
+      <c r="H1086" s="0" t="s">
         <v>1480</v>
       </c>
-      <c r="I1084" s="0" t="s">
+      <c r="I1086" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="J1084" s="0" t="s">
+      <c r="J1086" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="K1084" s="0" t="s">
+      <c r="K1086" s="0" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="1086" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1086" s="3" t="s">
+    <row r="1088" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1088" s="3" t="s">
         <v>1021</v>
       </c>
-      <c r="B1086" s="3" t="s">
-        <v>1725</v>
-      </c>
-      <c r="C1086" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1086" s="3" t="s">
+      <c r="B1088" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="C1088" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1088" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E1086" s="3" t="s">
-        <v>1726</v>
-      </c>
-      <c r="F1086" s="3" t="s">
+      <c r="E1088" s="3" t="s">
+        <v>1732</v>
+      </c>
+      <c r="F1088" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G1086" s="3" t="str">
+      <c r="G1088" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a796-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1086" s="0" t="s">
+      <c r="H1088" s="0" t="s">
         <v>1727</v>
       </c>
-      <c r="I1086" s="0" t="s">
-        <v>1728</v>
-      </c>
-      <c r="J1086" s="3" t="s">
-        <v>1729</v>
-      </c>
-      <c r="K1086" s="3" t="s">
+      <c r="I1088" s="0" t="s">
+        <v>1733</v>
+      </c>
+      <c r="J1088" s="3" t="s">
+        <v>1734</v>
+      </c>
+      <c r="K1088" s="3" t="s">
         <v>1031</v>
       </c>
     </row>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Moving the combinations E3hrPt o3 & Amon o3Clim to the ignored list #440.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="B1085" authorId="0">
+    <comment ref="B1087" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10257" uniqueCount="1735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10277" uniqueCount="1741">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -5237,6 +5237,24 @@
   </si>
   <si>
     <t xml:space="preserve">AerChemMIP,C4MIP,CDRMIP,CFMIP,CMIP,FAFMIP,GMMIP,GeoMIP,HighResMIP,LS3MIP,LUMIP,PMIP,RFMIP,VIACSAB,VolMIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole Fraction of O3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This combination is decided to be ignored in #440. tm5 code name = o3|ifs code name = 203.128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommi, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o3Clim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This combination is decided to be ignored in #440. tm5 code name = o3Clim</t>
   </si>
   <si>
     <t xml:space="preserve">fHarvestToProduct</t>
@@ -5388,8 +5406,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1058" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1083" activeCellId="0" sqref="1083:1083"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1058" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1083" activeCellId="0" sqref="I1083:I1084"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42224,7 +42242,7 @@
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/26a31ad76858198bd4d719aafeebe801.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1081" s="5" t="s">
+      <c r="H1081" s="3" t="s">
         <v>1727</v>
       </c>
       <c r="I1081" s="3" t="s">
@@ -42241,118 +42259,186 @@
       <c r="A1082" s="0"/>
     </row>
     <row r="1083" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1083" s="0"/>
-    </row>
-    <row r="1085" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1085" s="0" t="s">
+      <c r="A1083" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="B1083" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="C1083" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1083" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="E1083" s="3" t="s">
+        <v>1732</v>
+      </c>
+      <c r="F1083" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="G1083" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1d4594c97188efd47935238a429e02e4.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1083" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="I1083" s="5" t="s">
+        <v>1734</v>
+      </c>
+      <c r="J1083" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="K1083" s="3" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="1084" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1084" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="B1084" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="C1084" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1084" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="E1084" s="3" t="s">
+        <v>1732</v>
+      </c>
+      <c r="F1084" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="G1084" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1d4594c97188efd47935238a429e02e4.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H1084" s="3" t="s">
+        <v>1736</v>
+      </c>
+      <c r="I1084" s="5" t="s">
+        <v>1734</v>
+      </c>
+      <c r="J1084" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="K1084" s="3" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="1086" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1087" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1087" s="0" t="s">
         <v>433</v>
       </c>
-      <c r="B1085" s="0" t="s">
+      <c r="B1087" s="0" t="s">
         <v>1478</v>
       </c>
-      <c r="C1085" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1085" s="0" t="s">
+      <c r="C1087" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1087" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="E1085" s="0" t="s">
+      <c r="E1087" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="F1085" s="0" t="s">
+      <c r="F1087" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="G1085" s="0" t="str">
+      <c r="G1087" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1085" s="0" t="s">
+      <c r="H1087" s="0" t="s">
         <v>1480</v>
       </c>
-      <c r="I1085" s="0" t="s">
+      <c r="I1087" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="J1085" s="0" t="s">
+      <c r="J1087" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="K1085" s="0" t="s">
+      <c r="K1087" s="0" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="1086" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1086" s="0" t="s">
+    <row r="1088" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1088" s="0" t="s">
         <v>912</v>
       </c>
-      <c r="B1086" s="0" t="s">
+      <c r="B1088" s="0" t="s">
         <v>1478</v>
       </c>
-      <c r="C1086" s="0" t="s">
+      <c r="C1088" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D1086" s="0" t="s">
+      <c r="D1088" s="0" t="s">
         <v>911</v>
       </c>
-      <c r="E1086" s="0" t="s">
+      <c r="E1088" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="F1086" s="0" t="s">
+      <c r="F1088" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="G1086" s="0" t="str">
+      <c r="G1088" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1086" s="0" t="s">
+      <c r="H1088" s="0" t="s">
         <v>1480</v>
       </c>
-      <c r="I1086" s="0" t="s">
+      <c r="I1088" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="J1086" s="0" t="s">
+      <c r="J1088" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="K1086" s="0" t="s">
+      <c r="K1088" s="0" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="1088" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1088" s="3" t="s">
+    <row r="1090" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1090" s="3" t="s">
         <v>1021</v>
       </c>
-      <c r="B1088" s="3" t="s">
-        <v>1731</v>
-      </c>
-      <c r="C1088" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1088" s="3" t="s">
+      <c r="B1090" s="3" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C1090" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1090" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E1088" s="3" t="s">
-        <v>1732</v>
-      </c>
-      <c r="F1088" s="3" t="s">
+      <c r="E1090" s="3" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F1090" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G1088" s="3" t="str">
+      <c r="G1090" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a796-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1088" s="0" t="s">
+      <c r="H1090" s="0" t="s">
         <v>1727</v>
       </c>
-      <c r="I1088" s="0" t="s">
-        <v>1733</v>
-      </c>
-      <c r="J1088" s="3" t="s">
-        <v>1734</v>
-      </c>
-      <c r="K1088" s="3" t="s">
+      <c r="I1090" s="0" t="s">
+        <v>1739</v>
+      </c>
+      <c r="J1090" s="3" t="s">
+        <v>1740</v>
+      </c>
+      <c r="K1090" s="3" t="s">
         <v>1031</v>
       </c>
     </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Moving the combinations Amon ch4Clim & Amon ch4globalClim to the ignored list #441.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="B1087" authorId="0">
+    <comment ref="B1091" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10277" uniqueCount="1741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10297" uniqueCount="1746">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -5255,6 +5255,21 @@
   </si>
   <si>
     <t xml:space="preserve">This combination is decided to be ignored in #440. tm5 code name = o3Clim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch4Clim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mole Fraction of CH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This combination is decided to be ignored in #441 tm5 code name = ch4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch4globalClim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Mean Mole Fraction of CH4</t>
   </si>
   <si>
     <t xml:space="preserve">fHarvestToProduct</t>
@@ -5404,10 +5419,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K1094"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1058" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1083" activeCellId="0" sqref="I1083:I1084"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1061" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1084" activeCellId="0" sqref="1084:1084"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42295,154 +42310,225 @@
       </c>
     </row>
     <row r="1084" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1084" s="3" t="s">
+      <c r="I1084" s="5"/>
+    </row>
+    <row r="1085" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1085" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="B1084" s="3" t="s">
+      <c r="B1085" s="3" t="s">
         <v>1735</v>
       </c>
-      <c r="C1084" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1084" s="3" t="s">
+      <c r="C1085" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1085" s="3" t="s">
         <v>730</v>
       </c>
-      <c r="E1084" s="3" t="s">
+      <c r="E1085" s="3" t="s">
         <v>1732</v>
       </c>
-      <c r="F1084" s="3" t="s">
+      <c r="F1085" s="3" t="s">
         <v>696</v>
       </c>
-      <c r="G1084" s="3" t="str">
+      <c r="G1085" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1d4594c97188efd47935238a429e02e4.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1084" s="3" t="s">
+      <c r="H1085" s="3" t="s">
         <v>1736</v>
       </c>
-      <c r="I1084" s="5" t="s">
+      <c r="I1085" s="5" t="s">
         <v>1734</v>
       </c>
-      <c r="J1084" s="3" t="s">
+      <c r="J1085" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="K1084" s="3" t="s">
+      <c r="K1085" s="3" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="1086" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1087" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1086" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1086" s="0" t="s">
+        <v>717</v>
+      </c>
+      <c r="B1086" s="0" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C1086" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1086" s="0" t="s">
+        <v>730</v>
+      </c>
+      <c r="E1086" s="0" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F1086" s="0" t="s">
+        <v>696</v>
+      </c>
+      <c r="G1086" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H1086" s="0" t="s">
+        <v>1739</v>
+      </c>
+      <c r="I1086" s="0" t="s">
+        <v>1513</v>
+      </c>
+      <c r="J1086" s="0" t="s">
+        <v>727</v>
+      </c>
+      <c r="K1086" s="0" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="1087" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1087" s="0" t="s">
+        <v>717</v>
+      </c>
+      <c r="B1087" s="0" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C1087" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1087" s="0" t="s">
+        <v>739</v>
+      </c>
+      <c r="E1087" s="0" t="s">
+        <v>1741</v>
+      </c>
+      <c r="F1087" s="0" t="s">
+        <v>750</v>
+      </c>
+      <c r="G1087" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H1087" s="0" t="s">
+        <v>1739</v>
+      </c>
+      <c r="I1087" s="0" t="s">
+        <v>1513</v>
+      </c>
+      <c r="J1087" s="0" t="s">
+        <v>1741</v>
+      </c>
+      <c r="K1087" s="0" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="1088" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1089" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1090" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1091" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1091" s="0" t="s">
         <v>433</v>
       </c>
-      <c r="B1087" s="0" t="s">
+      <c r="B1091" s="0" t="s">
         <v>1478</v>
       </c>
-      <c r="C1087" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1087" s="0" t="s">
+      <c r="C1091" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1091" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="E1087" s="0" t="s">
+      <c r="E1091" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="F1087" s="0" t="s">
+      <c r="F1091" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="G1087" s="0" t="str">
+      <c r="G1091" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1087" s="0" t="s">
+      <c r="H1091" s="0" t="s">
         <v>1480</v>
       </c>
-      <c r="I1087" s="0" t="s">
+      <c r="I1091" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="J1087" s="0" t="s">
+      <c r="J1091" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="K1087" s="0" t="s">
+      <c r="K1091" s="0" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="1088" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1088" s="0" t="s">
+    <row r="1092" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1092" s="0" t="s">
         <v>912</v>
       </c>
-      <c r="B1088" s="0" t="s">
+      <c r="B1092" s="0" t="s">
         <v>1478</v>
       </c>
-      <c r="C1088" s="0" t="s">
+      <c r="C1092" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D1088" s="0" t="s">
+      <c r="D1092" s="0" t="s">
         <v>911</v>
       </c>
-      <c r="E1088" s="0" t="s">
+      <c r="E1092" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="F1088" s="0" t="s">
+      <c r="F1092" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="G1088" s="0" t="str">
+      <c r="G1092" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1088" s="0" t="s">
+      <c r="H1092" s="0" t="s">
         <v>1480</v>
       </c>
-      <c r="I1088" s="0" t="s">
+      <c r="I1092" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="J1088" s="0" t="s">
+      <c r="J1092" s="0" t="s">
         <v>1479</v>
       </c>
-      <c r="K1088" s="0" t="s">
+      <c r="K1092" s="0" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="1090" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1090" s="3" t="s">
+    <row r="1094" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1094" s="3" t="s">
         <v>1021</v>
       </c>
-      <c r="B1090" s="3" t="s">
-        <v>1737</v>
-      </c>
-      <c r="C1090" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1090" s="3" t="s">
+      <c r="B1094" s="3" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C1094" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1094" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E1090" s="3" t="s">
-        <v>1738</v>
-      </c>
-      <c r="F1090" s="3" t="s">
+      <c r="E1094" s="3" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F1094" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G1090" s="3" t="str">
+      <c r="G1094" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a796-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H1090" s="0" t="s">
+      <c r="H1094" s="0" t="s">
         <v>1727</v>
       </c>
-      <c r="I1090" s="0" t="s">
-        <v>1739</v>
-      </c>
-      <c r="J1090" s="3" t="s">
-        <v>1740</v>
-      </c>
-      <c r="K1090" s="3" t="s">
+      <c r="I1094" s="0" t="s">
+        <v>1744</v>
+      </c>
+      <c r="J1094" s="3" t="s">
+        <v>1745</v>
+      </c>
+      <c r="K1094" s="3" t="s">
         <v>1031</v>
       </c>
     </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Move CF3hr phalf to the ignored list #452, #450.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="B642" authorId="0">
+    <comment ref="B643" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5862" uniqueCount="1755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5872" uniqueCount="1755">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -5438,8 +5438,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A553" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A565" activeCellId="0" sqref="A565"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A546" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A565" activeCellId="0" sqref="565:565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23897,40 +23897,40 @@
         <v>741</v>
       </c>
     </row>
-    <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A567" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="B567" s="0" t="s">
-        <v>1495</v>
-      </c>
-      <c r="C567" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D567" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="E567" s="0" t="s">
-        <v>1496</v>
-      </c>
-      <c r="F567" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G567" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e0ecf1c1305c1bdc69bee0e7ba1e2e03.html","web")</f>
+    <row r="565" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A565" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B565" s="3" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C565" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D565" s="3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="E565" s="3" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F565" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G565" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154ab10964742eaff37de9cc5beef39c.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H567" s="0" t="s">
-        <v>1497</v>
-      </c>
-      <c r="I567" s="0" t="s">
+      <c r="H565" s="3" t="s">
+        <v>1492</v>
+      </c>
+      <c r="I565" s="3" t="s">
         <v>1493</v>
       </c>
-      <c r="J567" s="0" t="s">
-        <v>1498</v>
-      </c>
-      <c r="K567" s="0" t="s">
-        <v>305</v>
+      <c r="J565" s="3" t="s">
+        <v>1494</v>
+      </c>
+      <c r="K565" s="3" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23938,7 +23938,7 @@
         <v>303</v>
       </c>
       <c r="B568" s="0" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
       <c r="C568" s="0" t="s">
         <v>31</v>
@@ -23947,23 +23947,23 @@
         <v>312</v>
       </c>
       <c r="E568" s="0" t="s">
-        <v>1500</v>
+        <v>1496</v>
       </c>
       <c r="F568" s="0" t="s">
-        <v>1102</v>
+        <v>16</v>
       </c>
       <c r="G568" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b2b3318a73839edfafa9d46864aadc.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e0ecf1c1305c1bdc69bee0e7ba1e2e03.html","web")</f>
         <v>web</v>
       </c>
       <c r="H568" s="0" t="s">
-        <v>1501</v>
+        <v>1497</v>
       </c>
       <c r="I568" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J568" s="0" t="s">
-        <v>1502</v>
+        <v>1498</v>
       </c>
       <c r="K568" s="0" t="s">
         <v>305</v>
@@ -23974,7 +23974,7 @@
         <v>303</v>
       </c>
       <c r="B569" s="0" t="s">
-        <v>1503</v>
+        <v>1499</v>
       </c>
       <c r="C569" s="0" t="s">
         <v>31</v>
@@ -23983,23 +23983,23 @@
         <v>312</v>
       </c>
       <c r="E569" s="0" t="s">
-        <v>1504</v>
+        <v>1500</v>
       </c>
       <c r="F569" s="0" t="s">
         <v>1102</v>
       </c>
       <c r="G569" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/dd916e3e2eca18cda5d9f81749d0c91c.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b2b3318a73839edfafa9d46864aadc.html","web")</f>
         <v>web</v>
       </c>
       <c r="H569" s="0" t="s">
-        <v>1505</v>
+        <v>1501</v>
       </c>
       <c r="I569" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J569" s="0" t="s">
-        <v>1506</v>
+        <v>1502</v>
       </c>
       <c r="K569" s="0" t="s">
         <v>305</v>
@@ -24010,7 +24010,7 @@
         <v>303</v>
       </c>
       <c r="B570" s="0" t="s">
-        <v>1507</v>
+        <v>1503</v>
       </c>
       <c r="C570" s="0" t="s">
         <v>31</v>
@@ -24019,23 +24019,23 @@
         <v>312</v>
       </c>
       <c r="E570" s="0" t="s">
-        <v>1508</v>
+        <v>1504</v>
       </c>
       <c r="F570" s="0" t="s">
-        <v>841</v>
+        <v>1102</v>
       </c>
       <c r="G570" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b9c3eb96337c69c1c4a5aab1317f5563.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/dd916e3e2eca18cda5d9f81749d0c91c.html","web")</f>
         <v>web</v>
       </c>
       <c r="H570" s="0" t="s">
-        <v>1509</v>
+        <v>1505</v>
       </c>
       <c r="I570" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J570" s="0" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="K570" s="0" t="s">
         <v>305</v>
@@ -24046,7 +24046,7 @@
         <v>303</v>
       </c>
       <c r="B571" s="0" t="s">
-        <v>1510</v>
+        <v>1507</v>
       </c>
       <c r="C571" s="0" t="s">
         <v>31</v>
@@ -24055,23 +24055,23 @@
         <v>312</v>
       </c>
       <c r="E571" s="0" t="s">
-        <v>1511</v>
+        <v>1508</v>
       </c>
       <c r="F571" s="0" t="s">
-        <v>283</v>
+        <v>841</v>
       </c>
       <c r="G571" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/21db90c0a12448299f855fdab60930d4.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b9c3eb96337c69c1c4a5aab1317f5563.html","web")</f>
         <v>web</v>
       </c>
       <c r="H571" s="0" t="s">
-        <v>1512</v>
+        <v>1509</v>
       </c>
       <c r="I571" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J571" s="0" t="s">
-        <v>1513</v>
+        <v>1508</v>
       </c>
       <c r="K571" s="0" t="s">
         <v>305</v>
@@ -24082,7 +24082,7 @@
         <v>303</v>
       </c>
       <c r="B572" s="0" t="s">
-        <v>1514</v>
+        <v>1510</v>
       </c>
       <c r="C572" s="0" t="s">
         <v>31</v>
@@ -24091,23 +24091,23 @@
         <v>312</v>
       </c>
       <c r="E572" s="0" t="s">
-        <v>1515</v>
+        <v>1511</v>
       </c>
       <c r="F572" s="0" t="s">
         <v>283</v>
       </c>
       <c r="G572" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2dedcb347c18e132a2f4d625abf94585.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/21db90c0a12448299f855fdab60930d4.html","web")</f>
         <v>web</v>
       </c>
       <c r="H572" s="0" t="s">
-        <v>1516</v>
+        <v>1512</v>
       </c>
       <c r="I572" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J572" s="0" t="s">
-        <v>1517</v>
+        <v>1513</v>
       </c>
       <c r="K572" s="0" t="s">
         <v>305</v>
@@ -24118,7 +24118,7 @@
         <v>303</v>
       </c>
       <c r="B573" s="0" t="s">
-        <v>1518</v>
+        <v>1514</v>
       </c>
       <c r="C573" s="0" t="s">
         <v>31</v>
@@ -24127,23 +24127,23 @@
         <v>312</v>
       </c>
       <c r="E573" s="0" t="s">
-        <v>1519</v>
+        <v>1515</v>
       </c>
       <c r="F573" s="0" t="s">
-        <v>31</v>
+        <v>283</v>
       </c>
       <c r="G573" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53f4724d228998d54191c73352532ce3.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2dedcb347c18e132a2f4d625abf94585.html","web")</f>
         <v>web</v>
       </c>
       <c r="H573" s="0" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
       <c r="I573" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J573" s="0" t="s">
-        <v>1521</v>
+        <v>1517</v>
       </c>
       <c r="K573" s="0" t="s">
         <v>305</v>
@@ -24154,7 +24154,7 @@
         <v>303</v>
       </c>
       <c r="B574" s="0" t="s">
-        <v>1522</v>
+        <v>1518</v>
       </c>
       <c r="C574" s="0" t="s">
         <v>31</v>
@@ -24163,23 +24163,23 @@
         <v>312</v>
       </c>
       <c r="E574" s="0" t="s">
-        <v>1523</v>
+        <v>1519</v>
       </c>
       <c r="F574" s="0" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G574" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3cc6766c2d001a58d18dfe7f60fd5e66.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/53f4724d228998d54191c73352532ce3.html","web")</f>
         <v>web</v>
       </c>
       <c r="H574" s="0" t="s">
-        <v>1524</v>
+        <v>1520</v>
       </c>
       <c r="I574" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J574" s="0" t="s">
-        <v>975</v>
+        <v>1521</v>
       </c>
       <c r="K574" s="0" t="s">
         <v>305</v>
@@ -24190,7 +24190,7 @@
         <v>303</v>
       </c>
       <c r="B575" s="0" t="s">
-        <v>1525</v>
+        <v>1522</v>
       </c>
       <c r="C575" s="0" t="s">
         <v>31</v>
@@ -24199,23 +24199,23 @@
         <v>312</v>
       </c>
       <c r="E575" s="0" t="s">
-        <v>1526</v>
+        <v>1523</v>
       </c>
       <c r="F575" s="0" t="s">
-        <v>1527</v>
+        <v>16</v>
       </c>
       <c r="G575" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51fb29dd55442361fa9c5dbe23aca9c6.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3cc6766c2d001a58d18dfe7f60fd5e66.html","web")</f>
         <v>web</v>
       </c>
       <c r="H575" s="0" t="s">
-        <v>1528</v>
+        <v>1524</v>
       </c>
       <c r="I575" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J575" s="0" t="s">
-        <v>1529</v>
+        <v>975</v>
       </c>
       <c r="K575" s="0" t="s">
         <v>305</v>
@@ -24226,7 +24226,7 @@
         <v>303</v>
       </c>
       <c r="B576" s="0" t="s">
-        <v>1530</v>
+        <v>1525</v>
       </c>
       <c r="C576" s="0" t="s">
         <v>31</v>
@@ -24235,23 +24235,23 @@
         <v>312</v>
       </c>
       <c r="E576" s="0" t="s">
-        <v>1531</v>
+        <v>1526</v>
       </c>
       <c r="F576" s="0" t="s">
-        <v>24</v>
+        <v>1527</v>
       </c>
       <c r="G576" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/28e774ec0ecd561a6a3d437e6c443a6b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/51fb29dd55442361fa9c5dbe23aca9c6.html","web")</f>
         <v>web</v>
       </c>
       <c r="H576" s="0" t="s">
-        <v>1532</v>
+        <v>1528</v>
       </c>
       <c r="I576" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J576" s="0" t="s">
-        <v>1533</v>
+        <v>1529</v>
       </c>
       <c r="K576" s="0" t="s">
         <v>305</v>
@@ -24262,7 +24262,7 @@
         <v>303</v>
       </c>
       <c r="B577" s="0" t="s">
-        <v>1534</v>
+        <v>1530</v>
       </c>
       <c r="C577" s="0" t="s">
         <v>31</v>
@@ -24271,23 +24271,23 @@
         <v>312</v>
       </c>
       <c r="E577" s="0" t="s">
-        <v>1535</v>
+        <v>1531</v>
       </c>
       <c r="F577" s="0" t="s">
-        <v>219</v>
+        <v>24</v>
       </c>
       <c r="G577" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7a107875bd58c5e655e8f87152a3bad7.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/28e774ec0ecd561a6a3d437e6c443a6b.html","web")</f>
         <v>web</v>
       </c>
       <c r="H577" s="0" t="s">
-        <v>1536</v>
+        <v>1532</v>
       </c>
       <c r="I577" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J577" s="0" t="s">
-        <v>1537</v>
+        <v>1533</v>
       </c>
       <c r="K577" s="0" t="s">
         <v>305</v>
@@ -24298,32 +24298,32 @@
         <v>303</v>
       </c>
       <c r="B578" s="0" t="s">
-        <v>1489</v>
+        <v>1534</v>
       </c>
       <c r="C578" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D578" s="0" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="E578" s="0" t="s">
-        <v>1491</v>
+        <v>1535</v>
       </c>
       <c r="F578" s="0" t="s">
         <v>219</v>
       </c>
       <c r="G578" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154ab10964742eaff37de9cc5beef39c.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7a107875bd58c5e655e8f87152a3bad7.html","web")</f>
         <v>web</v>
       </c>
       <c r="H578" s="0" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="I578" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J578" s="0" t="s">
-        <v>1494</v>
+        <v>1537</v>
       </c>
       <c r="K578" s="0" t="s">
         <v>305</v>
@@ -24334,32 +24334,32 @@
         <v>303</v>
       </c>
       <c r="B579" s="0" t="s">
-        <v>1539</v>
+        <v>1489</v>
       </c>
       <c r="C579" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D579" s="0" t="s">
-        <v>1540</v>
+        <v>324</v>
       </c>
       <c r="E579" s="0" t="s">
-        <v>1541</v>
+        <v>1491</v>
       </c>
       <c r="F579" s="0" t="s">
-        <v>841</v>
+        <v>219</v>
       </c>
       <c r="G579" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5c4978e802ba55d5a298cf1b3bdc2b3a.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/154ab10964742eaff37de9cc5beef39c.html","web")</f>
         <v>web</v>
       </c>
       <c r="H579" s="0" t="s">
-        <v>1542</v>
+        <v>1538</v>
       </c>
       <c r="I579" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J579" s="0" t="s">
-        <v>1543</v>
+        <v>1494</v>
       </c>
       <c r="K579" s="0" t="s">
         <v>305</v>
@@ -24370,32 +24370,32 @@
         <v>303</v>
       </c>
       <c r="B580" s="0" t="s">
-        <v>1544</v>
+        <v>1539</v>
       </c>
       <c r="C580" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D580" s="0" t="s">
-        <v>304</v>
+        <v>1540</v>
       </c>
       <c r="E580" s="0" t="s">
-        <v>1545</v>
+        <v>1541</v>
       </c>
       <c r="F580" s="0" t="s">
         <v>841</v>
       </c>
       <c r="G580" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90c49fce92dc1f21647dad07d1342843.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5c4978e802ba55d5a298cf1b3bdc2b3a.html","web")</f>
         <v>web</v>
       </c>
       <c r="H580" s="0" t="s">
-        <v>1546</v>
+        <v>1542</v>
       </c>
       <c r="I580" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J580" s="0" t="s">
-        <v>1547</v>
+        <v>1543</v>
       </c>
       <c r="K580" s="0" t="s">
         <v>305</v>
@@ -24406,7 +24406,7 @@
         <v>303</v>
       </c>
       <c r="B581" s="0" t="s">
-        <v>1548</v>
+        <v>1544</v>
       </c>
       <c r="C581" s="0" t="s">
         <v>31</v>
@@ -24415,23 +24415,23 @@
         <v>304</v>
       </c>
       <c r="E581" s="0" t="s">
-        <v>1549</v>
+        <v>1545</v>
       </c>
       <c r="F581" s="0" t="s">
-        <v>219</v>
+        <v>841</v>
       </c>
       <c r="G581" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3d23c359f44d6a153c4dcab9e07d7cb6.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90c49fce92dc1f21647dad07d1342843.html","web")</f>
         <v>web</v>
       </c>
       <c r="H581" s="0" t="s">
-        <v>1550</v>
+        <v>1546</v>
       </c>
       <c r="I581" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J581" s="0" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="K581" s="0" t="s">
         <v>305</v>
@@ -24442,7 +24442,7 @@
         <v>303</v>
       </c>
       <c r="B582" s="0" t="s">
-        <v>1551</v>
+        <v>1548</v>
       </c>
       <c r="C582" s="0" t="s">
         <v>31</v>
@@ -24451,23 +24451,23 @@
         <v>304</v>
       </c>
       <c r="E582" s="0" t="s">
-        <v>1552</v>
+        <v>1549</v>
       </c>
       <c r="F582" s="0" t="s">
         <v>219</v>
       </c>
       <c r="G582" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8c9504d28596e05586c8e193082ac617.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3d23c359f44d6a153c4dcab9e07d7cb6.html","web")</f>
         <v>web</v>
       </c>
       <c r="H582" s="0" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="I582" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J582" s="0" t="s">
-        <v>1554</v>
+        <v>1549</v>
       </c>
       <c r="K582" s="0" t="s">
         <v>305</v>
@@ -24478,32 +24478,32 @@
         <v>303</v>
       </c>
       <c r="B583" s="0" t="s">
-        <v>1555</v>
+        <v>1551</v>
       </c>
       <c r="C583" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D583" s="0" t="s">
-        <v>1556</v>
+        <v>304</v>
       </c>
       <c r="E583" s="0" t="s">
-        <v>1557</v>
+        <v>1552</v>
       </c>
       <c r="F583" s="0" t="s">
-        <v>283</v>
+        <v>219</v>
       </c>
       <c r="G583" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e72b243a2a1c8691ab0168d8b62534c2.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/8c9504d28596e05586c8e193082ac617.html","web")</f>
         <v>web</v>
       </c>
       <c r="H583" s="0" t="s">
-        <v>1558</v>
+        <v>1553</v>
       </c>
       <c r="I583" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J583" s="0" t="s">
-        <v>1559</v>
+        <v>1554</v>
       </c>
       <c r="K583" s="0" t="s">
         <v>305</v>
@@ -24514,7 +24514,7 @@
         <v>303</v>
       </c>
       <c r="B584" s="0" t="s">
-        <v>1560</v>
+        <v>1555</v>
       </c>
       <c r="C584" s="0" t="s">
         <v>31</v>
@@ -24523,23 +24523,23 @@
         <v>1556</v>
       </c>
       <c r="E584" s="0" t="s">
-        <v>1561</v>
+        <v>1557</v>
       </c>
       <c r="F584" s="0" t="s">
         <v>283</v>
       </c>
       <c r="G584" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b1cd51f370e346ecb20f1e80cb6ea4.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/e72b243a2a1c8691ab0168d8b62534c2.html","web")</f>
         <v>web</v>
       </c>
       <c r="H584" s="0" t="s">
-        <v>1562</v>
+        <v>1558</v>
       </c>
       <c r="I584" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J584" s="0" t="s">
-        <v>1563</v>
+        <v>1559</v>
       </c>
       <c r="K584" s="0" t="s">
         <v>305</v>
@@ -24550,7 +24550,7 @@
         <v>303</v>
       </c>
       <c r="B585" s="0" t="s">
-        <v>1564</v>
+        <v>1560</v>
       </c>
       <c r="C585" s="0" t="s">
         <v>31</v>
@@ -24559,23 +24559,23 @@
         <v>1556</v>
       </c>
       <c r="E585" s="0" t="s">
-        <v>1565</v>
+        <v>1561</v>
       </c>
       <c r="F585" s="0" t="s">
         <v>283</v>
       </c>
       <c r="G585" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4b97609a32d53dff5b8e73729e4f258b.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/86b1cd51f370e346ecb20f1e80cb6ea4.html","web")</f>
         <v>web</v>
       </c>
       <c r="H585" s="0" t="s">
-        <v>1566</v>
+        <v>1562</v>
       </c>
       <c r="I585" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J585" s="0" t="s">
-        <v>1567</v>
+        <v>1563</v>
       </c>
       <c r="K585" s="0" t="s">
         <v>305</v>
@@ -24586,32 +24586,32 @@
         <v>303</v>
       </c>
       <c r="B586" s="0" t="s">
-        <v>1568</v>
+        <v>1564</v>
       </c>
       <c r="C586" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D586" s="0" t="s">
-        <v>1540</v>
+        <v>1556</v>
       </c>
       <c r="E586" s="0" t="s">
-        <v>1569</v>
+        <v>1565</v>
       </c>
       <c r="F586" s="0" t="s">
-        <v>16</v>
+        <v>283</v>
       </c>
       <c r="G586" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c75f684ec69602e9de82b48e53afb2cc.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/4b97609a32d53dff5b8e73729e4f258b.html","web")</f>
         <v>web</v>
       </c>
       <c r="H586" s="0" t="s">
-        <v>1570</v>
+        <v>1566</v>
       </c>
       <c r="I586" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J586" s="0" t="s">
-        <v>975</v>
+        <v>1567</v>
       </c>
       <c r="K586" s="0" t="s">
         <v>305</v>
@@ -24622,7 +24622,7 @@
         <v>303</v>
       </c>
       <c r="B587" s="0" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="C587" s="0" t="s">
         <v>31</v>
@@ -24631,23 +24631,23 @@
         <v>1540</v>
       </c>
       <c r="E587" s="0" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
       <c r="F587" s="0" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G587" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ebfefc2ab8716ef597b128171b275945.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c75f684ec69602e9de82b48e53afb2cc.html","web")</f>
         <v>web</v>
       </c>
       <c r="H587" s="0" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
       <c r="I587" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J587" s="0" t="s">
-        <v>1574</v>
+        <v>975</v>
       </c>
       <c r="K587" s="0" t="s">
         <v>305</v>
@@ -24658,32 +24658,32 @@
         <v>303</v>
       </c>
       <c r="B588" s="0" t="s">
-        <v>1575</v>
+        <v>1571</v>
       </c>
       <c r="C588" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D588" s="0" t="s">
-        <v>304</v>
+        <v>1540</v>
       </c>
       <c r="E588" s="0" t="s">
-        <v>1576</v>
+        <v>1572</v>
       </c>
       <c r="F588" s="0" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
       <c r="G588" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/62f26742cf240c1b5169a5cd511196b6.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/ebfefc2ab8716ef597b128171b275945.html","web")</f>
         <v>web</v>
       </c>
       <c r="H588" s="0" t="s">
-        <v>1577</v>
+        <v>1573</v>
       </c>
       <c r="I588" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J588" s="0" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="K588" s="0" t="s">
         <v>305</v>
@@ -24694,7 +24694,7 @@
         <v>303</v>
       </c>
       <c r="B589" s="0" t="s">
-        <v>1579</v>
+        <v>1575</v>
       </c>
       <c r="C589" s="0" t="s">
         <v>31</v>
@@ -24703,23 +24703,23 @@
         <v>304</v>
       </c>
       <c r="E589" s="0" t="s">
-        <v>1580</v>
+        <v>1576</v>
       </c>
       <c r="F589" s="0" t="s">
         <v>137</v>
       </c>
       <c r="G589" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/051919eddec810e292c883205c944ceb.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/62f26742cf240c1b5169a5cd511196b6.html","web")</f>
         <v>web</v>
       </c>
       <c r="H589" s="0" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="I589" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J589" s="0" t="s">
-        <v>1582</v>
+        <v>1578</v>
       </c>
       <c r="K589" s="0" t="s">
         <v>305</v>
@@ -24730,7 +24730,7 @@
         <v>303</v>
       </c>
       <c r="B590" s="0" t="s">
-        <v>1583</v>
+        <v>1579</v>
       </c>
       <c r="C590" s="0" t="s">
         <v>31</v>
@@ -24739,23 +24739,23 @@
         <v>304</v>
       </c>
       <c r="E590" s="0" t="s">
-        <v>1584</v>
+        <v>1580</v>
       </c>
       <c r="F590" s="0" t="s">
         <v>137</v>
       </c>
       <c r="G590" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/aa2bea81f238ad8f2c35a7e16ad97801.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/051919eddec810e292c883205c944ceb.html","web")</f>
         <v>web</v>
       </c>
       <c r="H590" s="0" t="s">
-        <v>1585</v>
+        <v>1581</v>
       </c>
       <c r="I590" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J590" s="0" t="s">
-        <v>1586</v>
+        <v>1582</v>
       </c>
       <c r="K590" s="0" t="s">
         <v>305</v>
@@ -24766,7 +24766,7 @@
         <v>303</v>
       </c>
       <c r="B591" s="0" t="s">
-        <v>1587</v>
+        <v>1583</v>
       </c>
       <c r="C591" s="0" t="s">
         <v>31</v>
@@ -24775,23 +24775,23 @@
         <v>304</v>
       </c>
       <c r="E591" s="0" t="s">
-        <v>1588</v>
+        <v>1584</v>
       </c>
       <c r="F591" s="0" t="s">
         <v>137</v>
       </c>
       <c r="G591" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/089961a3af4d54d5fb045cf3750e760c.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/aa2bea81f238ad8f2c35a7e16ad97801.html","web")</f>
         <v>web</v>
       </c>
       <c r="H591" s="0" t="s">
-        <v>1589</v>
+        <v>1585</v>
       </c>
       <c r="I591" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J591" s="0" t="s">
-        <v>1590</v>
+        <v>1586</v>
       </c>
       <c r="K591" s="0" t="s">
         <v>305</v>
@@ -24802,7 +24802,7 @@
         <v>303</v>
       </c>
       <c r="B592" s="0" t="s">
-        <v>1591</v>
+        <v>1587</v>
       </c>
       <c r="C592" s="0" t="s">
         <v>31</v>
@@ -24811,23 +24811,23 @@
         <v>304</v>
       </c>
       <c r="E592" s="0" t="s">
-        <v>1592</v>
+        <v>1588</v>
       </c>
       <c r="F592" s="0" t="s">
         <v>137</v>
       </c>
       <c r="G592" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3a8e1636a31c82fbdd9a1ae45ab3be7d.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/089961a3af4d54d5fb045cf3750e760c.html","web")</f>
         <v>web</v>
       </c>
       <c r="H592" s="0" t="s">
-        <v>1593</v>
+        <v>1589</v>
       </c>
       <c r="I592" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J592" s="0" t="s">
-        <v>1594</v>
+        <v>1590</v>
       </c>
       <c r="K592" s="0" t="s">
         <v>305</v>
@@ -24838,7 +24838,7 @@
         <v>303</v>
       </c>
       <c r="B593" s="0" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="C593" s="0" t="s">
         <v>31</v>
@@ -24847,23 +24847,23 @@
         <v>304</v>
       </c>
       <c r="E593" s="0" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="F593" s="0" t="s">
-        <v>219</v>
+        <v>137</v>
       </c>
       <c r="G593" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3abb7c5b4c4650e9d17a8439004aebea.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3a8e1636a31c82fbdd9a1ae45ab3be7d.html","web")</f>
         <v>web</v>
       </c>
       <c r="H593" s="0" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="I593" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J593" s="0" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="K593" s="0" t="s">
         <v>305</v>
@@ -24874,7 +24874,7 @@
         <v>303</v>
       </c>
       <c r="B594" s="0" t="s">
-        <v>1599</v>
+        <v>1595</v>
       </c>
       <c r="C594" s="0" t="s">
         <v>31</v>
@@ -24883,23 +24883,23 @@
         <v>304</v>
       </c>
       <c r="E594" s="0" t="s">
-        <v>1600</v>
+        <v>1596</v>
       </c>
       <c r="F594" s="0" t="s">
         <v>219</v>
       </c>
       <c r="G594" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bd10cebbde1593b65e5220911f9a997c.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/3abb7c5b4c4650e9d17a8439004aebea.html","web")</f>
         <v>web</v>
       </c>
       <c r="H594" s="0" t="s">
-        <v>1601</v>
+        <v>1597</v>
       </c>
       <c r="I594" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J594" s="0" t="s">
-        <v>1602</v>
+        <v>1598</v>
       </c>
       <c r="K594" s="0" t="s">
         <v>305</v>
@@ -24910,7 +24910,7 @@
         <v>303</v>
       </c>
       <c r="B595" s="0" t="s">
-        <v>1603</v>
+        <v>1599</v>
       </c>
       <c r="C595" s="0" t="s">
         <v>31</v>
@@ -24919,23 +24919,23 @@
         <v>304</v>
       </c>
       <c r="E595" s="0" t="s">
-        <v>1604</v>
+        <v>1600</v>
       </c>
       <c r="F595" s="0" t="s">
-        <v>327</v>
+        <v>219</v>
       </c>
       <c r="G595" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/95cbf6ac889c8fe7d92e20e8c34960d1.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/bd10cebbde1593b65e5220911f9a997c.html","web")</f>
         <v>web</v>
       </c>
       <c r="H595" s="0" t="s">
-        <v>1605</v>
+        <v>1601</v>
       </c>
       <c r="I595" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J595" s="0" t="s">
-        <v>1162</v>
+        <v>1602</v>
       </c>
       <c r="K595" s="0" t="s">
         <v>305</v>
@@ -24946,7 +24946,7 @@
         <v>303</v>
       </c>
       <c r="B596" s="0" t="s">
-        <v>1606</v>
+        <v>1603</v>
       </c>
       <c r="C596" s="0" t="s">
         <v>31</v>
@@ -24955,23 +24955,23 @@
         <v>304</v>
       </c>
       <c r="E596" s="0" t="s">
-        <v>1607</v>
+        <v>1604</v>
       </c>
       <c r="F596" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G596" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a13ed886b17e20cdae8b89b9ff8e4610.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/95cbf6ac889c8fe7d92e20e8c34960d1.html","web")</f>
         <v>web</v>
       </c>
       <c r="H596" s="0" t="s">
-        <v>1608</v>
+        <v>1605</v>
       </c>
       <c r="I596" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J596" s="0" t="s">
-        <v>1609</v>
+        <v>1162</v>
       </c>
       <c r="K596" s="0" t="s">
         <v>305</v>
@@ -24982,7 +24982,7 @@
         <v>303</v>
       </c>
       <c r="B597" s="0" t="s">
-        <v>1610</v>
+        <v>1606</v>
       </c>
       <c r="C597" s="0" t="s">
         <v>31</v>
@@ -24991,23 +24991,23 @@
         <v>304</v>
       </c>
       <c r="E597" s="0" t="s">
-        <v>1611</v>
+        <v>1607</v>
       </c>
       <c r="F597" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G597" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70d7d6fc0e9c2f14624a0270bf2b99b9.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a13ed886b17e20cdae8b89b9ff8e4610.html","web")</f>
         <v>web</v>
       </c>
       <c r="H597" s="0" t="s">
-        <v>1612</v>
+        <v>1608</v>
       </c>
       <c r="I597" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J597" s="0" t="s">
-        <v>1613</v>
+        <v>1609</v>
       </c>
       <c r="K597" s="0" t="s">
         <v>305</v>
@@ -25018,7 +25018,7 @@
         <v>303</v>
       </c>
       <c r="B598" s="0" t="s">
-        <v>1614</v>
+        <v>1610</v>
       </c>
       <c r="C598" s="0" t="s">
         <v>31</v>
@@ -25027,23 +25027,23 @@
         <v>304</v>
       </c>
       <c r="E598" s="0" t="s">
-        <v>1615</v>
+        <v>1611</v>
       </c>
       <c r="F598" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G598" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/89027ee0079acb709750ddeac1c08899.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70d7d6fc0e9c2f14624a0270bf2b99b9.html","web")</f>
         <v>web</v>
       </c>
       <c r="H598" s="0" t="s">
-        <v>1616</v>
+        <v>1612</v>
       </c>
       <c r="I598" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J598" s="0" t="s">
-        <v>1271</v>
+        <v>1613</v>
       </c>
       <c r="K598" s="0" t="s">
         <v>305</v>
@@ -25054,7 +25054,7 @@
         <v>303</v>
       </c>
       <c r="B599" s="0" t="s">
-        <v>1617</v>
+        <v>1614</v>
       </c>
       <c r="C599" s="0" t="s">
         <v>31</v>
@@ -25063,23 +25063,23 @@
         <v>304</v>
       </c>
       <c r="E599" s="0" t="s">
-        <v>1618</v>
+        <v>1615</v>
       </c>
       <c r="F599" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G599" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e7b9f984d3bba15daccaaa18039a85d.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/89027ee0079acb709750ddeac1c08899.html","web")</f>
         <v>web</v>
       </c>
       <c r="H599" s="0" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="I599" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J599" s="0" t="s">
-        <v>1620</v>
+        <v>1271</v>
       </c>
       <c r="K599" s="0" t="s">
         <v>305</v>
@@ -25090,7 +25090,7 @@
         <v>303</v>
       </c>
       <c r="B600" s="0" t="s">
-        <v>1621</v>
+        <v>1617</v>
       </c>
       <c r="C600" s="0" t="s">
         <v>31</v>
@@ -25099,23 +25099,23 @@
         <v>304</v>
       </c>
       <c r="E600" s="0" t="s">
-        <v>1622</v>
+        <v>1618</v>
       </c>
       <c r="F600" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G600" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70bf79db957daa3b82413da949233ac7.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/6e7b9f984d3bba15daccaaa18039a85d.html","web")</f>
         <v>web</v>
       </c>
       <c r="H600" s="0" t="s">
-        <v>1623</v>
+        <v>1619</v>
       </c>
       <c r="I600" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J600" s="0" t="s">
-        <v>1274</v>
+        <v>1620</v>
       </c>
       <c r="K600" s="0" t="s">
         <v>305</v>
@@ -25126,7 +25126,7 @@
         <v>303</v>
       </c>
       <c r="B601" s="0" t="s">
-        <v>1624</v>
+        <v>1621</v>
       </c>
       <c r="C601" s="0" t="s">
         <v>31</v>
@@ -25135,23 +25135,23 @@
         <v>304</v>
       </c>
       <c r="E601" s="0" t="s">
-        <v>1625</v>
+        <v>1622</v>
       </c>
       <c r="F601" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G601" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d0a35d5c99a0aa93ad4069cfe83bf748.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/70bf79db957daa3b82413da949233ac7.html","web")</f>
         <v>web</v>
       </c>
       <c r="H601" s="0" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
       <c r="I601" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J601" s="0" t="s">
-        <v>1627</v>
+        <v>1274</v>
       </c>
       <c r="K601" s="0" t="s">
         <v>305</v>
@@ -25162,7 +25162,7 @@
         <v>303</v>
       </c>
       <c r="B602" s="0" t="s">
-        <v>1628</v>
+        <v>1624</v>
       </c>
       <c r="C602" s="0" t="s">
         <v>31</v>
@@ -25171,23 +25171,23 @@
         <v>304</v>
       </c>
       <c r="E602" s="0" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
       <c r="F602" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G602" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e2.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/d0a35d5c99a0aa93ad4069cfe83bf748.html","web")</f>
         <v>web</v>
       </c>
       <c r="H602" s="0" t="s">
-        <v>1623</v>
+        <v>1626</v>
       </c>
       <c r="I602" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J602" s="0" t="s">
-        <v>1630</v>
+        <v>1627</v>
       </c>
       <c r="K602" s="0" t="s">
         <v>305</v>
@@ -25198,7 +25198,7 @@
         <v>303</v>
       </c>
       <c r="B603" s="0" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="C603" s="0" t="s">
         <v>31</v>
@@ -25207,23 +25207,23 @@
         <v>304</v>
       </c>
       <c r="E603" s="0" t="s">
-        <v>1632</v>
+        <v>1629</v>
       </c>
       <c r="F603" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G603" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7b2d1e1a3ece1169d8ac61af4b758ed2.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/90df05fe3dcd9fe0c9b48aaa74b5e9e2.html","web")</f>
         <v>web</v>
       </c>
       <c r="H603" s="0" t="s">
-        <v>1633</v>
+        <v>1623</v>
       </c>
       <c r="I603" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J603" s="0" t="s">
-        <v>1634</v>
+        <v>1630</v>
       </c>
       <c r="K603" s="0" t="s">
         <v>305</v>
@@ -25234,7 +25234,7 @@
         <v>303</v>
       </c>
       <c r="B604" s="0" t="s">
-        <v>1635</v>
+        <v>1631</v>
       </c>
       <c r="C604" s="0" t="s">
         <v>31</v>
@@ -25243,23 +25243,23 @@
         <v>304</v>
       </c>
       <c r="E604" s="0" t="s">
-        <v>1636</v>
+        <v>1632</v>
       </c>
       <c r="F604" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G604" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a21e250a10f96b1c1ad6d742206a157e.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7b2d1e1a3ece1169d8ac61af4b758ed2.html","web")</f>
         <v>web</v>
       </c>
       <c r="H604" s="0" t="s">
-        <v>1637</v>
+        <v>1633</v>
       </c>
       <c r="I604" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J604" s="0" t="s">
-        <v>1638</v>
+        <v>1634</v>
       </c>
       <c r="K604" s="0" t="s">
         <v>305</v>
@@ -25270,7 +25270,7 @@
         <v>303</v>
       </c>
       <c r="B605" s="0" t="s">
-        <v>1639</v>
+        <v>1635</v>
       </c>
       <c r="C605" s="0" t="s">
         <v>31</v>
@@ -25279,23 +25279,23 @@
         <v>304</v>
       </c>
       <c r="E605" s="0" t="s">
-        <v>1640</v>
+        <v>1636</v>
       </c>
       <c r="F605" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G605" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b907fef85d4c9571a9457ee1b259bb8f.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/a21e250a10f96b1c1ad6d742206a157e.html","web")</f>
         <v>web</v>
       </c>
       <c r="H605" s="0" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
       <c r="I605" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J605" s="0" t="s">
-        <v>1642</v>
+        <v>1638</v>
       </c>
       <c r="K605" s="0" t="s">
         <v>305</v>
@@ -25306,7 +25306,7 @@
         <v>303</v>
       </c>
       <c r="B606" s="0" t="s">
-        <v>1643</v>
+        <v>1639</v>
       </c>
       <c r="C606" s="0" t="s">
         <v>31</v>
@@ -25315,23 +25315,23 @@
         <v>304</v>
       </c>
       <c r="E606" s="0" t="s">
-        <v>1644</v>
+        <v>1640</v>
       </c>
       <c r="F606" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G606" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/63345d9732c72b97ca395f24ce2d6642.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/b907fef85d4c9571a9457ee1b259bb8f.html","web")</f>
         <v>web</v>
       </c>
       <c r="H606" s="0" t="s">
-        <v>1645</v>
+        <v>1641</v>
       </c>
       <c r="I606" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J606" s="0" t="s">
-        <v>1646</v>
+        <v>1642</v>
       </c>
       <c r="K606" s="0" t="s">
         <v>305</v>
@@ -25342,7 +25342,7 @@
         <v>303</v>
       </c>
       <c r="B607" s="0" t="s">
-        <v>1647</v>
+        <v>1643</v>
       </c>
       <c r="C607" s="0" t="s">
         <v>31</v>
@@ -25351,23 +25351,23 @@
         <v>304</v>
       </c>
       <c r="E607" s="0" t="s">
-        <v>1648</v>
+        <v>1644</v>
       </c>
       <c r="F607" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G607" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/921b8b8f6620826567d9324314c70410.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/63345d9732c72b97ca395f24ce2d6642.html","web")</f>
         <v>web</v>
       </c>
       <c r="H607" s="0" t="s">
-        <v>1649</v>
+        <v>1645</v>
       </c>
       <c r="I607" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J607" s="0" t="s">
-        <v>1650</v>
+        <v>1646</v>
       </c>
       <c r="K607" s="0" t="s">
         <v>305</v>
@@ -25378,7 +25378,7 @@
         <v>303</v>
       </c>
       <c r="B608" s="0" t="s">
-        <v>1651</v>
+        <v>1647</v>
       </c>
       <c r="C608" s="0" t="s">
         <v>31</v>
@@ -25387,23 +25387,23 @@
         <v>304</v>
       </c>
       <c r="E608" s="0" t="s">
-        <v>1652</v>
+        <v>1648</v>
       </c>
       <c r="F608" s="0" t="s">
         <v>327</v>
       </c>
       <c r="G608" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/12e0369ff0ba1a6f1a84e0d9565d4b07.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/921b8b8f6620826567d9324314c70410.html","web")</f>
         <v>web</v>
       </c>
       <c r="H608" s="0" t="s">
-        <v>1653</v>
+        <v>1649</v>
       </c>
       <c r="I608" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J608" s="0" t="s">
-        <v>1654</v>
+        <v>1650</v>
       </c>
       <c r="K608" s="0" t="s">
         <v>305</v>
@@ -25414,7 +25414,7 @@
         <v>303</v>
       </c>
       <c r="B609" s="0" t="s">
-        <v>1655</v>
+        <v>1651</v>
       </c>
       <c r="C609" s="0" t="s">
         <v>31</v>
@@ -25423,23 +25423,23 @@
         <v>304</v>
       </c>
       <c r="E609" s="0" t="s">
-        <v>1656</v>
+        <v>1652</v>
       </c>
       <c r="F609" s="0" t="s">
-        <v>967</v>
+        <v>327</v>
       </c>
       <c r="G609" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fc637f1c75e58be8a6e4112411a00f36.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/12e0369ff0ba1a6f1a84e0d9565d4b07.html","web")</f>
         <v>web</v>
       </c>
       <c r="H609" s="0" t="s">
-        <v>1657</v>
+        <v>1653</v>
       </c>
       <c r="I609" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J609" s="0" t="s">
-        <v>1658</v>
+        <v>1654</v>
       </c>
       <c r="K609" s="0" t="s">
         <v>305</v>
@@ -25450,7 +25450,7 @@
         <v>303</v>
       </c>
       <c r="B610" s="0" t="s">
-        <v>1659</v>
+        <v>1655</v>
       </c>
       <c r="C610" s="0" t="s">
         <v>31</v>
@@ -25459,23 +25459,23 @@
         <v>304</v>
       </c>
       <c r="E610" s="0" t="s">
-        <v>1660</v>
+        <v>1656</v>
       </c>
       <c r="F610" s="0" t="s">
-        <v>16</v>
+        <v>967</v>
       </c>
       <c r="G610" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7c2249d424dde72f8616d42870a9d425.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/fc637f1c75e58be8a6e4112411a00f36.html","web")</f>
         <v>web</v>
       </c>
       <c r="H610" s="0" t="s">
-        <v>1661</v>
+        <v>1657</v>
       </c>
       <c r="I610" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J610" s="0" t="s">
-        <v>1662</v>
+        <v>1658</v>
       </c>
       <c r="K610" s="0" t="s">
         <v>305</v>
@@ -25486,7 +25486,7 @@
         <v>303</v>
       </c>
       <c r="B611" s="0" t="s">
-        <v>1663</v>
+        <v>1659</v>
       </c>
       <c r="C611" s="0" t="s">
         <v>31</v>
@@ -25495,23 +25495,23 @@
         <v>304</v>
       </c>
       <c r="E611" s="0" t="s">
-        <v>1664</v>
+        <v>1660</v>
       </c>
       <c r="F611" s="0" t="s">
-        <v>967</v>
+        <v>16</v>
       </c>
       <c r="G611" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/80a1dd605b563e9f09c718a5ba9cb9cc.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/7c2249d424dde72f8616d42870a9d425.html","web")</f>
         <v>web</v>
       </c>
       <c r="H611" s="0" t="s">
-        <v>1665</v>
+        <v>1661</v>
       </c>
       <c r="I611" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J611" s="0" t="s">
-        <v>1666</v>
+        <v>1662</v>
       </c>
       <c r="K611" s="0" t="s">
         <v>305</v>
@@ -25522,7 +25522,7 @@
         <v>303</v>
       </c>
       <c r="B612" s="0" t="s">
-        <v>1667</v>
+        <v>1663</v>
       </c>
       <c r="C612" s="0" t="s">
         <v>31</v>
@@ -25531,23 +25531,23 @@
         <v>304</v>
       </c>
       <c r="E612" s="0" t="s">
-        <v>1668</v>
+        <v>1664</v>
       </c>
       <c r="F612" s="0" t="s">
         <v>967</v>
       </c>
       <c r="G612" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/73c496f5669cc122cf1cddfe4df2a27a.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/80a1dd605b563e9f09c718a5ba9cb9cc.html","web")</f>
         <v>web</v>
       </c>
       <c r="H612" s="0" t="s">
-        <v>1669</v>
+        <v>1665</v>
       </c>
       <c r="I612" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J612" s="0" t="s">
-        <v>1670</v>
+        <v>1666</v>
       </c>
       <c r="K612" s="0" t="s">
         <v>305</v>
@@ -25558,7 +25558,7 @@
         <v>303</v>
       </c>
       <c r="B613" s="0" t="s">
-        <v>1671</v>
+        <v>1667</v>
       </c>
       <c r="C613" s="0" t="s">
         <v>31</v>
@@ -25567,23 +25567,23 @@
         <v>304</v>
       </c>
       <c r="E613" s="0" t="s">
-        <v>1672</v>
+        <v>1668</v>
       </c>
       <c r="F613" s="0" t="s">
-        <v>327</v>
+        <v>967</v>
       </c>
       <c r="G613" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/26328c46dfcc65d454b6fd4c52ccb48f.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/73c496f5669cc122cf1cddfe4df2a27a.html","web")</f>
         <v>web</v>
       </c>
       <c r="H613" s="0" t="s">
-        <v>1673</v>
+        <v>1669</v>
       </c>
       <c r="I613" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J613" s="0" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
       <c r="K613" s="0" t="s">
         <v>305</v>
@@ -25594,7 +25594,7 @@
         <v>303</v>
       </c>
       <c r="B614" s="0" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="C614" s="0" t="s">
         <v>31</v>
@@ -25603,23 +25603,23 @@
         <v>304</v>
       </c>
       <c r="E614" s="0" t="s">
-        <v>1676</v>
+        <v>1672</v>
       </c>
       <c r="F614" s="0" t="s">
-        <v>137</v>
+        <v>327</v>
       </c>
       <c r="G614" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc1b9e3073d751143fe8ab63ca9fcc45.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/26328c46dfcc65d454b6fd4c52ccb48f.html","web")</f>
         <v>web</v>
       </c>
       <c r="H614" s="0" t="s">
-        <v>1677</v>
+        <v>1673</v>
       </c>
       <c r="I614" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J614" s="0" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
       <c r="K614" s="0" t="s">
         <v>305</v>
@@ -25630,7 +25630,7 @@
         <v>303</v>
       </c>
       <c r="B615" s="0" t="s">
-        <v>1679</v>
+        <v>1675</v>
       </c>
       <c r="C615" s="0" t="s">
         <v>31</v>
@@ -25639,23 +25639,23 @@
         <v>304</v>
       </c>
       <c r="E615" s="0" t="s">
-        <v>1680</v>
+        <v>1676</v>
       </c>
       <c r="F615" s="0" t="s">
         <v>137</v>
       </c>
       <c r="G615" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/299fb9d19040c4aa3862644286261ad2.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/cc1b9e3073d751143fe8ab63ca9fcc45.html","web")</f>
         <v>web</v>
       </c>
       <c r="H615" s="0" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
       <c r="I615" s="0" t="s">
         <v>1493</v>
       </c>
       <c r="J615" s="0" t="s">
-        <v>1682</v>
+        <v>1678</v>
       </c>
       <c r="K615" s="0" t="s">
         <v>305</v>
@@ -25666,31 +25666,32 @@
         <v>303</v>
       </c>
       <c r="B616" s="0" t="s">
-        <v>1683</v>
+        <v>1679</v>
       </c>
       <c r="C616" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D616" s="0" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="E616" s="0" t="s">
-        <v>1684</v>
+        <v>1680</v>
       </c>
       <c r="F616" s="0" t="s">
-        <v>357</v>
-      </c>
-      <c r="G616" s="0" t="n">
-        <v>0</v>
+        <v>137</v>
+      </c>
+      <c r="G616" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/299fb9d19040c4aa3862644286261ad2.html","web")</f>
+        <v>web</v>
       </c>
       <c r="H616" s="0" t="s">
-        <v>1685</v>
+        <v>1681</v>
       </c>
       <c r="I616" s="0" t="s">
-        <v>359</v>
+        <v>1493</v>
       </c>
       <c r="J616" s="0" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="K616" s="0" t="s">
         <v>305</v>
@@ -25701,7 +25702,7 @@
         <v>303</v>
       </c>
       <c r="B617" s="0" t="s">
-        <v>1686</v>
+        <v>1683</v>
       </c>
       <c r="C617" s="0" t="s">
         <v>31</v>
@@ -25710,7 +25711,7 @@
         <v>312</v>
       </c>
       <c r="E617" s="0" t="s">
-        <v>1687</v>
+        <v>1684</v>
       </c>
       <c r="F617" s="0" t="s">
         <v>357</v>
@@ -25719,13 +25720,13 @@
         <v>0</v>
       </c>
       <c r="H617" s="0" t="s">
-        <v>1688</v>
+        <v>1685</v>
       </c>
       <c r="I617" s="0" t="s">
         <v>359</v>
       </c>
       <c r="J617" s="0" t="s">
-        <v>1689</v>
+        <v>1684</v>
       </c>
       <c r="K617" s="0" t="s">
         <v>305</v>
@@ -25736,7 +25737,7 @@
         <v>303</v>
       </c>
       <c r="B618" s="0" t="s">
-        <v>1690</v>
+        <v>1686</v>
       </c>
       <c r="C618" s="0" t="s">
         <v>31</v>
@@ -25745,7 +25746,7 @@
         <v>312</v>
       </c>
       <c r="E618" s="0" t="s">
-        <v>1691</v>
+        <v>1687</v>
       </c>
       <c r="F618" s="0" t="s">
         <v>357</v>
@@ -25754,13 +25755,13 @@
         <v>0</v>
       </c>
       <c r="H618" s="0" t="s">
-        <v>1692</v>
+        <v>1688</v>
       </c>
       <c r="I618" s="0" t="s">
         <v>359</v>
       </c>
       <c r="J618" s="0" t="s">
-        <v>1693</v>
+        <v>1689</v>
       </c>
       <c r="K618" s="0" t="s">
         <v>305</v>
@@ -25771,7 +25772,7 @@
         <v>303</v>
       </c>
       <c r="B619" s="0" t="s">
-        <v>1694</v>
+        <v>1690</v>
       </c>
       <c r="C619" s="0" t="s">
         <v>31</v>
@@ -25780,22 +25781,22 @@
         <v>312</v>
       </c>
       <c r="E619" s="0" t="s">
-        <v>1695</v>
+        <v>1691</v>
       </c>
       <c r="F619" s="0" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="G619" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H619" s="0" t="s">
-        <v>1696</v>
+        <v>1692</v>
       </c>
       <c r="I619" s="0" t="s">
         <v>359</v>
       </c>
       <c r="J619" s="0" t="s">
-        <v>1689</v>
+        <v>1693</v>
       </c>
       <c r="K619" s="0" t="s">
         <v>305</v>
@@ -25806,7 +25807,7 @@
         <v>303</v>
       </c>
       <c r="B620" s="0" t="s">
-        <v>1697</v>
+        <v>1694</v>
       </c>
       <c r="C620" s="0" t="s">
         <v>31</v>
@@ -25815,7 +25816,7 @@
         <v>312</v>
       </c>
       <c r="E620" s="0" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F620" s="0" t="s">
         <v>370</v>
@@ -25824,13 +25825,13 @@
         <v>0</v>
       </c>
       <c r="H620" s="0" t="s">
-        <v>1699</v>
+        <v>1696</v>
       </c>
       <c r="I620" s="0" t="s">
         <v>359</v>
       </c>
       <c r="J620" s="0" t="s">
-        <v>1700</v>
+        <v>1689</v>
       </c>
       <c r="K620" s="0" t="s">
         <v>305</v>
@@ -25841,7 +25842,7 @@
         <v>303</v>
       </c>
       <c r="B621" s="0" t="s">
-        <v>368</v>
+        <v>1697</v>
       </c>
       <c r="C621" s="0" t="s">
         <v>31</v>
@@ -25850,22 +25851,22 @@
         <v>312</v>
       </c>
       <c r="E621" s="0" t="s">
-        <v>369</v>
+        <v>1698</v>
       </c>
       <c r="F621" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="G621" s="0" t="s">
-        <v>1701</v>
+      <c r="G621" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H621" s="0" t="s">
-        <v>371</v>
+        <v>1699</v>
       </c>
       <c r="I621" s="0" t="s">
         <v>359</v>
       </c>
       <c r="J621" s="0" t="s">
-        <v>369</v>
+        <v>1700</v>
       </c>
       <c r="K621" s="0" t="s">
         <v>305</v>
@@ -25876,31 +25877,31 @@
         <v>303</v>
       </c>
       <c r="B622" s="0" t="s">
-        <v>1702</v>
+        <v>368</v>
       </c>
       <c r="C622" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D622" s="0" t="s">
-        <v>1703</v>
+        <v>312</v>
       </c>
       <c r="E622" s="0" t="s">
-        <v>1704</v>
+        <v>369</v>
       </c>
       <c r="F622" s="0" t="s">
-        <v>1705</v>
+        <v>370</v>
       </c>
       <c r="G622" s="0" t="s">
         <v>1701</v>
       </c>
       <c r="H622" s="0" t="s">
-        <v>1706</v>
+        <v>371</v>
       </c>
       <c r="I622" s="0" t="s">
-        <v>226</v>
+        <v>359</v>
       </c>
       <c r="J622" s="0" t="s">
-        <v>1707</v>
+        <v>369</v>
       </c>
       <c r="K622" s="0" t="s">
         <v>305</v>
@@ -25911,7 +25912,7 @@
         <v>303</v>
       </c>
       <c r="B623" s="0" t="s">
-        <v>1708</v>
+        <v>1702</v>
       </c>
       <c r="C623" s="0" t="s">
         <v>31</v>
@@ -25920,10 +25921,10 @@
         <v>1703</v>
       </c>
       <c r="E623" s="0" t="s">
-        <v>1709</v>
+        <v>1704</v>
       </c>
       <c r="F623" s="0" t="s">
-        <v>1710</v>
+        <v>1705</v>
       </c>
       <c r="G623" s="0" t="s">
         <v>1701</v>
@@ -25935,46 +25936,45 @@
         <v>226</v>
       </c>
       <c r="J623" s="0" t="s">
-        <v>1711</v>
+        <v>1707</v>
       </c>
       <c r="K623" s="0" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A626" s="0" t="s">
-        <v>1019</v>
-      </c>
-      <c r="B626" s="0" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C626" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D626" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E626" s="0" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F626" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="G626" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/89c4bb4f45a0182fc00a1b86b13241a5.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H626" s="0" t="s">
-        <v>1714</v>
-      </c>
-      <c r="I626" s="0" t="s">
-        <v>1715</v>
-      </c>
-      <c r="J626" s="0" t="s">
-        <v>1716</v>
-      </c>
-      <c r="K626" s="0" t="s">
-        <v>981</v>
+    <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A624" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B624" s="0" t="s">
+        <v>1708</v>
+      </c>
+      <c r="C624" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D624" s="0" t="s">
+        <v>1703</v>
+      </c>
+      <c r="E624" s="0" t="s">
+        <v>1709</v>
+      </c>
+      <c r="F624" s="0" t="s">
+        <v>1710</v>
+      </c>
+      <c r="G624" s="0" t="s">
+        <v>1701</v>
+      </c>
+      <c r="H624" s="0" t="s">
+        <v>1706</v>
+      </c>
+      <c r="I624" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="J624" s="0" t="s">
+        <v>1711</v>
+      </c>
+      <c r="K624" s="0" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25982,7 +25982,7 @@
         <v>1019</v>
       </c>
       <c r="B627" s="0" t="s">
-        <v>1717</v>
+        <v>1712</v>
       </c>
       <c r="C627" s="0" t="s">
         <v>31</v>
@@ -25991,13 +25991,13 @@
         <v>135</v>
       </c>
       <c r="E627" s="0" t="s">
-        <v>1718</v>
+        <v>1713</v>
       </c>
       <c r="F627" s="0" t="s">
         <v>137</v>
       </c>
       <c r="G627" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2d38bda3114d03f7543b8af88aadd03a.html","web")</f>
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/89c4bb4f45a0182fc00a1b86b13241a5.html","web")</f>
         <v>web</v>
       </c>
       <c r="H627" s="0" t="s">
@@ -26007,7 +26007,7 @@
         <v>1715</v>
       </c>
       <c r="J627" s="0" t="s">
-        <v>1719</v>
+        <v>1716</v>
       </c>
       <c r="K627" s="0" t="s">
         <v>981</v>
@@ -26018,7 +26018,7 @@
         <v>1019</v>
       </c>
       <c r="B628" s="0" t="s">
-        <v>1720</v>
+        <v>1717</v>
       </c>
       <c r="C628" s="0" t="s">
         <v>31</v>
@@ -26027,62 +26027,62 @@
         <v>135</v>
       </c>
       <c r="E628" s="0" t="s">
-        <v>1721</v>
+        <v>1718</v>
       </c>
       <c r="F628" s="0" t="s">
         <v>137</v>
       </c>
       <c r="G628" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2d38bda3114d03f7543b8af88aadd03a.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H628" s="0" t="s">
+        <v>1714</v>
+      </c>
+      <c r="I628" s="0" t="s">
+        <v>1715</v>
+      </c>
+      <c r="J628" s="0" t="s">
+        <v>1719</v>
+      </c>
+      <c r="K628" s="0" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A629" s="0" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B629" s="0" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C629" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D629" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E629" s="0" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F629" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G629" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/93723bb54a2c43450d75403102e618ac.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H628" s="0" t="s">
+      <c r="H629" s="0" t="s">
         <v>1714</v>
       </c>
-      <c r="I628" s="0" t="s">
+      <c r="I629" s="0" t="s">
         <v>1715</v>
       </c>
-      <c r="J628" s="0" t="s">
+      <c r="J629" s="0" t="s">
         <v>1722</v>
       </c>
-      <c r="K628" s="0" t="s">
+      <c r="K629" s="0" t="s">
         <v>981</v>
-      </c>
-    </row>
-    <row r="630" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A630" s="3" t="s">
-        <v>949</v>
-      </c>
-      <c r="B630" s="3" t="s">
-        <v>1723</v>
-      </c>
-      <c r="C630" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D630" s="3" t="s">
-        <v>956</v>
-      </c>
-      <c r="E630" s="3" t="s">
-        <v>1724</v>
-      </c>
-      <c r="F630" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G630" s="3" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5aea9677ebbb40076a0e0b3b11fdb46f.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H630" s="3" t="s">
-        <v>1725</v>
-      </c>
-      <c r="I630" s="3" t="s">
-        <v>1726</v>
-      </c>
-      <c r="J630" s="3" t="s">
-        <v>1727</v>
-      </c>
-      <c r="K630" s="3" t="s">
-        <v>1728</v>
       </c>
     </row>
     <row r="631" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26090,183 +26090,184 @@
         <v>949</v>
       </c>
       <c r="B631" s="3" t="s">
-        <v>1729</v>
+        <v>1723</v>
       </c>
       <c r="C631" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D631" s="3" t="s">
         <v>956</v>
       </c>
       <c r="E631" s="3" t="s">
+        <v>1724</v>
+      </c>
+      <c r="F631" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G631" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5aea9677ebbb40076a0e0b3b11fdb46f.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H631" s="3" t="s">
+        <v>1725</v>
+      </c>
+      <c r="I631" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="J631" s="3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="K631" s="3" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="632" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A632" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="B632" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C632" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D632" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="E632" s="3" t="s">
         <v>1730</v>
       </c>
-      <c r="F631" s="3" t="s">
+      <c r="F632" s="3" t="s">
         <v>967</v>
       </c>
-      <c r="G631" s="3" t="str">
+      <c r="G632" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/9122e7b627c429163fd0857dc366e14e.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H631" s="3" t="s">
+      <c r="H632" s="3" t="s">
         <v>1731</v>
       </c>
-      <c r="I631" s="3" t="s">
+      <c r="I632" s="3" t="s">
         <v>1726</v>
       </c>
-      <c r="J631" s="3" t="s">
+      <c r="J632" s="3" t="s">
         <v>1732</v>
       </c>
-      <c r="K631" s="3" t="s">
+      <c r="K632" s="3" t="s">
         <v>1733</v>
       </c>
     </row>
-    <row r="632" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="633" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A633" s="0" t="s">
+    <row r="633" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="634" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A634" s="0" t="s">
         <v>964</v>
       </c>
-      <c r="B633" s="3" t="s">
+      <c r="B634" s="3" t="s">
         <v>1734</v>
       </c>
-      <c r="C633" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D633" s="3" t="s">
+      <c r="C634" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D634" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E633" s="3" t="s">
+      <c r="E634" s="3" t="s">
         <v>1735</v>
       </c>
-      <c r="F633" s="3" t="s">
+      <c r="F634" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G633" s="3" t="str">
+      <c r="G634" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/26a31ad76858198bd4d719aafeebe801.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H633" s="3" t="s">
+      <c r="H634" s="3" t="s">
         <v>1117</v>
       </c>
-      <c r="I633" s="3" t="s">
+      <c r="I634" s="3" t="s">
         <v>1736</v>
       </c>
-      <c r="J633" s="3" t="s">
+      <c r="J634" s="3" t="s">
         <v>1737</v>
       </c>
-      <c r="K633" s="3" t="s">
+      <c r="K634" s="3" t="s">
         <v>1738</v>
       </c>
     </row>
-    <row r="634" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A634" s="0"/>
-    </row>
     <row r="635" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A635" s="3" t="s">
+      <c r="A635" s="0"/>
+    </row>
+    <row r="636" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A636" s="3" t="s">
         <v>845</v>
       </c>
-      <c r="B635" s="3" t="s">
+      <c r="B636" s="3" t="s">
         <v>1739</v>
       </c>
-      <c r="C635" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D635" s="3" t="s">
+      <c r="C636" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D636" s="3" t="s">
         <v>868</v>
       </c>
-      <c r="E635" s="3" t="s">
+      <c r="E636" s="3" t="s">
         <v>1740</v>
       </c>
-      <c r="F635" s="3" t="s">
+      <c r="F636" s="3" t="s">
         <v>714</v>
       </c>
-      <c r="G635" s="3" t="str">
+      <c r="G636" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1d4594c97188efd47935238a429e02e4.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H635" s="3" t="s">
+      <c r="H636" s="3" t="s">
         <v>1741</v>
       </c>
-      <c r="I635" s="3" t="s">
+      <c r="I636" s="3" t="s">
         <v>1742</v>
       </c>
-      <c r="J635" s="3" t="s">
+      <c r="J636" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="K635" s="3" t="s">
+      <c r="K636" s="3" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="636" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="637" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A637" s="3" t="s">
+    <row r="637" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="638" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A638" s="3" t="s">
         <v>720</v>
       </c>
-      <c r="B637" s="3" t="s">
+      <c r="B638" s="3" t="s">
         <v>1743</v>
       </c>
-      <c r="C637" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D637" s="3" t="s">
+      <c r="C638" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D638" s="3" t="s">
         <v>730</v>
       </c>
-      <c r="E637" s="3" t="s">
+      <c r="E638" s="3" t="s">
         <v>1740</v>
       </c>
-      <c r="F637" s="3" t="s">
+      <c r="F638" s="3" t="s">
         <v>714</v>
       </c>
-      <c r="G637" s="3" t="str">
+      <c r="G638" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/1d4594c97188efd47935238a429e02e4.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H637" s="3" t="s">
+      <c r="H638" s="3" t="s">
         <v>1744</v>
       </c>
-      <c r="I637" s="3" t="s">
+      <c r="I638" s="3" t="s">
         <v>1742</v>
       </c>
-      <c r="J637" s="3" t="s">
+      <c r="J638" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="K637" s="3" t="s">
+      <c r="K638" s="3" t="s">
         <v>721</v>
-      </c>
-    </row>
-    <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A638" s="0" t="s">
-        <v>720</v>
-      </c>
-      <c r="B638" s="0" t="s">
-        <v>1745</v>
-      </c>
-      <c r="C638" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D638" s="0" t="s">
-        <v>730</v>
-      </c>
-      <c r="E638" s="0" t="s">
-        <v>1746</v>
-      </c>
-      <c r="F638" s="0" t="s">
-        <v>714</v>
-      </c>
-      <c r="G638" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H638" s="0" t="s">
-        <v>1747</v>
-      </c>
-      <c r="I638" s="0" t="s">
-        <v>1493</v>
-      </c>
-      <c r="J638" s="0" t="s">
-        <v>727</v>
-      </c>
-      <c r="K638" s="0" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26274,19 +26275,19 @@
         <v>720</v>
       </c>
       <c r="B639" s="0" t="s">
-        <v>1748</v>
+        <v>1745</v>
       </c>
       <c r="C639" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D639" s="0" t="s">
-        <v>739</v>
+        <v>730</v>
       </c>
       <c r="E639" s="0" t="s">
-        <v>1749</v>
+        <v>1746</v>
       </c>
       <c r="F639" s="0" t="s">
-        <v>752</v>
+        <v>714</v>
       </c>
       <c r="G639" s="0" t="n">
         <v>0</v>
@@ -26298,60 +26299,59 @@
         <v>1493</v>
       </c>
       <c r="J639" s="0" t="s">
-        <v>1749</v>
+        <v>727</v>
       </c>
       <c r="K639" s="0" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A642" s="0" t="s">
-        <v>436</v>
-      </c>
-      <c r="B642" s="0" t="s">
-        <v>368</v>
-      </c>
-      <c r="C642" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D642" s="0" t="s">
-        <v>438</v>
-      </c>
-      <c r="E642" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="F642" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="G642" s="0" t="str">
-        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
-        <v>web</v>
-      </c>
-      <c r="H642" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="I642" s="0" t="s">
-        <v>359</v>
-      </c>
-      <c r="J642" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="K642" s="0" t="s">
-        <v>441</v>
+    <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A640" s="0" t="s">
+        <v>720</v>
+      </c>
+      <c r="B640" s="0" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C640" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D640" s="0" t="s">
+        <v>739</v>
+      </c>
+      <c r="E640" s="0" t="s">
+        <v>1749</v>
+      </c>
+      <c r="F640" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="G640" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H640" s="0" t="s">
+        <v>1747</v>
+      </c>
+      <c r="I640" s="0" t="s">
+        <v>1493</v>
+      </c>
+      <c r="J640" s="0" t="s">
+        <v>1749</v>
+      </c>
+      <c r="K640" s="0" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="0" t="s">
-        <v>915</v>
+        <v>436</v>
       </c>
       <c r="B643" s="0" t="s">
         <v>368</v>
       </c>
       <c r="C643" s="0" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D643" s="0" t="s">
-        <v>868</v>
+        <v>438</v>
       </c>
       <c r="E643" s="0" t="s">
         <v>369</v>
@@ -26373,7 +26373,7 @@
         <v>369</v>
       </c>
       <c r="K643" s="0" t="s">
-        <v>711</v>
+        <v>441</v>
       </c>
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26381,7 +26381,7 @@
         <v>915</v>
       </c>
       <c r="B644" s="0" t="s">
-        <v>1683</v>
+        <v>368</v>
       </c>
       <c r="C644" s="0" t="s">
         <v>49</v>
@@ -26390,173 +26390,208 @@
         <v>868</v>
       </c>
       <c r="E644" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="F644" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="G644" s="0" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c8b1814845661bcad37910e70a59b285.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H644" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="I644" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="J644" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="K644" s="0" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A645" s="0" t="s">
+        <v>915</v>
+      </c>
+      <c r="B645" s="0" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C645" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D645" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="E645" s="0" t="s">
         <v>1684</v>
       </c>
-      <c r="F644" s="0" t="s">
+      <c r="F645" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="G644" s="0" t="str">
+      <c r="G645" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/2a6093caf9e5cd42fb2fba6bdb73d6db.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H644" s="0" t="s">
+      <c r="H645" s="0" t="s">
         <v>1685</v>
       </c>
-      <c r="I644" s="0" t="s">
+      <c r="I645" s="0" t="s">
         <v>359</v>
       </c>
-      <c r="J644" s="0" t="s">
+      <c r="J645" s="0" t="s">
         <v>1684</v>
       </c>
-      <c r="K644" s="0" t="s">
+      <c r="K645" s="0" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="646" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A646" s="3" t="s">
+    <row r="647" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A647" s="3" t="s">
         <v>1028</v>
       </c>
-      <c r="B646" s="3" t="s">
+      <c r="B647" s="3" t="s">
         <v>1115</v>
       </c>
-      <c r="C646" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D646" s="3" t="s">
+      <c r="C647" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D647" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E646" s="3" t="s">
+      <c r="E647" s="3" t="s">
         <v>1116</v>
       </c>
-      <c r="F646" s="3" t="s">
+      <c r="F647" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G646" s="3" t="str">
+      <c r="G647" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917a796-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H646" s="0" t="s">
+      <c r="H647" s="0" t="s">
         <v>1117</v>
       </c>
-      <c r="I646" s="0" t="s">
+      <c r="I647" s="0" t="s">
         <v>1118</v>
       </c>
-      <c r="J646" s="3" t="s">
+      <c r="J647" s="3" t="s">
         <v>1119</v>
       </c>
-      <c r="K646" s="3" t="s">
+      <c r="K647" s="3" t="s">
         <v>1063</v>
       </c>
     </row>
-    <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A648" s="0" t="s">
+    <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A649" s="0" t="s">
         <v>1019</v>
       </c>
-      <c r="B648" s="0" t="s">
+      <c r="B649" s="0" t="s">
         <v>1024</v>
       </c>
-      <c r="C648" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D648" s="0" t="s">
+      <c r="C649" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D649" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="E648" s="0" t="s">
+      <c r="E649" s="0" t="s">
         <v>1025</v>
       </c>
-      <c r="F648" s="0" t="s">
+      <c r="F649" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="G648" s="0" t="str">
+      <c r="G649" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917e2ba-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H648" s="0" t="s">
+      <c r="H649" s="0" t="s">
         <v>1026</v>
       </c>
-      <c r="I648" s="0" t="s">
+      <c r="I649" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="J648" s="0" t="s">
+      <c r="J649" s="0" t="s">
         <v>759</v>
       </c>
-      <c r="K648" s="0" t="s">
+      <c r="K649" s="0" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="649" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A649" s="3" t="s">
+    <row r="650" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A650" s="3" t="s">
         <v>964</v>
       </c>
-      <c r="B649" s="3" t="s">
+      <c r="B650" s="3" t="s">
         <v>1024</v>
       </c>
-      <c r="C649" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D649" s="3" t="s">
+      <c r="C650" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D650" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E649" s="3" t="s">
+      <c r="E650" s="3" t="s">
         <v>1750</v>
       </c>
-      <c r="F649" s="3" t="s">
+      <c r="F650" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G649" s="3" t="str">
+      <c r="G650" s="3" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5917e2ba-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H649" s="0" t="s">
+      <c r="H650" s="0" t="s">
         <v>1026</v>
       </c>
-      <c r="I649" s="3" t="s">
+      <c r="I650" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J649" s="3" t="s">
+      <c r="J650" s="3" t="s">
         <v>759</v>
       </c>
-      <c r="K649" s="3" t="s">
+      <c r="K650" s="3" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A652" s="0" t="s">
+    <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A653" s="0" t="s">
         <v>494</v>
       </c>
-      <c r="B652" s="0" t="s">
+      <c r="B653" s="0" t="s">
         <v>1751</v>
       </c>
-      <c r="C652" s="0" t="s">
+      <c r="C653" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D652" s="0" t="s">
+      <c r="D653" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="E652" s="0" t="s">
+      <c r="E653" s="0" t="s">
         <v>1752</v>
       </c>
-      <c r="F652" s="0" t="s">
+      <c r="F653" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="G652" s="0" t="str">
+      <c r="G653" s="0" t="str">
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/5912cab4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H652" s="0" t="s">
+      <c r="H653" s="0" t="s">
         <v>1753</v>
       </c>
-      <c r="I652" s="0" t="s">
+      <c r="I653" s="0" t="s">
         <v>1754</v>
       </c>
-      <c r="J652" s="0" t="s">
+      <c r="J653" s="0" t="s">
         <v>759</v>
       </c>
-      <c r="K652" s="0" t="s">
+      <c r="K653" s="0" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add Eday ec to the ignored files #557. Adjust ignore comment of E3hrPt rsutcsaf #556.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
+++ b/ece2cmor3/resources/list-of-ignored-cmpi6-requested-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6434" uniqueCount="1865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6444" uniqueCount="1870">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -5611,10 +5611,25 @@
     <t xml:space="preserve">TOA Outgoing Clear-Sky, Aerosol-Free Shortwave Radiation</t>
   </si>
   <si>
-    <t xml:space="preserve">Ignore because part of RFMIP-IRF and we don't participate in that experiment of RFMIP. Moreover grib 128.212-126.068 won't work here, because then accumulated and instantaneous fluxes are mixed.</t>
+    <t xml:space="preserve">ifs code name = 68.126</t>
   </si>
   <si>
     <t xml:space="preserve">Flux corresponding to rsutcs resulting from aerosol-free call to radiation, following Ghan (ACP, 2013)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interception Evaporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available in IFS   #557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franco, Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Water' means water in all phases. 'Canopy' means the plant or vegetation canopy. Evaporation is the conversion of liquid or solid into vapor. (The conversion of solid alone into vapor is called 'sublimation'.) In accordance with common usage in geophysical disciplines, 'flux' implies per unit area, called 'flux density' in physics. Unless indicated in the cell_methods attribute, a quantity is assumed to apply to the whole area of each horizontal grid box. Previously, the qualifier where_type was used to specify that the quantity applies only to the part of the grid box of the named type.  Names containing the where_type qualifier are deprecated and newly created data should use the cell_methods attribute to indicate the horizontal area to which the quantity applies.</t>
   </si>
 </sst>
 </file>
@@ -5624,7 +5639,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5654,6 +5669,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5698,12 +5719,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5727,7 +5756,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A684" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A706" activeCellId="0" sqref="706:706"/>
+      <selection pane="topLeft" activeCell="H706" activeCellId="0" sqref="H706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28495,7 +28524,7 @@
       </c>
     </row>
     <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="706" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A706" s="0" t="s">
         <v>860</v>
       </c>
@@ -28518,7 +28547,7 @@
         <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/c9a70b4e-c5f0-11e6-ac20-5404a60d96b5.html","web")</f>
         <v>web</v>
       </c>
-      <c r="H706" s="0" t="s">
+      <c r="H706" s="2" t="s">
         <v>1863</v>
       </c>
       <c r="I706" s="0" t="s">
@@ -28531,6 +28560,43 @@
         <v>866</v>
       </c>
     </row>
+    <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A708" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="B708" s="3" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C708" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D708" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E708" s="3" t="s">
+        <v>1866</v>
+      </c>
+      <c r="F708" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G708" s="3" t="str">
+        <f aca="false">HYPERLINK("http://clipc-services.ceda.ac.uk/dreq/u/590f0bf4-9e49-11e5-803c-0d0b866b59f3.html","web")</f>
+        <v>web</v>
+      </c>
+      <c r="H708" s="3" t="s">
+        <v>1867</v>
+      </c>
+      <c r="I708" s="3" t="s">
+        <v>1868</v>
+      </c>
+      <c r="J708" s="3" t="s">
+        <v>1869</v>
+      </c>
+      <c r="K708" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>